<commit_message>
Wrapping up sample problems for set-maps
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bharat/bctci/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C455B8-8F60-A64E-B1E7-CFDA61D0DD47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D70FD35D-72C2-7A4F-850F-07A3A3C9BC26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25600" yWindow="2180" windowWidth="26880" windowHeight="15120" xr2:uid="{233FF15D-0BCB-6B46-B450-599851EED7C1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="152">
   <si>
     <t>Sets &amp; Maps</t>
   </si>
@@ -473,6 +473,27 @@
   </si>
   <si>
     <t>Yes, canonical order for sets and comparison problems</t>
+  </si>
+  <si>
+    <t>Two sets, with normalised strings for ip-domain and subdomain-domain association</t>
+  </si>
+  <si>
+    <t>8 minutes</t>
+  </si>
+  <si>
+    <t>My hesitation with dictionaries was that I'd have to iterate over them to confirm membership. However, a set as a value of a dict can confirm membership in constant time</t>
+  </si>
+  <si>
+    <t>Yes, constant time solution</t>
+  </si>
+  <si>
+    <t>To use a set as a value for a dict</t>
+  </si>
+  <si>
+    <t>Internalise this pattern</t>
+  </si>
+  <si>
+    <t>Yes, sets as values for a dict</t>
   </si>
 </sst>
 </file>
@@ -1074,8 +1095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4095FB6B-33CD-C94D-A3B2-EAADF58B3AE5}">
   <dimension ref="A2:Q114"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="25" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="K6" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1387,28 +1408,58 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="116" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="22">
         <v>30.05</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="11"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="11"/>
+      <c r="C9" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="D9" s="21">
+        <v>45864</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="L9" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="M9" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="N9" s="9">
+        <v>4</v>
+      </c>
+      <c r="O9" s="10">
+        <v>4</v>
+      </c>
+      <c r="P9" s="10">
+        <v>3</v>
+      </c>
+      <c r="Q9" s="11">
+        <v>4</v>
+      </c>
     </row>
     <row r="10" spans="1:17" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22">

</xml_diff>

<commit_message>
2 problems from set-map problem set
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bharat/bctci/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D70FD35D-72C2-7A4F-850F-07A3A3C9BC26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EABE168-7886-5248-AAE6-1683B8B1D5BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25600" yWindow="2180" windowWidth="26880" windowHeight="15120" xr2:uid="{233FF15D-0BCB-6B46-B450-599851EED7C1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="162">
   <si>
     <t>Sets &amp; Maps</t>
   </si>
@@ -494,6 +494,36 @@
   </si>
   <si>
     <t>Yes, sets as values for a dict</t>
+  </si>
+  <si>
+    <t>Two iterations, one to map num to index, and second to check dict for presence of square and returning those that fit</t>
+  </si>
+  <si>
+    <t>Yes, linear time and space</t>
+  </si>
+  <si>
+    <t>Large potential integers, but Python handles large integers well</t>
+  </si>
+  <si>
+    <t>Remember to talk about Python's internals during interview</t>
+  </si>
+  <si>
+    <t>Approach</t>
+  </si>
+  <si>
+    <t>Store counter for each alphabet in original and expanded word. Check for one instance of extra count, if char missing or more than one word, reject</t>
+  </si>
+  <si>
+    <t>Iterating over the same counter</t>
+  </si>
+  <si>
+    <t>Order didn't matter, so dict counter made sense</t>
+  </si>
+  <si>
+    <t>No, but potentially smelly implementation</t>
+  </si>
+  <si>
+    <t>Spend time writing out the algorithm so that interviewer can call out code smells</t>
   </si>
 </sst>
 </file>
@@ -543,7 +573,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -629,9 +659,42 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -644,12 +707,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -659,9 +720,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -671,17 +730,6 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -714,25 +762,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -756,7 +798,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1093,15 +1141,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4095FB6B-33CD-C94D-A3B2-EAADF58B3AE5}">
-  <dimension ref="A2:Q114"/>
+  <dimension ref="A1:Q112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K6" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.83203125" style="22" customWidth="1"/>
+    <col min="1" max="1" width="14.83203125" style="20" customWidth="1"/>
     <col min="2" max="3" width="39.33203125" style="3" customWidth="1"/>
     <col min="4" max="4" width="13.83203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="15.1640625" style="1" customWidth="1"/>
@@ -1120,215 +1169,321 @@
     <col min="18" max="16384" width="14.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:17" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
+    <row r="1" spans="1:17" s="16" customFormat="1" ht="68" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18"/>
+      <c r="C1" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q1" s="11" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C2" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D2" s="26" t="s">
         <v>112</v>
       </c>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25" t="s">
+      <c r="E2" s="24"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25" t="s">
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="O3" s="25"/>
-      <c r="P3" s="25"/>
-      <c r="Q3" s="26"/>
-    </row>
-    <row r="4" spans="1:17" s="18" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="9" t="s">
-        <v>97</v>
+      <c r="O2" s="24"/>
+      <c r="P2" s="24"/>
+      <c r="Q2" s="27"/>
+    </row>
+    <row r="3" spans="1:17" s="10" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="18">
+        <v>30.01</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="D3" s="19">
+        <v>45862</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="M3" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="N3" s="9">
+        <v>4</v>
+      </c>
+      <c r="O3" s="10">
+        <v>3</v>
+      </c>
+      <c r="P3" s="10">
+        <v>3</v>
+      </c>
+      <c r="Q3" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="20">
+        <v>30.02</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="D4" s="19">
+        <v>45862</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>98</v>
+        <v>125</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>99</v>
+        <v>126</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>113</v>
+        <v>127</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>101</v>
+        <v>134</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>102</v>
+        <v>128</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>103</v>
+        <v>122</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>104</v>
+        <v>129</v>
       </c>
       <c r="M4" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="N4" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="O4" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="P4" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q4" s="11" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" s="10" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+      <c r="N4" s="9">
+        <v>4</v>
+      </c>
+      <c r="O4" s="10">
+        <v>4</v>
+      </c>
+      <c r="P4" s="10">
+        <v>3</v>
+      </c>
+      <c r="Q4" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20">
-        <v>30.01</v>
+        <v>30.03</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="D5" s="21">
-        <v>45862</v>
+        <v>3</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="D5" s="19">
+        <v>45863</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>115</v>
+        <v>131</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>116</v>
+        <v>132</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>117</v>
+        <v>133</v>
       </c>
       <c r="H5" s="10" t="s">
         <v>118</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>119</v>
+        <v>136</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="K5" s="10" t="s">
         <v>122</v>
       </c>
       <c r="L5" s="10" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="M5" s="11" t="s">
         <v>122</v>
       </c>
       <c r="N5" s="9">
+        <v>5</v>
+      </c>
+      <c r="O5" s="10">
+        <v>5</v>
+      </c>
+      <c r="P5" s="10">
         <v>4</v>
       </c>
-      <c r="O5" s="10">
-        <v>3</v>
-      </c>
-      <c r="P5" s="10">
-        <v>3</v>
-      </c>
       <c r="Q5" s="11">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22">
-        <v>30.02</v>
+      <c r="A6" s="20">
+        <v>30.04</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="D6" s="21">
-        <v>45862</v>
+        <v>4</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="D6" s="19">
+        <v>45864</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>125</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>126</v>
+        <v>139</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>128</v>
+        <v>142</v>
       </c>
       <c r="K6" s="10" t="s">
         <v>122</v>
       </c>
       <c r="L6" s="10" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="M6" s="11" t="s">
-        <v>122</v>
+        <v>144</v>
       </c>
       <c r="N6" s="9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O6" s="10">
         <v>4</v>
       </c>
       <c r="P6" s="10">
+        <v>4</v>
+      </c>
+      <c r="Q6" s="11">
         <v>3</v>
       </c>
-      <c r="Q6" s="11">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22">
-        <v>30.03</v>
+    </row>
+    <row r="7" spans="1:17" ht="116" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="20">
+        <v>30.05</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="D7" s="21">
-        <v>45863</v>
+        <v>5</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="D7" s="19">
+        <v>45864</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>131</v>
+        <v>146</v>
       </c>
       <c r="F7" s="11" t="s">
         <v>132</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>133</v>
+        <v>147</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>118</v>
+        <v>148</v>
       </c>
       <c r="I7" s="10" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
       <c r="J7" s="10" t="s">
         <v>122</v>
@@ -1337,66 +1492,66 @@
         <v>122</v>
       </c>
       <c r="L7" s="10" t="s">
-        <v>135</v>
+        <v>150</v>
       </c>
       <c r="M7" s="11" t="s">
-        <v>122</v>
+        <v>151</v>
       </c>
       <c r="N7" s="9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O7" s="10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P7" s="10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q7" s="11">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22">
-        <v>30.04</v>
+      <c r="A8" s="20">
+        <v>30.06</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="19" t="s">
-        <v>137</v>
-      </c>
-      <c r="D8" s="21">
+        <v>6</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="D8" s="19">
         <v>45864</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>140</v>
+        <v>153</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>141</v>
+        <v>154</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>142</v>
+        <v>122</v>
       </c>
       <c r="K8" s="10" t="s">
         <v>122</v>
       </c>
       <c r="L8" s="10" t="s">
-        <v>143</v>
+        <v>155</v>
       </c>
       <c r="M8" s="11" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="N8" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O8" s="10">
         <v>4</v>
@@ -1405,71 +1560,71 @@
         <v>4</v>
       </c>
       <c r="Q8" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" ht="116" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22">
-        <v>30.05</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="100" x14ac:dyDescent="0.25">
+      <c r="A9" s="20">
+        <v>30.07</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>145</v>
-      </c>
-      <c r="D9" s="21">
+        <v>7</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="D9" s="19">
         <v>45864</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="F9" s="11" t="s">
         <v>132</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>148</v>
+        <v>118</v>
       </c>
       <c r="I9" s="10" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="J9" s="10" t="s">
         <v>122</v>
       </c>
       <c r="K9" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="L9" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="M9" s="11" t="s">
         <v>122</v>
-      </c>
-      <c r="L9" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="M9" s="11" t="s">
-        <v>151</v>
       </c>
       <c r="N9" s="9">
         <v>4</v>
       </c>
       <c r="O9" s="10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P9" s="10">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Q9" s="11">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22">
-        <v>30.06</v>
+      <c r="A10" s="20">
+        <v>30.08</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="21"/>
+        <v>8</v>
+      </c>
+      <c r="C10" s="17"/>
+      <c r="D10" s="19"/>
       <c r="E10" s="10"/>
       <c r="F10" s="11"/>
       <c r="G10" s="9"/>
@@ -1485,14 +1640,14 @@
       <c r="Q10" s="11"/>
     </row>
     <row r="11" spans="1:17" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22">
-        <v>30.07</v>
+      <c r="A11" s="20">
+        <v>30.09</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="21"/>
+        <v>9</v>
+      </c>
+      <c r="C11" s="17"/>
+      <c r="D11" s="19"/>
       <c r="E11" s="10"/>
       <c r="F11" s="11"/>
       <c r="G11" s="9"/>
@@ -1508,14 +1663,14 @@
       <c r="Q11" s="11"/>
     </row>
     <row r="12" spans="1:17" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="22">
-        <v>30.08</v>
+      <c r="A12" s="20">
+        <v>30.1</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="21"/>
+        <v>10</v>
+      </c>
+      <c r="C12" s="17"/>
+      <c r="D12" s="19"/>
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
       <c r="G12" s="9"/>
@@ -1531,14 +1686,14 @@
       <c r="Q12" s="11"/>
     </row>
     <row r="13" spans="1:17" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="22">
-        <v>30.09</v>
+      <c r="A13" s="20">
+        <v>30.11</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="21"/>
+        <v>11</v>
+      </c>
+      <c r="C13" s="17"/>
+      <c r="D13" s="19"/>
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
       <c r="G13" s="9"/>
@@ -1553,51 +1708,26 @@
       <c r="P13" s="10"/>
       <c r="Q13" s="11"/>
     </row>
-    <row r="14" spans="1:17" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="22">
-        <v>30.1</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="11"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="10"/>
-      <c r="Q14" s="11"/>
-    </row>
-    <row r="15" spans="1:17" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="22">
-        <v>30.11</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="19"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="11"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="10"/>
-      <c r="Q15" s="11"/>
+    <row r="14" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="13"/>
+      <c r="D14" s="4"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="4"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="4"/>
+      <c r="Q14" s="5"/>
+    </row>
+    <row r="15" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="14"/>
+      <c r="D15" s="4"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="4"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="4"/>
+      <c r="Q15" s="5"/>
     </row>
     <row r="16" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="13"/>
@@ -1609,10 +1739,13 @@
       <c r="Q16" s="5"/>
     </row>
     <row r="17" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="14"/>
+      <c r="A17" s="20">
+        <v>32.01</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="13"/>
       <c r="D17" s="4"/>
       <c r="F17" s="5"/>
       <c r="G17" s="4"/>
@@ -1621,6 +1754,12 @@
       <c r="Q17" s="5"/>
     </row>
     <row r="18" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="20">
+        <v>32.020000000000003</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="C18" s="13"/>
       <c r="D18" s="4"/>
       <c r="F18" s="5"/>
@@ -1630,11 +1769,11 @@
       <c r="Q18" s="5"/>
     </row>
     <row r="19" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="22">
-        <v>32.01</v>
+      <c r="A19" s="20">
+        <v>32.03</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C19" s="13"/>
       <c r="D19" s="4"/>
@@ -1645,11 +1784,11 @@
       <c r="Q19" s="5"/>
     </row>
     <row r="20" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="22">
-        <v>32.020000000000003</v>
+      <c r="A20" s="20">
+        <v>32.04</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C20" s="13"/>
       <c r="D20" s="4"/>
@@ -1660,11 +1799,11 @@
       <c r="Q20" s="5"/>
     </row>
     <row r="21" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="22">
-        <v>32.03</v>
+      <c r="A21" s="20">
+        <v>32.049999999999997</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C21" s="13"/>
       <c r="D21" s="4"/>
@@ -1675,11 +1814,11 @@
       <c r="Q21" s="5"/>
     </row>
     <row r="22" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="22">
-        <v>32.04</v>
+      <c r="A22" s="20">
+        <v>32.06</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C22" s="13"/>
       <c r="D22" s="4"/>
@@ -1690,11 +1829,11 @@
       <c r="Q22" s="5"/>
     </row>
     <row r="23" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="22">
-        <v>32.049999999999997</v>
+      <c r="A23" s="20">
+        <v>32.07</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C23" s="13"/>
       <c r="D23" s="4"/>
@@ -1705,11 +1844,11 @@
       <c r="Q23" s="5"/>
     </row>
     <row r="24" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="22">
-        <v>32.06</v>
+      <c r="A24" s="20">
+        <v>32.08</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C24" s="13"/>
       <c r="D24" s="4"/>
@@ -1720,12 +1859,6 @@
       <c r="Q24" s="5"/>
     </row>
     <row r="25" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="22">
-        <v>32.07</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="C25" s="13"/>
       <c r="D25" s="4"/>
       <c r="F25" s="5"/>
@@ -1735,13 +1868,10 @@
       <c r="Q25" s="5"/>
     </row>
     <row r="26" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="22">
-        <v>32.08</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" s="13"/>
+      <c r="B26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="14"/>
       <c r="D26" s="4"/>
       <c r="F26" s="5"/>
       <c r="G26" s="4"/>
@@ -1750,7 +1880,8 @@
       <c r="Q26" s="5"/>
     </row>
     <row r="27" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C27" s="13"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="14"/>
       <c r="D27" s="4"/>
       <c r="F27" s="5"/>
       <c r="G27" s="4"/>
@@ -1759,10 +1890,13 @@
       <c r="Q27" s="5"/>
     </row>
     <row r="28" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C28" s="14"/>
+      <c r="A28" s="20">
+        <v>33.01</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="13"/>
       <c r="D28" s="4"/>
       <c r="F28" s="5"/>
       <c r="G28" s="4"/>
@@ -1771,8 +1905,13 @@
       <c r="Q28" s="5"/>
     </row>
     <row r="29" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="2"/>
-      <c r="C29" s="14"/>
+      <c r="A29" s="20">
+        <v>33.020000000000003</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="13"/>
       <c r="D29" s="4"/>
       <c r="F29" s="5"/>
       <c r="G29" s="4"/>
@@ -1781,11 +1920,11 @@
       <c r="Q29" s="5"/>
     </row>
     <row r="30" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="22">
-        <v>33.01</v>
+      <c r="A30" s="21">
+        <v>1</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C30" s="13"/>
       <c r="D30" s="4"/>
@@ -1796,11 +1935,11 @@
       <c r="Q30" s="5"/>
     </row>
     <row r="31" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="22">
-        <v>33.020000000000003</v>
+      <c r="A31" s="21">
+        <v>2</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C31" s="13"/>
       <c r="D31" s="4"/>
@@ -1811,11 +1950,11 @@
       <c r="Q31" s="5"/>
     </row>
     <row r="32" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="23">
-        <v>1</v>
+      <c r="A32" s="21">
+        <v>3</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C32" s="13"/>
       <c r="D32" s="4"/>
@@ -1826,11 +1965,11 @@
       <c r="Q32" s="5"/>
     </row>
     <row r="33" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="23">
-        <v>2</v>
+      <c r="A33" s="20">
+        <v>33.03</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C33" s="13"/>
       <c r="D33" s="4"/>
@@ -1841,11 +1980,11 @@
       <c r="Q33" s="5"/>
     </row>
     <row r="34" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="23">
-        <v>3</v>
+      <c r="A34" s="21">
+        <v>4</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C34" s="13"/>
       <c r="D34" s="4"/>
@@ -1856,11 +1995,11 @@
       <c r="Q34" s="5"/>
     </row>
     <row r="35" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="22">
-        <v>33.03</v>
+      <c r="A35" s="21">
+        <v>5</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C35" s="13"/>
       <c r="D35" s="4"/>
@@ -1871,11 +2010,11 @@
       <c r="Q35" s="5"/>
     </row>
     <row r="36" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="23">
-        <v>4</v>
+      <c r="A36" s="20">
+        <v>33.04</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C36" s="13"/>
       <c r="D36" s="4"/>
@@ -1886,11 +2025,11 @@
       <c r="Q36" s="5"/>
     </row>
     <row r="37" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="23">
-        <v>5</v>
+      <c r="A37" s="20">
+        <v>33.049999999999997</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C37" s="13"/>
       <c r="D37" s="4"/>
@@ -1901,12 +2040,6 @@
       <c r="Q37" s="5"/>
     </row>
     <row r="38" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="22">
-        <v>33.04</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="C38" s="13"/>
       <c r="D38" s="4"/>
       <c r="F38" s="5"/>
@@ -1916,13 +2049,10 @@
       <c r="Q38" s="5"/>
     </row>
     <row r="39" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="22">
-        <v>33.049999999999997</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C39" s="13"/>
+      <c r="B39" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C39" s="14"/>
       <c r="D39" s="4"/>
       <c r="F39" s="5"/>
       <c r="G39" s="4"/>
@@ -1931,7 +2061,8 @@
       <c r="Q39" s="5"/>
     </row>
     <row r="40" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C40" s="13"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="14"/>
       <c r="D40" s="4"/>
       <c r="F40" s="5"/>
       <c r="G40" s="4"/>
@@ -1940,10 +2071,13 @@
       <c r="Q40" s="5"/>
     </row>
     <row r="41" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C41" s="14"/>
+      <c r="A41" s="22">
+        <v>35.000999999999998</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C41" s="13"/>
       <c r="D41" s="4"/>
       <c r="F41" s="5"/>
       <c r="G41" s="4"/>
@@ -1952,8 +2086,13 @@
       <c r="Q41" s="5"/>
     </row>
     <row r="42" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="2"/>
-      <c r="C42" s="14"/>
+      <c r="A42" s="22">
+        <v>35.002000000000002</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C42" s="13"/>
       <c r="D42" s="4"/>
       <c r="F42" s="5"/>
       <c r="G42" s="4"/>
@@ -1962,11 +2101,11 @@
       <c r="Q42" s="5"/>
     </row>
     <row r="43" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="24">
-        <v>35.000999999999998</v>
+      <c r="A43" s="20">
+        <v>35.01</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C43" s="13"/>
       <c r="D43" s="4"/>
@@ -1977,11 +2116,11 @@
       <c r="Q43" s="5"/>
     </row>
     <row r="44" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="24">
-        <v>35.002000000000002</v>
+      <c r="A44" s="20">
+        <v>35.020000000000003</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C44" s="13"/>
       <c r="D44" s="4"/>
@@ -1992,11 +2131,11 @@
       <c r="Q44" s="5"/>
     </row>
     <row r="45" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="22">
-        <v>35.01</v>
+      <c r="A45" s="20">
+        <v>35.03</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C45" s="13"/>
       <c r="D45" s="4"/>
@@ -2007,11 +2146,11 @@
       <c r="Q45" s="5"/>
     </row>
     <row r="46" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="22">
-        <v>35.020000000000003</v>
+      <c r="A46" s="20">
+        <v>35.04</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C46" s="13"/>
       <c r="D46" s="4"/>
@@ -2022,11 +2161,11 @@
       <c r="Q46" s="5"/>
     </row>
     <row r="47" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="22">
-        <v>35.03</v>
+      <c r="A47" s="20">
+        <v>35.049999999999997</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C47" s="13"/>
       <c r="D47" s="4"/>
@@ -2037,11 +2176,11 @@
       <c r="Q47" s="5"/>
     </row>
     <row r="48" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="22">
-        <v>35.04</v>
+      <c r="A48" s="20">
+        <v>35.06</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C48" s="13"/>
       <c r="D48" s="4"/>
@@ -2052,11 +2191,11 @@
       <c r="Q48" s="5"/>
     </row>
     <row r="49" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="22">
-        <v>35.049999999999997</v>
+      <c r="A49" s="20">
+        <v>35.07</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C49" s="13"/>
       <c r="D49" s="4"/>
@@ -2067,11 +2206,11 @@
       <c r="Q49" s="5"/>
     </row>
     <row r="50" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="22">
-        <v>35.06</v>
+      <c r="A50" s="20">
+        <v>35.08</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C50" s="13"/>
       <c r="D50" s="4"/>
@@ -2082,11 +2221,11 @@
       <c r="Q50" s="5"/>
     </row>
     <row r="51" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="22">
-        <v>35.07</v>
+      <c r="A51" s="20">
+        <v>35.090000000000003</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C51" s="13"/>
       <c r="D51" s="4"/>
@@ -2097,11 +2236,11 @@
       <c r="Q51" s="5"/>
     </row>
     <row r="52" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="22">
-        <v>35.08</v>
+      <c r="A52" s="20">
+        <v>35.1</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C52" s="13"/>
       <c r="D52" s="4"/>
@@ -2112,11 +2251,11 @@
       <c r="Q52" s="5"/>
     </row>
     <row r="53" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="22">
-        <v>35.090000000000003</v>
+      <c r="A53" s="20">
+        <v>35.11</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C53" s="13"/>
       <c r="D53" s="4"/>
@@ -2127,11 +2266,11 @@
       <c r="Q53" s="5"/>
     </row>
     <row r="54" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="22">
-        <v>35.1</v>
+      <c r="A54" s="20">
+        <v>35.120000000000097</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C54" s="13"/>
       <c r="D54" s="4"/>
@@ -2142,11 +2281,11 @@
       <c r="Q54" s="5"/>
     </row>
     <row r="55" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="22">
-        <v>35.11</v>
+      <c r="A55" s="20">
+        <v>35.130000000000102</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C55" s="13"/>
       <c r="D55" s="4"/>
@@ -2157,11 +2296,11 @@
       <c r="Q55" s="5"/>
     </row>
     <row r="56" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="22">
-        <v>35.120000000000097</v>
+      <c r="A56" s="20">
+        <v>35.1400000000001</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C56" s="13"/>
       <c r="D56" s="4"/>
@@ -2172,11 +2311,11 @@
       <c r="Q56" s="5"/>
     </row>
     <row r="57" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="22">
-        <v>35.130000000000102</v>
+      <c r="A57" s="20">
+        <v>35.150000000000098</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C57" s="13"/>
       <c r="D57" s="4"/>
@@ -2187,11 +2326,11 @@
       <c r="Q57" s="5"/>
     </row>
     <row r="58" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="22">
-        <v>35.1400000000001</v>
+      <c r="A58" s="20">
+        <v>35.160000000000103</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C58" s="13"/>
       <c r="D58" s="4"/>
@@ -2202,11 +2341,11 @@
       <c r="Q58" s="5"/>
     </row>
     <row r="59" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="22">
-        <v>35.150000000000098</v>
+      <c r="A59" s="20">
+        <v>35.170000000000101</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C59" s="13"/>
       <c r="D59" s="4"/>
@@ -2217,12 +2356,6 @@
       <c r="Q59" s="5"/>
     </row>
     <row r="60" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="22">
-        <v>35.160000000000103</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>50</v>
-      </c>
       <c r="C60" s="13"/>
       <c r="D60" s="4"/>
       <c r="F60" s="5"/>
@@ -2232,13 +2365,10 @@
       <c r="Q60" s="5"/>
     </row>
     <row r="61" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="22">
-        <v>35.170000000000101</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C61" s="13"/>
+      <c r="B61" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C61" s="14"/>
       <c r="D61" s="4"/>
       <c r="F61" s="5"/>
       <c r="G61" s="4"/>
@@ -2256,10 +2386,13 @@
       <c r="Q62" s="5"/>
     </row>
     <row r="63" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C63" s="14"/>
+      <c r="A63" s="21">
+        <v>1</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C63" s="13"/>
       <c r="D63" s="4"/>
       <c r="F63" s="5"/>
       <c r="G63" s="4"/>
@@ -2268,6 +2401,12 @@
       <c r="Q63" s="5"/>
     </row>
     <row r="64" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="21">
+        <v>2</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="C64" s="13"/>
       <c r="D64" s="4"/>
       <c r="F64" s="5"/>
@@ -2277,11 +2416,11 @@
       <c r="Q64" s="5"/>
     </row>
     <row r="65" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="23">
-        <v>1</v>
+      <c r="A65" s="21">
+        <v>3</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C65" s="13"/>
       <c r="D65" s="4"/>
@@ -2292,11 +2431,11 @@
       <c r="Q65" s="5"/>
     </row>
     <row r="66" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="23">
-        <v>2</v>
+      <c r="A66" s="21">
+        <v>4</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C66" s="13"/>
       <c r="D66" s="4"/>
@@ -2307,11 +2446,11 @@
       <c r="Q66" s="5"/>
     </row>
     <row r="67" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="23">
-        <v>3</v>
+      <c r="A67" s="21">
+        <v>5</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C67" s="13"/>
       <c r="D67" s="4"/>
@@ -2322,11 +2461,11 @@
       <c r="Q67" s="5"/>
     </row>
     <row r="68" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="23">
-        <v>4</v>
+      <c r="A68" s="21">
+        <v>6</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C68" s="13"/>
       <c r="D68" s="4"/>
@@ -2337,12 +2476,6 @@
       <c r="Q68" s="5"/>
     </row>
     <row r="69" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="23">
-        <v>5</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>59</v>
-      </c>
       <c r="C69" s="13"/>
       <c r="D69" s="4"/>
       <c r="F69" s="5"/>
@@ -2352,13 +2485,10 @@
       <c r="Q69" s="5"/>
     </row>
     <row r="70" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="23">
-        <v>6</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C70" s="13"/>
+      <c r="B70" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C70" s="14"/>
       <c r="D70" s="4"/>
       <c r="F70" s="5"/>
       <c r="G70" s="4"/>
@@ -2376,10 +2506,13 @@
       <c r="Q71" s="5"/>
     </row>
     <row r="72" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C72" s="14"/>
+      <c r="A72" s="20">
+        <v>39.01</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C72" s="13"/>
       <c r="D72" s="4"/>
       <c r="F72" s="5"/>
       <c r="G72" s="4"/>
@@ -2388,6 +2521,12 @@
       <c r="Q72" s="5"/>
     </row>
     <row r="73" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="20">
+        <v>39.020000000000003</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>69</v>
+      </c>
       <c r="C73" s="13"/>
       <c r="D73" s="4"/>
       <c r="F73" s="5"/>
@@ -2397,11 +2536,11 @@
       <c r="Q73" s="5"/>
     </row>
     <row r="74" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="22">
-        <v>39.01</v>
+      <c r="A74" s="20">
+        <v>39.03</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C74" s="13"/>
       <c r="D74" s="4"/>
@@ -2412,11 +2551,11 @@
       <c r="Q74" s="5"/>
     </row>
     <row r="75" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="22">
-        <v>39.020000000000003</v>
+      <c r="A75" s="20">
+        <v>39.04</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C75" s="13"/>
       <c r="D75" s="4"/>
@@ -2427,11 +2566,11 @@
       <c r="Q75" s="5"/>
     </row>
     <row r="76" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="22">
-        <v>39.03</v>
+      <c r="A76" s="20">
+        <v>39.049999999999997</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C76" s="13"/>
       <c r="D76" s="4"/>
@@ -2442,11 +2581,11 @@
       <c r="Q76" s="5"/>
     </row>
     <row r="77" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="22">
-        <v>39.04</v>
+      <c r="A77" s="20">
+        <v>39.06</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C77" s="13"/>
       <c r="D77" s="4"/>
@@ -2457,11 +2596,11 @@
       <c r="Q77" s="5"/>
     </row>
     <row r="78" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="22">
-        <v>39.049999999999997</v>
+      <c r="A78" s="20">
+        <v>39.07</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C78" s="13"/>
       <c r="D78" s="4"/>
@@ -2472,11 +2611,11 @@
       <c r="Q78" s="5"/>
     </row>
     <row r="79" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="22">
-        <v>39.06</v>
+      <c r="A79" s="20">
+        <v>39.08</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C79" s="13"/>
       <c r="D79" s="4"/>
@@ -2487,11 +2626,11 @@
       <c r="Q79" s="5"/>
     </row>
     <row r="80" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="22">
-        <v>39.07</v>
+      <c r="A80" s="20">
+        <v>39.090000000000003</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C80" s="13"/>
       <c r="D80" s="4"/>
@@ -2502,11 +2641,11 @@
       <c r="Q80" s="5"/>
     </row>
     <row r="81" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="22">
-        <v>39.08</v>
+      <c r="A81" s="20">
+        <v>39.1</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C81" s="13"/>
       <c r="D81" s="4"/>
@@ -2517,11 +2656,11 @@
       <c r="Q81" s="5"/>
     </row>
     <row r="82" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="22">
-        <v>39.090000000000003</v>
+      <c r="A82" s="20">
+        <v>39.11</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C82" s="13"/>
       <c r="D82" s="4"/>
@@ -2532,12 +2671,6 @@
       <c r="Q82" s="5"/>
     </row>
     <row r="83" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="22">
-        <v>39.1</v>
-      </c>
-      <c r="B83" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="C83" s="13"/>
       <c r="D83" s="4"/>
       <c r="F83" s="5"/>
@@ -2547,13 +2680,10 @@
       <c r="Q83" s="5"/>
     </row>
     <row r="84" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="22">
-        <v>39.11</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C84" s="13"/>
+      <c r="B84" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C84" s="14"/>
       <c r="D84" s="4"/>
       <c r="F84" s="5"/>
       <c r="G84" s="4"/>
@@ -2562,6 +2692,7 @@
       <c r="Q84" s="5"/>
     </row>
     <row r="85" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="22"/>
       <c r="C85" s="13"/>
       <c r="D85" s="4"/>
       <c r="F85" s="5"/>
@@ -2571,10 +2702,11 @@
       <c r="Q85" s="5"/>
     </row>
     <row r="86" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B86" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C86" s="14"/>
+      <c r="A86" s="22"/>
+      <c r="B86" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C86" s="13"/>
       <c r="D86" s="4"/>
       <c r="F86" s="5"/>
       <c r="G86" s="4"/>
@@ -2583,7 +2715,12 @@
       <c r="Q86" s="5"/>
     </row>
     <row r="87" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="24"/>
+      <c r="A87" s="20">
+        <v>41.01</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="C87" s="13"/>
       <c r="D87" s="4"/>
       <c r="F87" s="5"/>
@@ -2593,9 +2730,11 @@
       <c r="Q87" s="5"/>
     </row>
     <row r="88" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="24"/>
+      <c r="A88" s="20">
+        <v>41.02</v>
+      </c>
       <c r="B88" s="3" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C88" s="13"/>
       <c r="D88" s="4"/>
@@ -2606,11 +2745,11 @@
       <c r="Q88" s="5"/>
     </row>
     <row r="89" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="22">
-        <v>41.01</v>
+      <c r="A89" s="20">
+        <v>41.03</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C89" s="13"/>
       <c r="D89" s="4"/>
@@ -2621,11 +2760,11 @@
       <c r="Q89" s="5"/>
     </row>
     <row r="90" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="22">
-        <v>41.02</v>
+      <c r="A90" s="20">
+        <v>41.04</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C90" s="13"/>
       <c r="D90" s="4"/>
@@ -2636,11 +2775,11 @@
       <c r="Q90" s="5"/>
     </row>
     <row r="91" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="22">
-        <v>41.03</v>
+      <c r="A91" s="20">
+        <v>41.05</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C91" s="13"/>
       <c r="D91" s="4"/>
@@ -2651,11 +2790,11 @@
       <c r="Q91" s="5"/>
     </row>
     <row r="92" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="22">
-        <v>41.04</v>
+      <c r="A92" s="20">
+        <v>41.06</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C92" s="13"/>
       <c r="D92" s="4"/>
@@ -2666,12 +2805,6 @@
       <c r="Q92" s="5"/>
     </row>
     <row r="93" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="22">
-        <v>41.05</v>
-      </c>
-      <c r="B93" s="3" t="s">
-        <v>75</v>
-      </c>
       <c r="C93" s="13"/>
       <c r="D93" s="4"/>
       <c r="F93" s="5"/>
@@ -2681,13 +2814,10 @@
       <c r="Q93" s="5"/>
     </row>
     <row r="94" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="22">
-        <v>41.06</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C94" s="13"/>
+      <c r="B94" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C94" s="14"/>
       <c r="D94" s="4"/>
       <c r="F94" s="5"/>
       <c r="G94" s="4"/>
@@ -2705,10 +2835,13 @@
       <c r="Q95" s="5"/>
     </row>
     <row r="96" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B96" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C96" s="14"/>
+      <c r="A96" s="20">
+        <v>36.01</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C96" s="13"/>
       <c r="D96" s="4"/>
       <c r="F96" s="5"/>
       <c r="G96" s="4"/>
@@ -2717,6 +2850,12 @@
       <c r="Q96" s="5"/>
     </row>
     <row r="97" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="20">
+        <v>36.020000000000003</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="C97" s="13"/>
       <c r="D97" s="4"/>
       <c r="F97" s="5"/>
@@ -2726,11 +2865,11 @@
       <c r="Q97" s="5"/>
     </row>
     <row r="98" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="22">
-        <v>36.01</v>
+      <c r="A98" s="20">
+        <v>36.03</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C98" s="13"/>
       <c r="D98" s="4"/>
@@ -2741,11 +2880,11 @@
       <c r="Q98" s="5"/>
     </row>
     <row r="99" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="22">
-        <v>36.020000000000003</v>
+      <c r="A99" s="20">
+        <v>36.04</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C99" s="13"/>
       <c r="D99" s="4"/>
@@ -2756,11 +2895,11 @@
       <c r="Q99" s="5"/>
     </row>
     <row r="100" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="22">
-        <v>36.03</v>
+      <c r="A100" s="20">
+        <v>36.049999999999997</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C100" s="13"/>
       <c r="D100" s="4"/>
@@ -2771,11 +2910,11 @@
       <c r="Q100" s="5"/>
     </row>
     <row r="101" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="22">
-        <v>36.04</v>
+      <c r="A101" s="20">
+        <v>36.06</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C101" s="13"/>
       <c r="D101" s="4"/>
@@ -2786,11 +2925,11 @@
       <c r="Q101" s="5"/>
     </row>
     <row r="102" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="22">
-        <v>36.049999999999997</v>
+      <c r="A102" s="20">
+        <v>36.07</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C102" s="13"/>
       <c r="D102" s="4"/>
@@ -2801,11 +2940,11 @@
       <c r="Q102" s="5"/>
     </row>
     <row r="103" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="22">
-        <v>36.06</v>
+      <c r="A103" s="20">
+        <v>36.08</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C103" s="13"/>
       <c r="D103" s="4"/>
@@ -2816,11 +2955,11 @@
       <c r="Q103" s="5"/>
     </row>
     <row r="104" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="22">
-        <v>36.07</v>
+      <c r="A104" s="20">
+        <v>36.090000000000003</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C104" s="13"/>
       <c r="D104" s="4"/>
@@ -2831,11 +2970,11 @@
       <c r="Q104" s="5"/>
     </row>
     <row r="105" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="22">
-        <v>36.08</v>
+      <c r="A105" s="20">
+        <v>36.1</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C105" s="13"/>
       <c r="D105" s="4"/>
@@ -2846,11 +2985,11 @@
       <c r="Q105" s="5"/>
     </row>
     <row r="106" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="22">
-        <v>36.090000000000003</v>
+      <c r="A106" s="20">
+        <v>36.11</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C106" s="13"/>
       <c r="D106" s="4"/>
@@ -2861,11 +3000,11 @@
       <c r="Q106" s="5"/>
     </row>
     <row r="107" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="22">
-        <v>36.1</v>
+      <c r="A107" s="20">
+        <v>36.120000000000097</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C107" s="13"/>
       <c r="D107" s="4"/>
@@ -2876,11 +3015,11 @@
       <c r="Q107" s="5"/>
     </row>
     <row r="108" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="22">
-        <v>36.11</v>
+      <c r="A108" s="20">
+        <v>36.130000000000102</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C108" s="13"/>
       <c r="D108" s="4"/>
@@ -2891,11 +3030,11 @@
       <c r="Q108" s="5"/>
     </row>
     <row r="109" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="22">
-        <v>36.120000000000097</v>
+      <c r="A109" s="20">
+        <v>36.1400000000001</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C109" s="13"/>
       <c r="D109" s="4"/>
@@ -2906,11 +3045,11 @@
       <c r="Q109" s="5"/>
     </row>
     <row r="110" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="22">
-        <v>36.130000000000102</v>
+      <c r="A110" s="20">
+        <v>36.150000000000098</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C110" s="13"/>
       <c r="D110" s="4"/>
@@ -2921,11 +3060,11 @@
       <c r="Q110" s="5"/>
     </row>
     <row r="111" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="22">
-        <v>36.1400000000001</v>
+      <c r="A111" s="20">
+        <v>36.160000000000103</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C111" s="13"/>
       <c r="D111" s="4"/>
@@ -2936,63 +3075,33 @@
       <c r="Q111" s="5"/>
     </row>
     <row r="112" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="22">
-        <v>36.150000000000098</v>
+      <c r="A112" s="20">
+        <v>36.170000000000101</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C112" s="13"/>
-      <c r="D112" s="4"/>
-      <c r="F112" s="5"/>
-      <c r="G112" s="4"/>
-      <c r="M112" s="5"/>
-      <c r="N112" s="4"/>
-      <c r="Q112" s="5"/>
-    </row>
-    <row r="113" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="22">
-        <v>36.160000000000103</v>
-      </c>
-      <c r="B113" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C113" s="13"/>
-      <c r="D113" s="4"/>
-      <c r="F113" s="5"/>
-      <c r="G113" s="4"/>
-      <c r="M113" s="5"/>
-      <c r="N113" s="4"/>
-      <c r="Q113" s="5"/>
-    </row>
-    <row r="114" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="22">
-        <v>36.170000000000101</v>
-      </c>
-      <c r="B114" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C114" s="15"/>
-      <c r="D114" s="6"/>
-      <c r="E114" s="7"/>
-      <c r="F114" s="8"/>
-      <c r="G114" s="6"/>
-      <c r="H114" s="7"/>
-      <c r="I114" s="7"/>
-      <c r="J114" s="7"/>
-      <c r="K114" s="7"/>
-      <c r="L114" s="7"/>
-      <c r="M114" s="8"/>
-      <c r="N114" s="6"/>
-      <c r="O114" s="7"/>
-      <c r="P114" s="7"/>
-      <c r="Q114" s="8"/>
+      <c r="C112" s="15"/>
+      <c r="D112" s="6"/>
+      <c r="E112" s="7"/>
+      <c r="F112" s="8"/>
+      <c r="G112" s="6"/>
+      <c r="H112" s="7"/>
+      <c r="I112" s="7"/>
+      <c r="J112" s="7"/>
+      <c r="K112" s="7"/>
+      <c r="L112" s="7"/>
+      <c r="M112" s="8"/>
+      <c r="N112" s="6"/>
+      <c r="O112" s="7"/>
+      <c r="P112" s="7"/>
+      <c r="Q112" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="N3:Q3"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="G3:M3"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:M2"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
First two stacks-queues problems
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bharat/bctci/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EABE168-7886-5248-AAE6-1683B8B1D5BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44EFF378-C152-4344-9C5B-1B8DCF7CC70C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25600" yWindow="2180" windowWidth="26880" windowHeight="15120" xr2:uid="{233FF15D-0BCB-6B46-B450-599851EED7C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="173">
   <si>
     <t>Sets &amp; Maps</t>
   </si>
@@ -524,6 +525,39 @@
   </si>
   <si>
     <t>Spend time writing out the algorithm so that interviewer can call out code smells</t>
+  </si>
+  <si>
+    <t>In a loop, keep compressing array until fully compressed</t>
+  </si>
+  <si>
+    <t>Started with an excessively complex test case. Should have used a simpler test case</t>
+  </si>
+  <si>
+    <t>Didn't even use a stack</t>
+  </si>
+  <si>
+    <t>Better to iterate through the whole array, and process that number wrt stack</t>
+  </si>
+  <si>
+    <t>Awkward handling of last character when doing pairwise comparison</t>
+  </si>
+  <si>
+    <t>Stacking loop</t>
+  </si>
+  <si>
+    <t>Like candy crush, iterate over array and stack, keep a loop to compress if last k elements in the stack are the same</t>
+  </si>
+  <si>
+    <t>Using a stack with metadata, which is arguable, in my opinion</t>
+  </si>
+  <si>
+    <t>Variation of previous problem</t>
+  </si>
+  <si>
+    <t>Test cases were fine</t>
+  </si>
+  <si>
+    <t>I think my solution was clearer</t>
   </si>
 </sst>
 </file>
@@ -533,7 +567,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -563,6 +597,24 @@
       <sz val="14"/>
       <color theme="1"/>
       <name val="Aptos ExtraBold"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -736,7 +788,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -792,19 +844,38 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1144,8 +1215,8 @@
   <dimension ref="A1:Q112"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q10" sqref="Q10"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1224,26 +1295,26 @@
       <c r="C2" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="33" t="s">
         <v>112</v>
       </c>
-      <c r="E2" s="24"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="23" t="s">
+      <c r="E2" s="31"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="23" t="s">
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="27"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="32"/>
     </row>
     <row r="3" spans="1:17" s="10" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="18">
@@ -1738,35 +1809,107 @@
       <c r="N16" s="4"/>
       <c r="Q16" s="5"/>
     </row>
-    <row r="17" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" ht="100" x14ac:dyDescent="0.25">
       <c r="A17" s="20">
         <v>32.01</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="4"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="4"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="4"/>
-      <c r="Q17" s="5"/>
-    </row>
-    <row r="18" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="D17" s="19">
+        <v>45864</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="J17" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="M17" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="N17" s="9">
+        <v>2</v>
+      </c>
+      <c r="O17" s="10">
+        <v>3</v>
+      </c>
+      <c r="P17" s="10">
+        <v>2</v>
+      </c>
+      <c r="Q17" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="80" x14ac:dyDescent="0.25">
       <c r="A18" s="20">
         <v>32.020000000000003</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="4"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="4"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="4"/>
-      <c r="Q18" s="5"/>
+      <c r="C18" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="D18" s="19">
+        <v>45864</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="J18" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="M18" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="N18" s="9">
+        <v>4</v>
+      </c>
+      <c r="O18" s="10">
+        <v>4</v>
+      </c>
+      <c r="P18" s="10">
+        <v>3</v>
+      </c>
+      <c r="Q18" s="11">
+        <v>4</v>
+      </c>
     </row>
     <row r="19" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20">
@@ -3106,4 +3249,288 @@
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6E5E05C-FD85-A84F-B5CD-386963B8CD1F}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="D6:E39"/>
+  <sheetViews>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="4" width="10.83203125" style="25"/>
+    <col min="5" max="5" width="17.1640625" style="25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="25"/>
+    <col min="7" max="7" width="22.1640625" style="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="25"/>
+    <col min="9" max="9" width="21.6640625" style="25" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="25"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D6" s="23"/>
+      <c r="E6" s="24" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D7" s="23"/>
+      <c r="E7" s="24"/>
+    </row>
+    <row r="8" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D8" s="26">
+        <v>33.01</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D9" s="26">
+        <v>33.020000000000003</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D10" s="29">
+        <v>1</v>
+      </c>
+      <c r="E10" s="27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D11" s="29">
+        <v>2</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D12" s="29">
+        <v>3</v>
+      </c>
+      <c r="E12" s="27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D13" s="26">
+        <v>33.03</v>
+      </c>
+      <c r="E13" s="27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D14" s="29">
+        <v>4</v>
+      </c>
+      <c r="E14" s="27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D15" s="29">
+        <v>5</v>
+      </c>
+      <c r="E15" s="27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D16" s="26">
+        <v>33.04</v>
+      </c>
+      <c r="E16" s="27" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D17" s="26">
+        <v>33.049999999999997</v>
+      </c>
+      <c r="E17" s="27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D18" s="23"/>
+      <c r="E18" s="27"/>
+    </row>
+    <row r="19" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D19" s="23"/>
+      <c r="E19" s="24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D20" s="23"/>
+      <c r="E20" s="24"/>
+    </row>
+    <row r="21" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D21" s="28">
+        <v>35.000999999999998</v>
+      </c>
+      <c r="E21" s="27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D22" s="28">
+        <v>35.002000000000002</v>
+      </c>
+      <c r="E22" s="27" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D23" s="26">
+        <v>35.01</v>
+      </c>
+      <c r="E23" s="27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D24" s="26">
+        <v>35.020000000000003</v>
+      </c>
+      <c r="E24" s="27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D25" s="26">
+        <v>35.03</v>
+      </c>
+      <c r="E25" s="27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D26" s="26">
+        <v>35.04</v>
+      </c>
+      <c r="E26" s="27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D27" s="26">
+        <v>35.049999999999997</v>
+      </c>
+      <c r="E27" s="27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D28" s="26">
+        <v>35.06</v>
+      </c>
+      <c r="E28" s="27" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D29" s="26">
+        <v>35.07</v>
+      </c>
+      <c r="E29" s="27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D30" s="26">
+        <v>35.08</v>
+      </c>
+      <c r="E30" s="27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D31" s="26">
+        <v>35.090000000000003</v>
+      </c>
+      <c r="E31" s="27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D32" s="26">
+        <v>35.1</v>
+      </c>
+      <c r="E32" s="27" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D33" s="26">
+        <v>35.11</v>
+      </c>
+      <c r="E33" s="27" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D34" s="26">
+        <v>35.120000000000097</v>
+      </c>
+      <c r="E34" s="27" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D35" s="26">
+        <v>35.130000000000102</v>
+      </c>
+      <c r="E35" s="27" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D36" s="26">
+        <v>35.1400000000001</v>
+      </c>
+      <c r="E36" s="27" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D37" s="26">
+        <v>35.150000000000098</v>
+      </c>
+      <c r="E37" s="27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="38" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D38" s="26">
+        <v>35.160000000000103</v>
+      </c>
+      <c r="E38" s="27" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D39" s="26">
+        <v>35.170000000000101</v>
+      </c>
+      <c r="E39" s="27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Medium difficulty set&map problem
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bharat/bctci/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44EFF378-C152-4344-9C5B-1B8DCF7CC70C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B426B2A-8AC8-894E-AE1D-B6F497303533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="2180" windowWidth="26880" windowHeight="15120" xr2:uid="{233FF15D-0BCB-6B46-B450-599851EED7C1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{233FF15D-0BCB-6B46-B450-599851EED7C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="179">
   <si>
     <t>Sets &amp; Maps</t>
   </si>
@@ -558,6 +558,24 @@
   </si>
   <si>
     <t>I think my solution was clearer</t>
+  </si>
+  <si>
+    <t>Two dictionaries, one for seating per row, one for mistakes. Iterate over seating, and check if mistakes dictionary has consecutive students</t>
+  </si>
+  <si>
+    <t>Check for consecutive and same row can be done in the same loop, and no need for a sparse array</t>
+  </si>
+  <si>
+    <t>Time complexity yes, space complexity no</t>
+  </si>
+  <si>
+    <t>The fact that row number was not important in result</t>
+  </si>
+  <si>
+    <t>That accessing an uninitialised member for defaultdict via subscript initialises, and to use get instead</t>
+  </si>
+  <si>
+    <t>Fairly well done</t>
   </si>
 </sst>
 </file>
@@ -788,7 +806,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -797,8 +815,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -813,12 +829,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1214,14 +1224,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4095FB6B-33CD-C94D-A3B2-EAADF58B3AE5}">
   <dimension ref="A1:Q112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q18" sqref="Q18"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.83203125" style="20" customWidth="1"/>
+    <col min="1" max="1" width="14.83203125" style="16"/>
     <col min="2" max="3" width="39.33203125" style="3" customWidth="1"/>
     <col min="4" max="4" width="13.83203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="15.1640625" style="1" customWidth="1"/>
@@ -1240,51 +1250,51 @@
     <col min="18" max="16384" width="14.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="16" customFormat="1" ht="68" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="18"/>
-      <c r="C1" s="17" t="s">
+    <row r="1" spans="1:17" s="12" customFormat="1" ht="68" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14"/>
+      <c r="C1" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="M1" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="O1" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="P1" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="Q1" s="11" t="s">
+      <c r="Q1" s="9" t="s">
         <v>110</v>
       </c>
     </row>
@@ -1292,1953 +1302,2751 @@
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="D2" s="33" t="s">
+      <c r="D2" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="E2" s="31"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="30" t="s">
+      <c r="E2" s="27"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="30" t="s">
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="O2" s="31"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="32"/>
-    </row>
-    <row r="3" spans="1:17" s="10" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="18">
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
+      <c r="Q2" s="28"/>
+    </row>
+    <row r="3" spans="1:17" s="8" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="14">
         <v>30.01</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="D3" s="19">
+      <c r="D3" s="15">
         <v>45862</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="K3" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="L3" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="M3" s="11" t="s">
+      <c r="M3" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="N3" s="9">
+      <c r="N3" s="7">
         <v>4</v>
       </c>
-      <c r="O3" s="10">
+      <c r="O3" s="8">
         <v>3</v>
       </c>
-      <c r="P3" s="10">
+      <c r="P3" s="8">
         <v>3</v>
       </c>
-      <c r="Q3" s="11">
+      <c r="Q3" s="9">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="20">
+      <c r="A4" s="16">
         <v>30.02</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="15">
         <v>45862</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I4" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="J4" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="K4" s="10" t="s">
+      <c r="K4" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="L4" s="10" t="s">
+      <c r="L4" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="M4" s="11" t="s">
+      <c r="M4" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="N4" s="9">
+      <c r="N4" s="7">
         <v>4</v>
       </c>
-      <c r="O4" s="10">
+      <c r="O4" s="8">
         <v>4</v>
       </c>
-      <c r="P4" s="10">
+      <c r="P4" s="8">
         <v>3</v>
       </c>
-      <c r="Q4" s="11">
+      <c r="Q4" s="9">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="20">
+      <c r="A5" s="16">
         <v>30.03</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="15">
         <v>45863</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="I5" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="J5" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="K5" s="10" t="s">
+      <c r="K5" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="L5" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="M5" s="11" t="s">
+      <c r="M5" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="N5" s="9">
+      <c r="N5" s="7">
         <v>5</v>
       </c>
-      <c r="O5" s="10">
+      <c r="O5" s="8">
         <v>5</v>
       </c>
-      <c r="P5" s="10">
+      <c r="P5" s="8">
         <v>4</v>
       </c>
-      <c r="Q5" s="11">
+      <c r="Q5" s="9">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="20">
+      <c r="A6" s="16">
         <v>30.04</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="15">
         <v>45864</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="I6" s="10" t="s">
+      <c r="I6" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="J6" s="10" t="s">
+      <c r="J6" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="K6" s="10" t="s">
+      <c r="K6" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="L6" s="10" t="s">
+      <c r="L6" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="M6" s="11" t="s">
+      <c r="M6" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="N6" s="9">
+      <c r="N6" s="7">
         <v>3</v>
       </c>
-      <c r="O6" s="10">
+      <c r="O6" s="8">
         <v>4</v>
       </c>
-      <c r="P6" s="10">
+      <c r="P6" s="8">
         <v>4</v>
       </c>
-      <c r="Q6" s="11">
+      <c r="Q6" s="9">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="116" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="20">
+      <c r="A7" s="16">
         <v>30.05</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="D7" s="19">
+      <c r="D7" s="15">
         <v>45864</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="H7" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="I7" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="J7" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="K7" s="10" t="s">
+      <c r="K7" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="L7" s="10" t="s">
+      <c r="L7" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="M7" s="11" t="s">
+      <c r="M7" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="N7" s="9">
+      <c r="N7" s="7">
         <v>4</v>
       </c>
-      <c r="O7" s="10">
+      <c r="O7" s="8">
         <v>4</v>
       </c>
-      <c r="P7" s="10">
+      <c r="P7" s="8">
         <v>3</v>
       </c>
-      <c r="Q7" s="11">
+      <c r="Q7" s="9">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="20">
+      <c r="A8" s="16">
         <v>30.06</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="D8" s="19">
+      <c r="D8" s="15">
         <v>45864</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H8" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="I8" s="10" t="s">
+      <c r="I8" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="J8" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="K8" s="10" t="s">
+      <c r="K8" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="L8" s="10" t="s">
+      <c r="L8" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="M8" s="11" t="s">
+      <c r="M8" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="N8" s="9">
+      <c r="N8" s="7">
         <v>4</v>
       </c>
-      <c r="O8" s="10">
+      <c r="O8" s="8">
         <v>4</v>
       </c>
-      <c r="P8" s="10">
+      <c r="P8" s="8">
         <v>4</v>
       </c>
-      <c r="Q8" s="11">
+      <c r="Q8" s="9">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="100" x14ac:dyDescent="0.25">
-      <c r="A9" s="20">
+      <c r="A9" s="16">
         <v>30.07</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="D9" s="19">
+      <c r="D9" s="15">
         <v>45864</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="H9" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="I9" s="10" t="s">
+      <c r="I9" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="J9" s="10" t="s">
+      <c r="J9" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="K9" s="10" t="s">
+      <c r="K9" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="L9" s="10" t="s">
+      <c r="L9" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="M9" s="11" t="s">
+      <c r="M9" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="N9" s="9">
+      <c r="N9" s="7">
         <v>4</v>
       </c>
-      <c r="O9" s="10">
+      <c r="O9" s="8">
         <v>3</v>
       </c>
-      <c r="P9" s="10">
+      <c r="P9" s="8">
         <v>5</v>
       </c>
-      <c r="Q9" s="11">
+      <c r="Q9" s="9">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="20">
+      <c r="A10" s="16">
         <v>30.08</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="11"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
-      <c r="Q10" s="11"/>
+      <c r="C10" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="D10" s="15">
+        <v>45865</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="M10" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="N10" s="7">
+        <v>4</v>
+      </c>
+      <c r="O10" s="8">
+        <v>3</v>
+      </c>
+      <c r="P10" s="8">
+        <v>4</v>
+      </c>
+      <c r="Q10" s="9">
+        <v>4</v>
+      </c>
     </row>
     <row r="11" spans="1:17" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="20">
+      <c r="A11" s="16">
         <v>30.09</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="11"/>
-      <c r="N11" s="9"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="10"/>
-      <c r="Q11" s="11"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="9"/>
     </row>
     <row r="12" spans="1:17" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="20">
+      <c r="A12" s="16">
         <v>30.1</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="17"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="11"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="10"/>
-      <c r="Q12" s="11"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="9"/>
     </row>
     <row r="13" spans="1:17" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="20">
+      <c r="A13" s="16">
         <v>30.11</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="11"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="10"/>
-      <c r="Q13" s="11"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="9"/>
     </row>
     <row r="14" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="13"/>
-      <c r="D14" s="4"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="4"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="4"/>
-      <c r="Q14" s="5"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="9"/>
     </row>
     <row r="15" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="4"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="4"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="4"/>
-      <c r="Q15" s="5"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="9"/>
     </row>
     <row r="16" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="13"/>
-      <c r="D16" s="4"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="4"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="4"/>
-      <c r="Q16" s="5"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="9"/>
     </row>
     <row r="17" spans="1:17" ht="100" x14ac:dyDescent="0.25">
-      <c r="A17" s="20">
+      <c r="A17" s="16">
         <v>32.01</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="D17" s="19">
+      <c r="D17" s="15">
         <v>45864</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="F17" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="G17" s="9" t="s">
+      <c r="G17" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="H17" s="10" t="s">
+      <c r="H17" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="I17" s="10" t="s">
+      <c r="I17" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="J17" s="10" t="s">
+      <c r="J17" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10" t="s">
+      <c r="K17" s="8"/>
+      <c r="L17" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="M17" s="11" t="s">
+      <c r="M17" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="N17" s="9">
+      <c r="N17" s="7">
         <v>2</v>
       </c>
-      <c r="O17" s="10">
+      <c r="O17" s="8">
         <v>3</v>
       </c>
-      <c r="P17" s="10">
+      <c r="P17" s="8">
         <v>2</v>
       </c>
-      <c r="Q17" s="11">
+      <c r="Q17" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:17" ht="80" x14ac:dyDescent="0.25">
-      <c r="A18" s="20">
+      <c r="A18" s="16">
         <v>32.020000000000003</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="D18" s="19">
+      <c r="D18" s="15">
         <v>45864</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F18" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="G18" s="9" t="s">
+      <c r="G18" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="H18" s="10" t="s">
+      <c r="H18" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="I18" s="10" t="s">
+      <c r="I18" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="J18" s="10" t="s">
+      <c r="J18" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10" t="s">
+      <c r="K18" s="8"/>
+      <c r="L18" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="M18" s="11" t="s">
+      <c r="M18" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="N18" s="9">
+      <c r="N18" s="7">
         <v>4</v>
       </c>
-      <c r="O18" s="10">
+      <c r="O18" s="8">
         <v>4</v>
       </c>
-      <c r="P18" s="10">
+      <c r="P18" s="8">
         <v>3</v>
       </c>
-      <c r="Q18" s="11">
+      <c r="Q18" s="9">
         <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="20">
+      <c r="A19" s="16">
         <v>32.03</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C19" s="13"/>
-      <c r="D19" s="4"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="4"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="4"/>
-      <c r="Q19" s="5"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
+      <c r="Q19" s="9"/>
     </row>
     <row r="20" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="20">
+      <c r="A20" s="16">
         <v>32.04</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C20" s="13"/>
-      <c r="D20" s="4"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="4"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="4"/>
-      <c r="Q20" s="5"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="9"/>
     </row>
     <row r="21" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="20">
+      <c r="A21" s="16">
         <v>32.049999999999997</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C21" s="13"/>
-      <c r="D21" s="4"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="4"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="4"/>
-      <c r="Q21" s="5"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8"/>
+      <c r="Q21" s="9"/>
     </row>
     <row r="22" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="20">
+      <c r="A22" s="16">
         <v>32.06</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C22" s="13"/>
-      <c r="D22" s="4"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="4"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="4"/>
-      <c r="Q22" s="5"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="7"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
+      <c r="Q22" s="9"/>
     </row>
     <row r="23" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="20">
+      <c r="A23" s="16">
         <v>32.07</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C23" s="13"/>
-      <c r="D23" s="4"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="4"/>
-      <c r="M23" s="5"/>
-      <c r="N23" s="4"/>
-      <c r="Q23" s="5"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="8"/>
+      <c r="Q23" s="9"/>
     </row>
     <row r="24" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="20">
+      <c r="A24" s="16">
         <v>32.08</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C24" s="13"/>
-      <c r="D24" s="4"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="4"/>
-      <c r="M24" s="5"/>
-      <c r="N24" s="4"/>
-      <c r="Q24" s="5"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="8"/>
+      <c r="Q24" s="9"/>
     </row>
     <row r="25" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="13"/>
-      <c r="D25" s="4"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="4"/>
-      <c r="M25" s="5"/>
-      <c r="N25" s="4"/>
-      <c r="Q25" s="5"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="8"/>
+      <c r="Q25" s="9"/>
     </row>
     <row r="26" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="14"/>
-      <c r="D26" s="4"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="4"/>
-      <c r="M26" s="5"/>
-      <c r="N26" s="4"/>
-      <c r="Q26" s="5"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="8"/>
+      <c r="P26" s="8"/>
+      <c r="Q26" s="9"/>
     </row>
     <row r="27" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="4"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="4"/>
-      <c r="M27" s="5"/>
-      <c r="N27" s="4"/>
-      <c r="Q27" s="5"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="9"/>
+      <c r="N27" s="7"/>
+      <c r="O27" s="8"/>
+      <c r="P27" s="8"/>
+      <c r="Q27" s="9"/>
     </row>
     <row r="28" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="20">
+      <c r="A28" s="16">
         <v>33.01</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C28" s="13"/>
-      <c r="D28" s="4"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="4"/>
-      <c r="M28" s="5"/>
-      <c r="N28" s="4"/>
-      <c r="Q28" s="5"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="8"/>
+      <c r="P28" s="8"/>
+      <c r="Q28" s="9"/>
     </row>
     <row r="29" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="20">
+      <c r="A29" s="16">
         <v>33.020000000000003</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C29" s="13"/>
-      <c r="D29" s="4"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="4"/>
-      <c r="M29" s="5"/>
-      <c r="N29" s="4"/>
-      <c r="Q29" s="5"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="9"/>
+      <c r="N29" s="7"/>
+      <c r="O29" s="8"/>
+      <c r="P29" s="8"/>
+      <c r="Q29" s="9"/>
     </row>
     <row r="30" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="21">
+      <c r="A30" s="17">
         <v>1</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>29</v>
       </c>
       <c r="C30" s="13"/>
-      <c r="D30" s="4"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="4"/>
-      <c r="M30" s="5"/>
-      <c r="N30" s="4"/>
-      <c r="Q30" s="5"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
+      <c r="L30" s="8"/>
+      <c r="M30" s="9"/>
+      <c r="N30" s="7"/>
+      <c r="O30" s="8"/>
+      <c r="P30" s="8"/>
+      <c r="Q30" s="9"/>
     </row>
     <row r="31" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="21">
+      <c r="A31" s="17">
         <v>2</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C31" s="13"/>
-      <c r="D31" s="4"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="4"/>
-      <c r="M31" s="5"/>
-      <c r="N31" s="4"/>
-      <c r="Q31" s="5"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
+      <c r="L31" s="8"/>
+      <c r="M31" s="9"/>
+      <c r="N31" s="7"/>
+      <c r="O31" s="8"/>
+      <c r="P31" s="8"/>
+      <c r="Q31" s="9"/>
     </row>
     <row r="32" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="21">
+      <c r="A32" s="17">
         <v>3</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C32" s="13"/>
-      <c r="D32" s="4"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="4"/>
-      <c r="M32" s="5"/>
-      <c r="N32" s="4"/>
-      <c r="Q32" s="5"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="8"/>
+      <c r="L32" s="8"/>
+      <c r="M32" s="9"/>
+      <c r="N32" s="7"/>
+      <c r="O32" s="8"/>
+      <c r="P32" s="8"/>
+      <c r="Q32" s="9"/>
     </row>
     <row r="33" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="20">
+      <c r="A33" s="16">
         <v>33.03</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C33" s="13"/>
-      <c r="D33" s="4"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="4"/>
-      <c r="M33" s="5"/>
-      <c r="N33" s="4"/>
-      <c r="Q33" s="5"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8"/>
+      <c r="K33" s="8"/>
+      <c r="L33" s="8"/>
+      <c r="M33" s="9"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="8"/>
+      <c r="P33" s="8"/>
+      <c r="Q33" s="9"/>
     </row>
     <row r="34" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="21">
+      <c r="A34" s="17">
         <v>4</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C34" s="13"/>
-      <c r="D34" s="4"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="4"/>
-      <c r="M34" s="5"/>
-      <c r="N34" s="4"/>
-      <c r="Q34" s="5"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="8"/>
+      <c r="M34" s="9"/>
+      <c r="N34" s="7"/>
+      <c r="O34" s="8"/>
+      <c r="P34" s="8"/>
+      <c r="Q34" s="9"/>
     </row>
     <row r="35" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="21">
+      <c r="A35" s="17">
         <v>5</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>24</v>
       </c>
       <c r="C35" s="13"/>
-      <c r="D35" s="4"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="4"/>
-      <c r="M35" s="5"/>
-      <c r="N35" s="4"/>
-      <c r="Q35" s="5"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="8"/>
+      <c r="K35" s="8"/>
+      <c r="L35" s="8"/>
+      <c r="M35" s="9"/>
+      <c r="N35" s="7"/>
+      <c r="O35" s="8"/>
+      <c r="P35" s="8"/>
+      <c r="Q35" s="9"/>
     </row>
     <row r="36" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="20">
+      <c r="A36" s="16">
         <v>33.04</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C36" s="13"/>
-      <c r="D36" s="4"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="4"/>
-      <c r="M36" s="5"/>
-      <c r="N36" s="4"/>
-      <c r="Q36" s="5"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="8"/>
+      <c r="L36" s="8"/>
+      <c r="M36" s="9"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="8"/>
+      <c r="P36" s="8"/>
+      <c r="Q36" s="9"/>
     </row>
     <row r="37" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="20">
+      <c r="A37" s="16">
         <v>33.049999999999997</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C37" s="13"/>
-      <c r="D37" s="4"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="4"/>
-      <c r="M37" s="5"/>
-      <c r="N37" s="4"/>
-      <c r="Q37" s="5"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
+      <c r="L37" s="8"/>
+      <c r="M37" s="9"/>
+      <c r="N37" s="7"/>
+      <c r="O37" s="8"/>
+      <c r="P37" s="8"/>
+      <c r="Q37" s="9"/>
     </row>
     <row r="38" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C38" s="13"/>
-      <c r="D38" s="4"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="4"/>
-      <c r="M38" s="5"/>
-      <c r="N38" s="4"/>
-      <c r="Q38" s="5"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
+      <c r="K38" s="8"/>
+      <c r="L38" s="8"/>
+      <c r="M38" s="9"/>
+      <c r="N38" s="7"/>
+      <c r="O38" s="8"/>
+      <c r="P38" s="8"/>
+      <c r="Q38" s="9"/>
     </row>
     <row r="39" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C39" s="14"/>
-      <c r="D39" s="4"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="4"/>
-      <c r="M39" s="5"/>
-      <c r="N39" s="4"/>
-      <c r="Q39" s="5"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
+      <c r="K39" s="8"/>
+      <c r="L39" s="8"/>
+      <c r="M39" s="9"/>
+      <c r="N39" s="7"/>
+      <c r="O39" s="8"/>
+      <c r="P39" s="8"/>
+      <c r="Q39" s="9"/>
     </row>
     <row r="40" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="2"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="4"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="4"/>
-      <c r="M40" s="5"/>
-      <c r="N40" s="4"/>
-      <c r="Q40" s="5"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="8"/>
+      <c r="J40" s="8"/>
+      <c r="K40" s="8"/>
+      <c r="L40" s="8"/>
+      <c r="M40" s="9"/>
+      <c r="N40" s="7"/>
+      <c r="O40" s="8"/>
+      <c r="P40" s="8"/>
+      <c r="Q40" s="9"/>
     </row>
     <row r="41" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="22">
+      <c r="A41" s="18">
         <v>35.000999999999998</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C41" s="13"/>
-      <c r="D41" s="4"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="4"/>
-      <c r="M41" s="5"/>
-      <c r="N41" s="4"/>
-      <c r="Q41" s="5"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="8"/>
+      <c r="J41" s="8"/>
+      <c r="K41" s="8"/>
+      <c r="L41" s="8"/>
+      <c r="M41" s="9"/>
+      <c r="N41" s="7"/>
+      <c r="O41" s="8"/>
+      <c r="P41" s="8"/>
+      <c r="Q41" s="9"/>
     </row>
     <row r="42" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="22">
+      <c r="A42" s="18">
         <v>35.002000000000002</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C42" s="13"/>
-      <c r="D42" s="4"/>
-      <c r="F42" s="5"/>
-      <c r="G42" s="4"/>
-      <c r="M42" s="5"/>
-      <c r="N42" s="4"/>
-      <c r="Q42" s="5"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
+      <c r="J42" s="8"/>
+      <c r="K42" s="8"/>
+      <c r="L42" s="8"/>
+      <c r="M42" s="9"/>
+      <c r="N42" s="7"/>
+      <c r="O42" s="8"/>
+      <c r="P42" s="8"/>
+      <c r="Q42" s="9"/>
     </row>
     <row r="43" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="20">
+      <c r="A43" s="16">
         <v>35.01</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C43" s="13"/>
-      <c r="D43" s="4"/>
-      <c r="F43" s="5"/>
-      <c r="G43" s="4"/>
-      <c r="M43" s="5"/>
-      <c r="N43" s="4"/>
-      <c r="Q43" s="5"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8"/>
+      <c r="J43" s="8"/>
+      <c r="K43" s="8"/>
+      <c r="L43" s="8"/>
+      <c r="M43" s="9"/>
+      <c r="N43" s="7"/>
+      <c r="O43" s="8"/>
+      <c r="P43" s="8"/>
+      <c r="Q43" s="9"/>
     </row>
     <row r="44" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="20">
+      <c r="A44" s="16">
         <v>35.020000000000003</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C44" s="13"/>
-      <c r="D44" s="4"/>
-      <c r="F44" s="5"/>
-      <c r="G44" s="4"/>
-      <c r="M44" s="5"/>
-      <c r="N44" s="4"/>
-      <c r="Q44" s="5"/>
+      <c r="D44" s="15"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="8"/>
+      <c r="J44" s="8"/>
+      <c r="K44" s="8"/>
+      <c r="L44" s="8"/>
+      <c r="M44" s="9"/>
+      <c r="N44" s="7"/>
+      <c r="O44" s="8"/>
+      <c r="P44" s="8"/>
+      <c r="Q44" s="9"/>
     </row>
     <row r="45" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="20">
+      <c r="A45" s="16">
         <v>35.03</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>37</v>
       </c>
       <c r="C45" s="13"/>
-      <c r="D45" s="4"/>
-      <c r="F45" s="5"/>
-      <c r="G45" s="4"/>
-      <c r="M45" s="5"/>
-      <c r="N45" s="4"/>
-      <c r="Q45" s="5"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="8"/>
+      <c r="I45" s="8"/>
+      <c r="J45" s="8"/>
+      <c r="K45" s="8"/>
+      <c r="L45" s="8"/>
+      <c r="M45" s="9"/>
+      <c r="N45" s="7"/>
+      <c r="O45" s="8"/>
+      <c r="P45" s="8"/>
+      <c r="Q45" s="9"/>
     </row>
     <row r="46" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="20">
+      <c r="A46" s="16">
         <v>35.04</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>38</v>
       </c>
       <c r="C46" s="13"/>
-      <c r="D46" s="4"/>
-      <c r="F46" s="5"/>
-      <c r="G46" s="4"/>
-      <c r="M46" s="5"/>
-      <c r="N46" s="4"/>
-      <c r="Q46" s="5"/>
+      <c r="D46" s="15"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="7"/>
+      <c r="H46" s="8"/>
+      <c r="I46" s="8"/>
+      <c r="J46" s="8"/>
+      <c r="K46" s="8"/>
+      <c r="L46" s="8"/>
+      <c r="M46" s="9"/>
+      <c r="N46" s="7"/>
+      <c r="O46" s="8"/>
+      <c r="P46" s="8"/>
+      <c r="Q46" s="9"/>
     </row>
     <row r="47" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="20">
+      <c r="A47" s="16">
         <v>35.049999999999997</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>39</v>
       </c>
       <c r="C47" s="13"/>
-      <c r="D47" s="4"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="4"/>
-      <c r="M47" s="5"/>
-      <c r="N47" s="4"/>
-      <c r="Q47" s="5"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="9"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="8"/>
+      <c r="I47" s="8"/>
+      <c r="J47" s="8"/>
+      <c r="K47" s="8"/>
+      <c r="L47" s="8"/>
+      <c r="M47" s="9"/>
+      <c r="N47" s="7"/>
+      <c r="O47" s="8"/>
+      <c r="P47" s="8"/>
+      <c r="Q47" s="9"/>
     </row>
     <row r="48" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="20">
+      <c r="A48" s="16">
         <v>35.06</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>40</v>
       </c>
       <c r="C48" s="13"/>
-      <c r="D48" s="4"/>
-      <c r="F48" s="5"/>
-      <c r="G48" s="4"/>
-      <c r="M48" s="5"/>
-      <c r="N48" s="4"/>
-      <c r="Q48" s="5"/>
+      <c r="D48" s="15"/>
+      <c r="E48" s="8"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="7"/>
+      <c r="H48" s="8"/>
+      <c r="I48" s="8"/>
+      <c r="J48" s="8"/>
+      <c r="K48" s="8"/>
+      <c r="L48" s="8"/>
+      <c r="M48" s="9"/>
+      <c r="N48" s="7"/>
+      <c r="O48" s="8"/>
+      <c r="P48" s="8"/>
+      <c r="Q48" s="9"/>
     </row>
     <row r="49" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="20">
+      <c r="A49" s="16">
         <v>35.07</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C49" s="13"/>
-      <c r="D49" s="4"/>
-      <c r="F49" s="5"/>
-      <c r="G49" s="4"/>
-      <c r="M49" s="5"/>
-      <c r="N49" s="4"/>
-      <c r="Q49" s="5"/>
+      <c r="D49" s="15"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="9"/>
+      <c r="G49" s="7"/>
+      <c r="H49" s="8"/>
+      <c r="I49" s="8"/>
+      <c r="J49" s="8"/>
+      <c r="K49" s="8"/>
+      <c r="L49" s="8"/>
+      <c r="M49" s="9"/>
+      <c r="N49" s="7"/>
+      <c r="O49" s="8"/>
+      <c r="P49" s="8"/>
+      <c r="Q49" s="9"/>
     </row>
     <row r="50" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="20">
+      <c r="A50" s="16">
         <v>35.08</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>42</v>
       </c>
       <c r="C50" s="13"/>
-      <c r="D50" s="4"/>
-      <c r="F50" s="5"/>
-      <c r="G50" s="4"/>
-      <c r="M50" s="5"/>
-      <c r="N50" s="4"/>
-      <c r="Q50" s="5"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="8"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="7"/>
+      <c r="H50" s="8"/>
+      <c r="I50" s="8"/>
+      <c r="J50" s="8"/>
+      <c r="K50" s="8"/>
+      <c r="L50" s="8"/>
+      <c r="M50" s="9"/>
+      <c r="N50" s="7"/>
+      <c r="O50" s="8"/>
+      <c r="P50" s="8"/>
+      <c r="Q50" s="9"/>
     </row>
     <row r="51" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="20">
+      <c r="A51" s="16">
         <v>35.090000000000003</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>43</v>
       </c>
       <c r="C51" s="13"/>
-      <c r="D51" s="4"/>
-      <c r="F51" s="5"/>
-      <c r="G51" s="4"/>
-      <c r="M51" s="5"/>
-      <c r="N51" s="4"/>
-      <c r="Q51" s="5"/>
+      <c r="D51" s="15"/>
+      <c r="E51" s="8"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="7"/>
+      <c r="H51" s="8"/>
+      <c r="I51" s="8"/>
+      <c r="J51" s="8"/>
+      <c r="K51" s="8"/>
+      <c r="L51" s="8"/>
+      <c r="M51" s="9"/>
+      <c r="N51" s="7"/>
+      <c r="O51" s="8"/>
+      <c r="P51" s="8"/>
+      <c r="Q51" s="9"/>
     </row>
     <row r="52" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="20">
+      <c r="A52" s="16">
         <v>35.1</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>44</v>
       </c>
       <c r="C52" s="13"/>
-      <c r="D52" s="4"/>
-      <c r="F52" s="5"/>
-      <c r="G52" s="4"/>
-      <c r="M52" s="5"/>
-      <c r="N52" s="4"/>
-      <c r="Q52" s="5"/>
+      <c r="D52" s="15"/>
+      <c r="E52" s="8"/>
+      <c r="F52" s="9"/>
+      <c r="G52" s="7"/>
+      <c r="H52" s="8"/>
+      <c r="I52" s="8"/>
+      <c r="J52" s="8"/>
+      <c r="K52" s="8"/>
+      <c r="L52" s="8"/>
+      <c r="M52" s="9"/>
+      <c r="N52" s="7"/>
+      <c r="O52" s="8"/>
+      <c r="P52" s="8"/>
+      <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="20">
+      <c r="A53" s="16">
         <v>35.11</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>45</v>
       </c>
       <c r="C53" s="13"/>
-      <c r="D53" s="4"/>
-      <c r="F53" s="5"/>
-      <c r="G53" s="4"/>
-      <c r="M53" s="5"/>
-      <c r="N53" s="4"/>
-      <c r="Q53" s="5"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="8"/>
+      <c r="F53" s="9"/>
+      <c r="G53" s="7"/>
+      <c r="H53" s="8"/>
+      <c r="I53" s="8"/>
+      <c r="J53" s="8"/>
+      <c r="K53" s="8"/>
+      <c r="L53" s="8"/>
+      <c r="M53" s="9"/>
+      <c r="N53" s="7"/>
+      <c r="O53" s="8"/>
+      <c r="P53" s="8"/>
+      <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="20">
+      <c r="A54" s="16">
         <v>35.120000000000097</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>46</v>
       </c>
       <c r="C54" s="13"/>
-      <c r="D54" s="4"/>
-      <c r="F54" s="5"/>
-      <c r="G54" s="4"/>
-      <c r="M54" s="5"/>
-      <c r="N54" s="4"/>
-      <c r="Q54" s="5"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="8"/>
+      <c r="F54" s="9"/>
+      <c r="G54" s="7"/>
+      <c r="H54" s="8"/>
+      <c r="I54" s="8"/>
+      <c r="J54" s="8"/>
+      <c r="K54" s="8"/>
+      <c r="L54" s="8"/>
+      <c r="M54" s="9"/>
+      <c r="N54" s="7"/>
+      <c r="O54" s="8"/>
+      <c r="P54" s="8"/>
+      <c r="Q54" s="9"/>
     </row>
     <row r="55" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="20">
+      <c r="A55" s="16">
         <v>35.130000000000102</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>47</v>
       </c>
       <c r="C55" s="13"/>
-      <c r="D55" s="4"/>
-      <c r="F55" s="5"/>
-      <c r="G55" s="4"/>
-      <c r="M55" s="5"/>
-      <c r="N55" s="4"/>
-      <c r="Q55" s="5"/>
+      <c r="D55" s="15"/>
+      <c r="E55" s="8"/>
+      <c r="F55" s="9"/>
+      <c r="G55" s="7"/>
+      <c r="H55" s="8"/>
+      <c r="I55" s="8"/>
+      <c r="J55" s="8"/>
+      <c r="K55" s="8"/>
+      <c r="L55" s="8"/>
+      <c r="M55" s="9"/>
+      <c r="N55" s="7"/>
+      <c r="O55" s="8"/>
+      <c r="P55" s="8"/>
+      <c r="Q55" s="9"/>
     </row>
     <row r="56" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="20">
+      <c r="A56" s="16">
         <v>35.1400000000001</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>48</v>
       </c>
       <c r="C56" s="13"/>
-      <c r="D56" s="4"/>
-      <c r="F56" s="5"/>
-      <c r="G56" s="4"/>
-      <c r="M56" s="5"/>
-      <c r="N56" s="4"/>
-      <c r="Q56" s="5"/>
+      <c r="D56" s="15"/>
+      <c r="E56" s="8"/>
+      <c r="F56" s="9"/>
+      <c r="G56" s="7"/>
+      <c r="H56" s="8"/>
+      <c r="I56" s="8"/>
+      <c r="J56" s="8"/>
+      <c r="K56" s="8"/>
+      <c r="L56" s="8"/>
+      <c r="M56" s="9"/>
+      <c r="N56" s="7"/>
+      <c r="O56" s="8"/>
+      <c r="P56" s="8"/>
+      <c r="Q56" s="9"/>
     </row>
     <row r="57" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="20">
+      <c r="A57" s="16">
         <v>35.150000000000098</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>49</v>
       </c>
       <c r="C57" s="13"/>
-      <c r="D57" s="4"/>
-      <c r="F57" s="5"/>
-      <c r="G57" s="4"/>
-      <c r="M57" s="5"/>
-      <c r="N57" s="4"/>
-      <c r="Q57" s="5"/>
+      <c r="D57" s="15"/>
+      <c r="E57" s="8"/>
+      <c r="F57" s="9"/>
+      <c r="G57" s="7"/>
+      <c r="H57" s="8"/>
+      <c r="I57" s="8"/>
+      <c r="J57" s="8"/>
+      <c r="K57" s="8"/>
+      <c r="L57" s="8"/>
+      <c r="M57" s="9"/>
+      <c r="N57" s="7"/>
+      <c r="O57" s="8"/>
+      <c r="P57" s="8"/>
+      <c r="Q57" s="9"/>
     </row>
     <row r="58" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="20">
+      <c r="A58" s="16">
         <v>35.160000000000103</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>50</v>
       </c>
       <c r="C58" s="13"/>
-      <c r="D58" s="4"/>
-      <c r="F58" s="5"/>
-      <c r="G58" s="4"/>
-      <c r="M58" s="5"/>
-      <c r="N58" s="4"/>
-      <c r="Q58" s="5"/>
+      <c r="D58" s="15"/>
+      <c r="E58" s="8"/>
+      <c r="F58" s="9"/>
+      <c r="G58" s="7"/>
+      <c r="H58" s="8"/>
+      <c r="I58" s="8"/>
+      <c r="J58" s="8"/>
+      <c r="K58" s="8"/>
+      <c r="L58" s="8"/>
+      <c r="M58" s="9"/>
+      <c r="N58" s="7"/>
+      <c r="O58" s="8"/>
+      <c r="P58" s="8"/>
+      <c r="Q58" s="9"/>
     </row>
     <row r="59" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="20">
+      <c r="A59" s="16">
         <v>35.170000000000101</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>51</v>
       </c>
       <c r="C59" s="13"/>
-      <c r="D59" s="4"/>
-      <c r="F59" s="5"/>
-      <c r="G59" s="4"/>
-      <c r="M59" s="5"/>
-      <c r="N59" s="4"/>
-      <c r="Q59" s="5"/>
+      <c r="D59" s="15"/>
+      <c r="E59" s="8"/>
+      <c r="F59" s="9"/>
+      <c r="G59" s="7"/>
+      <c r="H59" s="8"/>
+      <c r="I59" s="8"/>
+      <c r="J59" s="8"/>
+      <c r="K59" s="8"/>
+      <c r="L59" s="8"/>
+      <c r="M59" s="9"/>
+      <c r="N59" s="7"/>
+      <c r="O59" s="8"/>
+      <c r="P59" s="8"/>
+      <c r="Q59" s="9"/>
     </row>
     <row r="60" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C60" s="13"/>
-      <c r="D60" s="4"/>
-      <c r="F60" s="5"/>
-      <c r="G60" s="4"/>
-      <c r="M60" s="5"/>
-      <c r="N60" s="4"/>
-      <c r="Q60" s="5"/>
+      <c r="D60" s="15"/>
+      <c r="E60" s="8"/>
+      <c r="F60" s="9"/>
+      <c r="G60" s="7"/>
+      <c r="H60" s="8"/>
+      <c r="I60" s="8"/>
+      <c r="J60" s="8"/>
+      <c r="K60" s="8"/>
+      <c r="L60" s="8"/>
+      <c r="M60" s="9"/>
+      <c r="N60" s="7"/>
+      <c r="O60" s="8"/>
+      <c r="P60" s="8"/>
+      <c r="Q60" s="9"/>
     </row>
     <row r="61" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C61" s="14"/>
-      <c r="D61" s="4"/>
-      <c r="F61" s="5"/>
-      <c r="G61" s="4"/>
-      <c r="M61" s="5"/>
-      <c r="N61" s="4"/>
-      <c r="Q61" s="5"/>
+      <c r="C61" s="13"/>
+      <c r="D61" s="15"/>
+      <c r="E61" s="8"/>
+      <c r="F61" s="9"/>
+      <c r="G61" s="7"/>
+      <c r="H61" s="8"/>
+      <c r="I61" s="8"/>
+      <c r="J61" s="8"/>
+      <c r="K61" s="8"/>
+      <c r="L61" s="8"/>
+      <c r="M61" s="9"/>
+      <c r="N61" s="7"/>
+      <c r="O61" s="8"/>
+      <c r="P61" s="8"/>
+      <c r="Q61" s="9"/>
     </row>
     <row r="62" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C62" s="13"/>
-      <c r="D62" s="4"/>
-      <c r="F62" s="5"/>
-      <c r="G62" s="4"/>
-      <c r="M62" s="5"/>
-      <c r="N62" s="4"/>
-      <c r="Q62" s="5"/>
+      <c r="D62" s="15"/>
+      <c r="E62" s="8"/>
+      <c r="F62" s="9"/>
+      <c r="G62" s="7"/>
+      <c r="H62" s="8"/>
+      <c r="I62" s="8"/>
+      <c r="J62" s="8"/>
+      <c r="K62" s="8"/>
+      <c r="L62" s="8"/>
+      <c r="M62" s="9"/>
+      <c r="N62" s="7"/>
+      <c r="O62" s="8"/>
+      <c r="P62" s="8"/>
+      <c r="Q62" s="9"/>
     </row>
     <row r="63" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="21">
+      <c r="A63" s="17">
         <v>1</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C63" s="13"/>
-      <c r="D63" s="4"/>
-      <c r="F63" s="5"/>
-      <c r="G63" s="4"/>
-      <c r="M63" s="5"/>
-      <c r="N63" s="4"/>
-      <c r="Q63" s="5"/>
+      <c r="D63" s="15"/>
+      <c r="E63" s="8"/>
+      <c r="F63" s="9"/>
+      <c r="G63" s="7"/>
+      <c r="H63" s="8"/>
+      <c r="I63" s="8"/>
+      <c r="J63" s="8"/>
+      <c r="K63" s="8"/>
+      <c r="L63" s="8"/>
+      <c r="M63" s="9"/>
+      <c r="N63" s="7"/>
+      <c r="O63" s="8"/>
+      <c r="P63" s="8"/>
+      <c r="Q63" s="9"/>
     </row>
     <row r="64" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="21">
+      <c r="A64" s="17">
         <v>2</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C64" s="13"/>
-      <c r="D64" s="4"/>
-      <c r="F64" s="5"/>
-      <c r="G64" s="4"/>
-      <c r="M64" s="5"/>
-      <c r="N64" s="4"/>
-      <c r="Q64" s="5"/>
+      <c r="D64" s="15"/>
+      <c r="E64" s="8"/>
+      <c r="F64" s="9"/>
+      <c r="G64" s="7"/>
+      <c r="H64" s="8"/>
+      <c r="I64" s="8"/>
+      <c r="J64" s="8"/>
+      <c r="K64" s="8"/>
+      <c r="L64" s="8"/>
+      <c r="M64" s="9"/>
+      <c r="N64" s="7"/>
+      <c r="O64" s="8"/>
+      <c r="P64" s="8"/>
+      <c r="Q64" s="9"/>
     </row>
     <row r="65" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="21">
+      <c r="A65" s="17">
         <v>3</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C65" s="13"/>
-      <c r="D65" s="4"/>
-      <c r="F65" s="5"/>
-      <c r="G65" s="4"/>
-      <c r="M65" s="5"/>
-      <c r="N65" s="4"/>
-      <c r="Q65" s="5"/>
+      <c r="D65" s="15"/>
+      <c r="E65" s="8"/>
+      <c r="F65" s="9"/>
+      <c r="G65" s="7"/>
+      <c r="H65" s="8"/>
+      <c r="I65" s="8"/>
+      <c r="J65" s="8"/>
+      <c r="K65" s="8"/>
+      <c r="L65" s="8"/>
+      <c r="M65" s="9"/>
+      <c r="N65" s="7"/>
+      <c r="O65" s="8"/>
+      <c r="P65" s="8"/>
+      <c r="Q65" s="9"/>
     </row>
     <row r="66" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="21">
+      <c r="A66" s="17">
         <v>4</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>57</v>
       </c>
       <c r="C66" s="13"/>
-      <c r="D66" s="4"/>
-      <c r="F66" s="5"/>
-      <c r="G66" s="4"/>
-      <c r="M66" s="5"/>
-      <c r="N66" s="4"/>
-      <c r="Q66" s="5"/>
+      <c r="D66" s="15"/>
+      <c r="E66" s="8"/>
+      <c r="F66" s="9"/>
+      <c r="G66" s="7"/>
+      <c r="H66" s="8"/>
+      <c r="I66" s="8"/>
+      <c r="J66" s="8"/>
+      <c r="K66" s="8"/>
+      <c r="L66" s="8"/>
+      <c r="M66" s="9"/>
+      <c r="N66" s="7"/>
+      <c r="O66" s="8"/>
+      <c r="P66" s="8"/>
+      <c r="Q66" s="9"/>
     </row>
     <row r="67" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="21">
+      <c r="A67" s="17">
         <v>5</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C67" s="13"/>
-      <c r="D67" s="4"/>
-      <c r="F67" s="5"/>
-      <c r="G67" s="4"/>
-      <c r="M67" s="5"/>
-      <c r="N67" s="4"/>
-      <c r="Q67" s="5"/>
+      <c r="D67" s="15"/>
+      <c r="E67" s="8"/>
+      <c r="F67" s="9"/>
+      <c r="G67" s="7"/>
+      <c r="H67" s="8"/>
+      <c r="I67" s="8"/>
+      <c r="J67" s="8"/>
+      <c r="K67" s="8"/>
+      <c r="L67" s="8"/>
+      <c r="M67" s="9"/>
+      <c r="N67" s="7"/>
+      <c r="O67" s="8"/>
+      <c r="P67" s="8"/>
+      <c r="Q67" s="9"/>
     </row>
     <row r="68" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="21">
+      <c r="A68" s="17">
         <v>6</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>58</v>
       </c>
       <c r="C68" s="13"/>
-      <c r="D68" s="4"/>
-      <c r="F68" s="5"/>
-      <c r="G68" s="4"/>
-      <c r="M68" s="5"/>
-      <c r="N68" s="4"/>
-      <c r="Q68" s="5"/>
+      <c r="D68" s="15"/>
+      <c r="E68" s="8"/>
+      <c r="F68" s="9"/>
+      <c r="G68" s="7"/>
+      <c r="H68" s="8"/>
+      <c r="I68" s="8"/>
+      <c r="J68" s="8"/>
+      <c r="K68" s="8"/>
+      <c r="L68" s="8"/>
+      <c r="M68" s="9"/>
+      <c r="N68" s="7"/>
+      <c r="O68" s="8"/>
+      <c r="P68" s="8"/>
+      <c r="Q68" s="9"/>
     </row>
     <row r="69" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C69" s="13"/>
-      <c r="D69" s="4"/>
-      <c r="F69" s="5"/>
-      <c r="G69" s="4"/>
-      <c r="M69" s="5"/>
-      <c r="N69" s="4"/>
-      <c r="Q69" s="5"/>
+      <c r="D69" s="15"/>
+      <c r="E69" s="8"/>
+      <c r="F69" s="9"/>
+      <c r="G69" s="7"/>
+      <c r="H69" s="8"/>
+      <c r="I69" s="8"/>
+      <c r="J69" s="8"/>
+      <c r="K69" s="8"/>
+      <c r="L69" s="8"/>
+      <c r="M69" s="9"/>
+      <c r="N69" s="7"/>
+      <c r="O69" s="8"/>
+      <c r="P69" s="8"/>
+      <c r="Q69" s="9"/>
     </row>
     <row r="70" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C70" s="14"/>
-      <c r="D70" s="4"/>
-      <c r="F70" s="5"/>
-      <c r="G70" s="4"/>
-      <c r="M70" s="5"/>
-      <c r="N70" s="4"/>
-      <c r="Q70" s="5"/>
+      <c r="C70" s="13"/>
+      <c r="D70" s="15"/>
+      <c r="E70" s="8"/>
+      <c r="F70" s="9"/>
+      <c r="G70" s="7"/>
+      <c r="H70" s="8"/>
+      <c r="I70" s="8"/>
+      <c r="J70" s="8"/>
+      <c r="K70" s="8"/>
+      <c r="L70" s="8"/>
+      <c r="M70" s="9"/>
+      <c r="N70" s="7"/>
+      <c r="O70" s="8"/>
+      <c r="P70" s="8"/>
+      <c r="Q70" s="9"/>
     </row>
     <row r="71" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C71" s="13"/>
-      <c r="D71" s="4"/>
-      <c r="F71" s="5"/>
-      <c r="G71" s="4"/>
-      <c r="M71" s="5"/>
-      <c r="N71" s="4"/>
-      <c r="Q71" s="5"/>
+      <c r="D71" s="15"/>
+      <c r="E71" s="8"/>
+      <c r="F71" s="9"/>
+      <c r="G71" s="7"/>
+      <c r="H71" s="8"/>
+      <c r="I71" s="8"/>
+      <c r="J71" s="8"/>
+      <c r="K71" s="8"/>
+      <c r="L71" s="8"/>
+      <c r="M71" s="9"/>
+      <c r="N71" s="7"/>
+      <c r="O71" s="8"/>
+      <c r="P71" s="8"/>
+      <c r="Q71" s="9"/>
     </row>
     <row r="72" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="20">
+      <c r="A72" s="16">
         <v>39.01</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>70</v>
       </c>
       <c r="C72" s="13"/>
-      <c r="D72" s="4"/>
-      <c r="F72" s="5"/>
-      <c r="G72" s="4"/>
-      <c r="M72" s="5"/>
-      <c r="N72" s="4"/>
-      <c r="Q72" s="5"/>
+      <c r="D72" s="15"/>
+      <c r="E72" s="8"/>
+      <c r="F72" s="9"/>
+      <c r="G72" s="7"/>
+      <c r="H72" s="8"/>
+      <c r="I72" s="8"/>
+      <c r="J72" s="8"/>
+      <c r="K72" s="8"/>
+      <c r="L72" s="8"/>
+      <c r="M72" s="9"/>
+      <c r="N72" s="7"/>
+      <c r="O72" s="8"/>
+      <c r="P72" s="8"/>
+      <c r="Q72" s="9"/>
     </row>
     <row r="73" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="20">
+      <c r="A73" s="16">
         <v>39.020000000000003</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>69</v>
       </c>
       <c r="C73" s="13"/>
-      <c r="D73" s="4"/>
-      <c r="F73" s="5"/>
-      <c r="G73" s="4"/>
-      <c r="M73" s="5"/>
-      <c r="N73" s="4"/>
-      <c r="Q73" s="5"/>
+      <c r="D73" s="15"/>
+      <c r="E73" s="8"/>
+      <c r="F73" s="9"/>
+      <c r="G73" s="7"/>
+      <c r="H73" s="8"/>
+      <c r="I73" s="8"/>
+      <c r="J73" s="8"/>
+      <c r="K73" s="8"/>
+      <c r="L73" s="8"/>
+      <c r="M73" s="9"/>
+      <c r="N73" s="7"/>
+      <c r="O73" s="8"/>
+      <c r="P73" s="8"/>
+      <c r="Q73" s="9"/>
     </row>
     <row r="74" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="20">
+      <c r="A74" s="16">
         <v>39.03</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>68</v>
       </c>
       <c r="C74" s="13"/>
-      <c r="D74" s="4"/>
-      <c r="F74" s="5"/>
-      <c r="G74" s="4"/>
-      <c r="M74" s="5"/>
-      <c r="N74" s="4"/>
-      <c r="Q74" s="5"/>
+      <c r="D74" s="15"/>
+      <c r="E74" s="8"/>
+      <c r="F74" s="9"/>
+      <c r="G74" s="7"/>
+      <c r="H74" s="8"/>
+      <c r="I74" s="8"/>
+      <c r="J74" s="8"/>
+      <c r="K74" s="8"/>
+      <c r="L74" s="8"/>
+      <c r="M74" s="9"/>
+      <c r="N74" s="7"/>
+      <c r="O74" s="8"/>
+      <c r="P74" s="8"/>
+      <c r="Q74" s="9"/>
     </row>
     <row r="75" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="20">
+      <c r="A75" s="16">
         <v>39.04</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>67</v>
       </c>
       <c r="C75" s="13"/>
-      <c r="D75" s="4"/>
-      <c r="F75" s="5"/>
-      <c r="G75" s="4"/>
-      <c r="M75" s="5"/>
-      <c r="N75" s="4"/>
-      <c r="Q75" s="5"/>
+      <c r="D75" s="15"/>
+      <c r="E75" s="8"/>
+      <c r="F75" s="9"/>
+      <c r="G75" s="7"/>
+      <c r="H75" s="8"/>
+      <c r="I75" s="8"/>
+      <c r="J75" s="8"/>
+      <c r="K75" s="8"/>
+      <c r="L75" s="8"/>
+      <c r="M75" s="9"/>
+      <c r="N75" s="7"/>
+      <c r="O75" s="8"/>
+      <c r="P75" s="8"/>
+      <c r="Q75" s="9"/>
     </row>
     <row r="76" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="20">
+      <c r="A76" s="16">
         <v>39.049999999999997</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>66</v>
       </c>
       <c r="C76" s="13"/>
-      <c r="D76" s="4"/>
-      <c r="F76" s="5"/>
-      <c r="G76" s="4"/>
-      <c r="M76" s="5"/>
-      <c r="N76" s="4"/>
-      <c r="Q76" s="5"/>
+      <c r="D76" s="15"/>
+      <c r="E76" s="8"/>
+      <c r="F76" s="9"/>
+      <c r="G76" s="7"/>
+      <c r="H76" s="8"/>
+      <c r="I76" s="8"/>
+      <c r="J76" s="8"/>
+      <c r="K76" s="8"/>
+      <c r="L76" s="8"/>
+      <c r="M76" s="9"/>
+      <c r="N76" s="7"/>
+      <c r="O76" s="8"/>
+      <c r="P76" s="8"/>
+      <c r="Q76" s="9"/>
     </row>
     <row r="77" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="20">
+      <c r="A77" s="16">
         <v>39.06</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C77" s="13"/>
-      <c r="D77" s="4"/>
-      <c r="F77" s="5"/>
-      <c r="G77" s="4"/>
-      <c r="M77" s="5"/>
-      <c r="N77" s="4"/>
-      <c r="Q77" s="5"/>
+      <c r="D77" s="15"/>
+      <c r="E77" s="8"/>
+      <c r="F77" s="9"/>
+      <c r="G77" s="7"/>
+      <c r="H77" s="8"/>
+      <c r="I77" s="8"/>
+      <c r="J77" s="8"/>
+      <c r="K77" s="8"/>
+      <c r="L77" s="8"/>
+      <c r="M77" s="9"/>
+      <c r="N77" s="7"/>
+      <c r="O77" s="8"/>
+      <c r="P77" s="8"/>
+      <c r="Q77" s="9"/>
     </row>
     <row r="78" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="20">
+      <c r="A78" s="16">
         <v>39.07</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>64</v>
       </c>
       <c r="C78" s="13"/>
-      <c r="D78" s="4"/>
-      <c r="F78" s="5"/>
-      <c r="G78" s="4"/>
-      <c r="M78" s="5"/>
-      <c r="N78" s="4"/>
-      <c r="Q78" s="5"/>
+      <c r="D78" s="15"/>
+      <c r="E78" s="8"/>
+      <c r="F78" s="9"/>
+      <c r="G78" s="7"/>
+      <c r="H78" s="8"/>
+      <c r="I78" s="8"/>
+      <c r="J78" s="8"/>
+      <c r="K78" s="8"/>
+      <c r="L78" s="8"/>
+      <c r="M78" s="9"/>
+      <c r="N78" s="7"/>
+      <c r="O78" s="8"/>
+      <c r="P78" s="8"/>
+      <c r="Q78" s="9"/>
     </row>
     <row r="79" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="20">
+      <c r="A79" s="16">
         <v>39.08</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>63</v>
       </c>
       <c r="C79" s="13"/>
-      <c r="D79" s="4"/>
-      <c r="F79" s="5"/>
-      <c r="G79" s="4"/>
-      <c r="M79" s="5"/>
-      <c r="N79" s="4"/>
-      <c r="Q79" s="5"/>
+      <c r="D79" s="15"/>
+      <c r="E79" s="8"/>
+      <c r="F79" s="9"/>
+      <c r="G79" s="7"/>
+      <c r="H79" s="8"/>
+      <c r="I79" s="8"/>
+      <c r="J79" s="8"/>
+      <c r="K79" s="8"/>
+      <c r="L79" s="8"/>
+      <c r="M79" s="9"/>
+      <c r="N79" s="7"/>
+      <c r="O79" s="8"/>
+      <c r="P79" s="8"/>
+      <c r="Q79" s="9"/>
     </row>
     <row r="80" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="20">
+      <c r="A80" s="16">
         <v>39.090000000000003</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>62</v>
       </c>
       <c r="C80" s="13"/>
-      <c r="D80" s="4"/>
-      <c r="F80" s="5"/>
-      <c r="G80" s="4"/>
-      <c r="M80" s="5"/>
-      <c r="N80" s="4"/>
-      <c r="Q80" s="5"/>
+      <c r="D80" s="15"/>
+      <c r="E80" s="8"/>
+      <c r="F80" s="9"/>
+      <c r="G80" s="7"/>
+      <c r="H80" s="8"/>
+      <c r="I80" s="8"/>
+      <c r="J80" s="8"/>
+      <c r="K80" s="8"/>
+      <c r="L80" s="8"/>
+      <c r="M80" s="9"/>
+      <c r="N80" s="7"/>
+      <c r="O80" s="8"/>
+      <c r="P80" s="8"/>
+      <c r="Q80" s="9"/>
     </row>
     <row r="81" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="20">
+      <c r="A81" s="16">
         <v>39.1</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C81" s="13"/>
-      <c r="D81" s="4"/>
-      <c r="F81" s="5"/>
-      <c r="G81" s="4"/>
-      <c r="M81" s="5"/>
-      <c r="N81" s="4"/>
-      <c r="Q81" s="5"/>
+      <c r="D81" s="15"/>
+      <c r="E81" s="8"/>
+      <c r="F81" s="9"/>
+      <c r="G81" s="7"/>
+      <c r="H81" s="8"/>
+      <c r="I81" s="8"/>
+      <c r="J81" s="8"/>
+      <c r="K81" s="8"/>
+      <c r="L81" s="8"/>
+      <c r="M81" s="9"/>
+      <c r="N81" s="7"/>
+      <c r="O81" s="8"/>
+      <c r="P81" s="8"/>
+      <c r="Q81" s="9"/>
     </row>
     <row r="82" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="20">
+      <c r="A82" s="16">
         <v>39.11</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>60</v>
       </c>
       <c r="C82" s="13"/>
-      <c r="D82" s="4"/>
-      <c r="F82" s="5"/>
-      <c r="G82" s="4"/>
-      <c r="M82" s="5"/>
-      <c r="N82" s="4"/>
-      <c r="Q82" s="5"/>
+      <c r="D82" s="15"/>
+      <c r="E82" s="8"/>
+      <c r="F82" s="9"/>
+      <c r="G82" s="7"/>
+      <c r="H82" s="8"/>
+      <c r="I82" s="8"/>
+      <c r="J82" s="8"/>
+      <c r="K82" s="8"/>
+      <c r="L82" s="8"/>
+      <c r="M82" s="9"/>
+      <c r="N82" s="7"/>
+      <c r="O82" s="8"/>
+      <c r="P82" s="8"/>
+      <c r="Q82" s="9"/>
     </row>
     <row r="83" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C83" s="13"/>
-      <c r="D83" s="4"/>
-      <c r="F83" s="5"/>
-      <c r="G83" s="4"/>
-      <c r="M83" s="5"/>
-      <c r="N83" s="4"/>
-      <c r="Q83" s="5"/>
+      <c r="D83" s="15"/>
+      <c r="E83" s="8"/>
+      <c r="F83" s="9"/>
+      <c r="G83" s="7"/>
+      <c r="H83" s="8"/>
+      <c r="I83" s="8"/>
+      <c r="J83" s="8"/>
+      <c r="K83" s="8"/>
+      <c r="L83" s="8"/>
+      <c r="M83" s="9"/>
+      <c r="N83" s="7"/>
+      <c r="O83" s="8"/>
+      <c r="P83" s="8"/>
+      <c r="Q83" s="9"/>
     </row>
     <row r="84" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B84" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C84" s="14"/>
-      <c r="D84" s="4"/>
-      <c r="F84" s="5"/>
-      <c r="G84" s="4"/>
-      <c r="M84" s="5"/>
-      <c r="N84" s="4"/>
-      <c r="Q84" s="5"/>
+      <c r="C84" s="13"/>
+      <c r="D84" s="15"/>
+      <c r="E84" s="8"/>
+      <c r="F84" s="9"/>
+      <c r="G84" s="7"/>
+      <c r="H84" s="8"/>
+      <c r="I84" s="8"/>
+      <c r="J84" s="8"/>
+      <c r="K84" s="8"/>
+      <c r="L84" s="8"/>
+      <c r="M84" s="9"/>
+      <c r="N84" s="7"/>
+      <c r="O84" s="8"/>
+      <c r="P84" s="8"/>
+      <c r="Q84" s="9"/>
     </row>
     <row r="85" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="22"/>
+      <c r="A85" s="18"/>
       <c r="C85" s="13"/>
-      <c r="D85" s="4"/>
-      <c r="F85" s="5"/>
-      <c r="G85" s="4"/>
-      <c r="M85" s="5"/>
-      <c r="N85" s="4"/>
-      <c r="Q85" s="5"/>
+      <c r="D85" s="15"/>
+      <c r="E85" s="8"/>
+      <c r="F85" s="9"/>
+      <c r="G85" s="7"/>
+      <c r="H85" s="8"/>
+      <c r="I85" s="8"/>
+      <c r="J85" s="8"/>
+      <c r="K85" s="8"/>
+      <c r="L85" s="8"/>
+      <c r="M85" s="9"/>
+      <c r="N85" s="7"/>
+      <c r="O85" s="8"/>
+      <c r="P85" s="8"/>
+      <c r="Q85" s="9"/>
     </row>
     <row r="86" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="22"/>
+      <c r="A86" s="18"/>
       <c r="B86" s="3" t="s">
         <v>73</v>
       </c>
       <c r="C86" s="13"/>
-      <c r="D86" s="4"/>
-      <c r="F86" s="5"/>
-      <c r="G86" s="4"/>
-      <c r="M86" s="5"/>
-      <c r="N86" s="4"/>
-      <c r="Q86" s="5"/>
+      <c r="D86" s="15"/>
+      <c r="E86" s="8"/>
+      <c r="F86" s="9"/>
+      <c r="G86" s="7"/>
+      <c r="H86" s="8"/>
+      <c r="I86" s="8"/>
+      <c r="J86" s="8"/>
+      <c r="K86" s="8"/>
+      <c r="L86" s="8"/>
+      <c r="M86" s="9"/>
+      <c r="N86" s="7"/>
+      <c r="O86" s="8"/>
+      <c r="P86" s="8"/>
+      <c r="Q86" s="9"/>
     </row>
     <row r="87" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="20">
+      <c r="A87" s="16">
         <v>41.01</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>72</v>
       </c>
       <c r="C87" s="13"/>
-      <c r="D87" s="4"/>
-      <c r="F87" s="5"/>
-      <c r="G87" s="4"/>
-      <c r="M87" s="5"/>
-      <c r="N87" s="4"/>
-      <c r="Q87" s="5"/>
+      <c r="D87" s="15"/>
+      <c r="E87" s="8"/>
+      <c r="F87" s="9"/>
+      <c r="G87" s="7"/>
+      <c r="H87" s="8"/>
+      <c r="I87" s="8"/>
+      <c r="J87" s="8"/>
+      <c r="K87" s="8"/>
+      <c r="L87" s="8"/>
+      <c r="M87" s="9"/>
+      <c r="N87" s="7"/>
+      <c r="O87" s="8"/>
+      <c r="P87" s="8"/>
+      <c r="Q87" s="9"/>
     </row>
     <row r="88" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="20">
+      <c r="A88" s="16">
         <v>41.02</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>78</v>
       </c>
       <c r="C88" s="13"/>
-      <c r="D88" s="4"/>
-      <c r="F88" s="5"/>
-      <c r="G88" s="4"/>
-      <c r="M88" s="5"/>
-      <c r="N88" s="4"/>
-      <c r="Q88" s="5"/>
+      <c r="D88" s="15"/>
+      <c r="E88" s="8"/>
+      <c r="F88" s="9"/>
+      <c r="G88" s="7"/>
+      <c r="H88" s="8"/>
+      <c r="I88" s="8"/>
+      <c r="J88" s="8"/>
+      <c r="K88" s="8"/>
+      <c r="L88" s="8"/>
+      <c r="M88" s="9"/>
+      <c r="N88" s="7"/>
+      <c r="O88" s="8"/>
+      <c r="P88" s="8"/>
+      <c r="Q88" s="9"/>
     </row>
     <row r="89" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="20">
+      <c r="A89" s="16">
         <v>41.03</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>77</v>
       </c>
       <c r="C89" s="13"/>
-      <c r="D89" s="4"/>
-      <c r="F89" s="5"/>
-      <c r="G89" s="4"/>
-      <c r="M89" s="5"/>
-      <c r="N89" s="4"/>
-      <c r="Q89" s="5"/>
+      <c r="D89" s="15"/>
+      <c r="E89" s="8"/>
+      <c r="F89" s="9"/>
+      <c r="G89" s="7"/>
+      <c r="H89" s="8"/>
+      <c r="I89" s="8"/>
+      <c r="J89" s="8"/>
+      <c r="K89" s="8"/>
+      <c r="L89" s="8"/>
+      <c r="M89" s="9"/>
+      <c r="N89" s="7"/>
+      <c r="O89" s="8"/>
+      <c r="P89" s="8"/>
+      <c r="Q89" s="9"/>
     </row>
     <row r="90" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="20">
+      <c r="A90" s="16">
         <v>41.04</v>
       </c>
       <c r="B90" s="3" t="s">
         <v>76</v>
       </c>
       <c r="C90" s="13"/>
-      <c r="D90" s="4"/>
-      <c r="F90" s="5"/>
-      <c r="G90" s="4"/>
-      <c r="M90" s="5"/>
-      <c r="N90" s="4"/>
-      <c r="Q90" s="5"/>
+      <c r="D90" s="15"/>
+      <c r="E90" s="8"/>
+      <c r="F90" s="9"/>
+      <c r="G90" s="7"/>
+      <c r="H90" s="8"/>
+      <c r="I90" s="8"/>
+      <c r="J90" s="8"/>
+      <c r="K90" s="8"/>
+      <c r="L90" s="8"/>
+      <c r="M90" s="9"/>
+      <c r="N90" s="7"/>
+      <c r="O90" s="8"/>
+      <c r="P90" s="8"/>
+      <c r="Q90" s="9"/>
     </row>
     <row r="91" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="20">
+      <c r="A91" s="16">
         <v>41.05</v>
       </c>
       <c r="B91" s="3" t="s">
         <v>75</v>
       </c>
       <c r="C91" s="13"/>
-      <c r="D91" s="4"/>
-      <c r="F91" s="5"/>
-      <c r="G91" s="4"/>
-      <c r="M91" s="5"/>
-      <c r="N91" s="4"/>
-      <c r="Q91" s="5"/>
+      <c r="D91" s="15"/>
+      <c r="E91" s="8"/>
+      <c r="F91" s="9"/>
+      <c r="G91" s="7"/>
+      <c r="H91" s="8"/>
+      <c r="I91" s="8"/>
+      <c r="J91" s="8"/>
+      <c r="K91" s="8"/>
+      <c r="L91" s="8"/>
+      <c r="M91" s="9"/>
+      <c r="N91" s="7"/>
+      <c r="O91" s="8"/>
+      <c r="P91" s="8"/>
+      <c r="Q91" s="9"/>
     </row>
     <row r="92" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="20">
+      <c r="A92" s="16">
         <v>41.06</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>74</v>
       </c>
       <c r="C92" s="13"/>
-      <c r="D92" s="4"/>
-      <c r="F92" s="5"/>
-      <c r="G92" s="4"/>
-      <c r="M92" s="5"/>
-      <c r="N92" s="4"/>
-      <c r="Q92" s="5"/>
+      <c r="D92" s="15"/>
+      <c r="E92" s="8"/>
+      <c r="F92" s="9"/>
+      <c r="G92" s="7"/>
+      <c r="H92" s="8"/>
+      <c r="I92" s="8"/>
+      <c r="J92" s="8"/>
+      <c r="K92" s="8"/>
+      <c r="L92" s="8"/>
+      <c r="M92" s="9"/>
+      <c r="N92" s="7"/>
+      <c r="O92" s="8"/>
+      <c r="P92" s="8"/>
+      <c r="Q92" s="9"/>
     </row>
     <row r="93" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C93" s="13"/>
-      <c r="D93" s="4"/>
-      <c r="F93" s="5"/>
-      <c r="G93" s="4"/>
-      <c r="M93" s="5"/>
-      <c r="N93" s="4"/>
-      <c r="Q93" s="5"/>
+      <c r="D93" s="15"/>
+      <c r="E93" s="8"/>
+      <c r="F93" s="9"/>
+      <c r="G93" s="7"/>
+      <c r="H93" s="8"/>
+      <c r="I93" s="8"/>
+      <c r="J93" s="8"/>
+      <c r="K93" s="8"/>
+      <c r="L93" s="8"/>
+      <c r="M93" s="9"/>
+      <c r="N93" s="7"/>
+      <c r="O93" s="8"/>
+      <c r="P93" s="8"/>
+      <c r="Q93" s="9"/>
     </row>
     <row r="94" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B94" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C94" s="14"/>
-      <c r="D94" s="4"/>
-      <c r="F94" s="5"/>
-      <c r="G94" s="4"/>
-      <c r="M94" s="5"/>
-      <c r="N94" s="4"/>
-      <c r="Q94" s="5"/>
+      <c r="C94" s="13"/>
+      <c r="D94" s="15"/>
+      <c r="E94" s="8"/>
+      <c r="F94" s="9"/>
+      <c r="G94" s="7"/>
+      <c r="H94" s="8"/>
+      <c r="I94" s="8"/>
+      <c r="J94" s="8"/>
+      <c r="K94" s="8"/>
+      <c r="L94" s="8"/>
+      <c r="M94" s="9"/>
+      <c r="N94" s="7"/>
+      <c r="O94" s="8"/>
+      <c r="P94" s="8"/>
+      <c r="Q94" s="9"/>
     </row>
     <row r="95" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C95" s="13"/>
-      <c r="D95" s="4"/>
-      <c r="F95" s="5"/>
-      <c r="G95" s="4"/>
-      <c r="M95" s="5"/>
-      <c r="N95" s="4"/>
-      <c r="Q95" s="5"/>
+      <c r="D95" s="15"/>
+      <c r="E95" s="8"/>
+      <c r="F95" s="9"/>
+      <c r="G95" s="7"/>
+      <c r="H95" s="8"/>
+      <c r="I95" s="8"/>
+      <c r="J95" s="8"/>
+      <c r="K95" s="8"/>
+      <c r="L95" s="8"/>
+      <c r="M95" s="9"/>
+      <c r="N95" s="7"/>
+      <c r="O95" s="8"/>
+      <c r="P95" s="8"/>
+      <c r="Q95" s="9"/>
     </row>
     <row r="96" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="20">
+      <c r="A96" s="16">
         <v>36.01</v>
       </c>
       <c r="B96" s="3" t="s">
         <v>80</v>
       </c>
       <c r="C96" s="13"/>
-      <c r="D96" s="4"/>
-      <c r="F96" s="5"/>
-      <c r="G96" s="4"/>
-      <c r="M96" s="5"/>
-      <c r="N96" s="4"/>
-      <c r="Q96" s="5"/>
+      <c r="D96" s="15"/>
+      <c r="E96" s="8"/>
+      <c r="F96" s="9"/>
+      <c r="G96" s="7"/>
+      <c r="H96" s="8"/>
+      <c r="I96" s="8"/>
+      <c r="J96" s="8"/>
+      <c r="K96" s="8"/>
+      <c r="L96" s="8"/>
+      <c r="M96" s="9"/>
+      <c r="N96" s="7"/>
+      <c r="O96" s="8"/>
+      <c r="P96" s="8"/>
+      <c r="Q96" s="9"/>
     </row>
     <row r="97" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="20">
+      <c r="A97" s="16">
         <v>36.020000000000003</v>
       </c>
       <c r="B97" s="3" t="s">
         <v>81</v>
       </c>
       <c r="C97" s="13"/>
-      <c r="D97" s="4"/>
-      <c r="F97" s="5"/>
-      <c r="G97" s="4"/>
-      <c r="M97" s="5"/>
-      <c r="N97" s="4"/>
-      <c r="Q97" s="5"/>
+      <c r="D97" s="15"/>
+      <c r="E97" s="8"/>
+      <c r="F97" s="9"/>
+      <c r="G97" s="7"/>
+      <c r="H97" s="8"/>
+      <c r="I97" s="8"/>
+      <c r="J97" s="8"/>
+      <c r="K97" s="8"/>
+      <c r="L97" s="8"/>
+      <c r="M97" s="9"/>
+      <c r="N97" s="7"/>
+      <c r="O97" s="8"/>
+      <c r="P97" s="8"/>
+      <c r="Q97" s="9"/>
     </row>
     <row r="98" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="20">
+      <c r="A98" s="16">
         <v>36.03</v>
       </c>
       <c r="B98" s="3" t="s">
         <v>82</v>
       </c>
       <c r="C98" s="13"/>
-      <c r="D98" s="4"/>
-      <c r="F98" s="5"/>
-      <c r="G98" s="4"/>
-      <c r="M98" s="5"/>
-      <c r="N98" s="4"/>
-      <c r="Q98" s="5"/>
+      <c r="D98" s="15"/>
+      <c r="E98" s="8"/>
+      <c r="F98" s="9"/>
+      <c r="G98" s="7"/>
+      <c r="H98" s="8"/>
+      <c r="I98" s="8"/>
+      <c r="J98" s="8"/>
+      <c r="K98" s="8"/>
+      <c r="L98" s="8"/>
+      <c r="M98" s="9"/>
+      <c r="N98" s="7"/>
+      <c r="O98" s="8"/>
+      <c r="P98" s="8"/>
+      <c r="Q98" s="9"/>
     </row>
     <row r="99" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="20">
+      <c r="A99" s="16">
         <v>36.04</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C99" s="13"/>
-      <c r="D99" s="4"/>
-      <c r="F99" s="5"/>
-      <c r="G99" s="4"/>
-      <c r="M99" s="5"/>
-      <c r="N99" s="4"/>
-      <c r="Q99" s="5"/>
+      <c r="D99" s="15"/>
+      <c r="E99" s="8"/>
+      <c r="F99" s="9"/>
+      <c r="G99" s="7"/>
+      <c r="H99" s="8"/>
+      <c r="I99" s="8"/>
+      <c r="J99" s="8"/>
+      <c r="K99" s="8"/>
+      <c r="L99" s="8"/>
+      <c r="M99" s="9"/>
+      <c r="N99" s="7"/>
+      <c r="O99" s="8"/>
+      <c r="P99" s="8"/>
+      <c r="Q99" s="9"/>
     </row>
     <row r="100" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="20">
+      <c r="A100" s="16">
         <v>36.049999999999997</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>84</v>
       </c>
       <c r="C100" s="13"/>
-      <c r="D100" s="4"/>
-      <c r="F100" s="5"/>
-      <c r="G100" s="4"/>
-      <c r="M100" s="5"/>
-      <c r="N100" s="4"/>
-      <c r="Q100" s="5"/>
+      <c r="D100" s="15"/>
+      <c r="E100" s="8"/>
+      <c r="F100" s="9"/>
+      <c r="G100" s="7"/>
+      <c r="H100" s="8"/>
+      <c r="I100" s="8"/>
+      <c r="J100" s="8"/>
+      <c r="K100" s="8"/>
+      <c r="L100" s="8"/>
+      <c r="M100" s="9"/>
+      <c r="N100" s="7"/>
+      <c r="O100" s="8"/>
+      <c r="P100" s="8"/>
+      <c r="Q100" s="9"/>
     </row>
     <row r="101" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="20">
+      <c r="A101" s="16">
         <v>36.06</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>85</v>
       </c>
       <c r="C101" s="13"/>
-      <c r="D101" s="4"/>
-      <c r="F101" s="5"/>
-      <c r="G101" s="4"/>
-      <c r="M101" s="5"/>
-      <c r="N101" s="4"/>
-      <c r="Q101" s="5"/>
+      <c r="D101" s="15"/>
+      <c r="E101" s="8"/>
+      <c r="F101" s="9"/>
+      <c r="G101" s="7"/>
+      <c r="H101" s="8"/>
+      <c r="I101" s="8"/>
+      <c r="J101" s="8"/>
+      <c r="K101" s="8"/>
+      <c r="L101" s="8"/>
+      <c r="M101" s="9"/>
+      <c r="N101" s="7"/>
+      <c r="O101" s="8"/>
+      <c r="P101" s="8"/>
+      <c r="Q101" s="9"/>
     </row>
     <row r="102" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="20">
+      <c r="A102" s="16">
         <v>36.07</v>
       </c>
       <c r="B102" s="3" t="s">
         <v>86</v>
       </c>
       <c r="C102" s="13"/>
-      <c r="D102" s="4"/>
-      <c r="F102" s="5"/>
-      <c r="G102" s="4"/>
-      <c r="M102" s="5"/>
-      <c r="N102" s="4"/>
-      <c r="Q102" s="5"/>
+      <c r="D102" s="15"/>
+      <c r="E102" s="8"/>
+      <c r="F102" s="9"/>
+      <c r="G102" s="7"/>
+      <c r="H102" s="8"/>
+      <c r="I102" s="8"/>
+      <c r="J102" s="8"/>
+      <c r="K102" s="8"/>
+      <c r="L102" s="8"/>
+      <c r="M102" s="9"/>
+      <c r="N102" s="7"/>
+      <c r="O102" s="8"/>
+      <c r="P102" s="8"/>
+      <c r="Q102" s="9"/>
     </row>
     <row r="103" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="20">
+      <c r="A103" s="16">
         <v>36.08</v>
       </c>
       <c r="B103" s="3" t="s">
         <v>87</v>
       </c>
       <c r="C103" s="13"/>
-      <c r="D103" s="4"/>
-      <c r="F103" s="5"/>
-      <c r="G103" s="4"/>
-      <c r="M103" s="5"/>
-      <c r="N103" s="4"/>
-      <c r="Q103" s="5"/>
+      <c r="D103" s="15"/>
+      <c r="E103" s="8"/>
+      <c r="F103" s="9"/>
+      <c r="G103" s="7"/>
+      <c r="H103" s="8"/>
+      <c r="I103" s="8"/>
+      <c r="J103" s="8"/>
+      <c r="K103" s="8"/>
+      <c r="L103" s="8"/>
+      <c r="M103" s="9"/>
+      <c r="N103" s="7"/>
+      <c r="O103" s="8"/>
+      <c r="P103" s="8"/>
+      <c r="Q103" s="9"/>
     </row>
     <row r="104" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="20">
+      <c r="A104" s="16">
         <v>36.090000000000003</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>88</v>
       </c>
       <c r="C104" s="13"/>
-      <c r="D104" s="4"/>
-      <c r="F104" s="5"/>
-      <c r="G104" s="4"/>
-      <c r="M104" s="5"/>
-      <c r="N104" s="4"/>
-      <c r="Q104" s="5"/>
+      <c r="D104" s="15"/>
+      <c r="E104" s="8"/>
+      <c r="F104" s="9"/>
+      <c r="G104" s="7"/>
+      <c r="H104" s="8"/>
+      <c r="I104" s="8"/>
+      <c r="J104" s="8"/>
+      <c r="K104" s="8"/>
+      <c r="L104" s="8"/>
+      <c r="M104" s="9"/>
+      <c r="N104" s="7"/>
+      <c r="O104" s="8"/>
+      <c r="P104" s="8"/>
+      <c r="Q104" s="9"/>
     </row>
     <row r="105" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="20">
+      <c r="A105" s="16">
         <v>36.1</v>
       </c>
       <c r="B105" s="3" t="s">
         <v>89</v>
       </c>
       <c r="C105" s="13"/>
-      <c r="D105" s="4"/>
-      <c r="F105" s="5"/>
-      <c r="G105" s="4"/>
-      <c r="M105" s="5"/>
-      <c r="N105" s="4"/>
-      <c r="Q105" s="5"/>
+      <c r="D105" s="15"/>
+      <c r="E105" s="8"/>
+      <c r="F105" s="9"/>
+      <c r="G105" s="7"/>
+      <c r="H105" s="8"/>
+      <c r="I105" s="8"/>
+      <c r="J105" s="8"/>
+      <c r="K105" s="8"/>
+      <c r="L105" s="8"/>
+      <c r="M105" s="9"/>
+      <c r="N105" s="7"/>
+      <c r="O105" s="8"/>
+      <c r="P105" s="8"/>
+      <c r="Q105" s="9"/>
     </row>
     <row r="106" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="20">
+      <c r="A106" s="16">
         <v>36.11</v>
       </c>
       <c r="B106" s="3" t="s">
         <v>90</v>
       </c>
       <c r="C106" s="13"/>
-      <c r="D106" s="4"/>
-      <c r="F106" s="5"/>
-      <c r="G106" s="4"/>
-      <c r="M106" s="5"/>
-      <c r="N106" s="4"/>
-      <c r="Q106" s="5"/>
+      <c r="D106" s="15"/>
+      <c r="E106" s="8"/>
+      <c r="F106" s="9"/>
+      <c r="G106" s="7"/>
+      <c r="H106" s="8"/>
+      <c r="I106" s="8"/>
+      <c r="J106" s="8"/>
+      <c r="K106" s="8"/>
+      <c r="L106" s="8"/>
+      <c r="M106" s="9"/>
+      <c r="N106" s="7"/>
+      <c r="O106" s="8"/>
+      <c r="P106" s="8"/>
+      <c r="Q106" s="9"/>
     </row>
     <row r="107" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="20">
+      <c r="A107" s="16">
         <v>36.120000000000097</v>
       </c>
       <c r="B107" s="3" t="s">
         <v>91</v>
       </c>
       <c r="C107" s="13"/>
-      <c r="D107" s="4"/>
-      <c r="F107" s="5"/>
-      <c r="G107" s="4"/>
-      <c r="M107" s="5"/>
-      <c r="N107" s="4"/>
-      <c r="Q107" s="5"/>
+      <c r="D107" s="15"/>
+      <c r="E107" s="8"/>
+      <c r="F107" s="9"/>
+      <c r="G107" s="7"/>
+      <c r="H107" s="8"/>
+      <c r="I107" s="8"/>
+      <c r="J107" s="8"/>
+      <c r="K107" s="8"/>
+      <c r="L107" s="8"/>
+      <c r="M107" s="9"/>
+      <c r="N107" s="7"/>
+      <c r="O107" s="8"/>
+      <c r="P107" s="8"/>
+      <c r="Q107" s="9"/>
     </row>
     <row r="108" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="20">
+      <c r="A108" s="16">
         <v>36.130000000000102</v>
       </c>
       <c r="B108" s="3" t="s">
         <v>92</v>
       </c>
       <c r="C108" s="13"/>
-      <c r="D108" s="4"/>
-      <c r="F108" s="5"/>
-      <c r="G108" s="4"/>
-      <c r="M108" s="5"/>
-      <c r="N108" s="4"/>
-      <c r="Q108" s="5"/>
+      <c r="D108" s="15"/>
+      <c r="E108" s="8"/>
+      <c r="F108" s="9"/>
+      <c r="G108" s="7"/>
+      <c r="H108" s="8"/>
+      <c r="I108" s="8"/>
+      <c r="J108" s="8"/>
+      <c r="K108" s="8"/>
+      <c r="L108" s="8"/>
+      <c r="M108" s="9"/>
+      <c r="N108" s="7"/>
+      <c r="O108" s="8"/>
+      <c r="P108" s="8"/>
+      <c r="Q108" s="9"/>
     </row>
     <row r="109" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="20">
+      <c r="A109" s="16">
         <v>36.1400000000001</v>
       </c>
       <c r="B109" s="3" t="s">
         <v>93</v>
       </c>
       <c r="C109" s="13"/>
-      <c r="D109" s="4"/>
-      <c r="F109" s="5"/>
-      <c r="G109" s="4"/>
-      <c r="M109" s="5"/>
-      <c r="N109" s="4"/>
-      <c r="Q109" s="5"/>
+      <c r="D109" s="15"/>
+      <c r="E109" s="8"/>
+      <c r="F109" s="9"/>
+      <c r="G109" s="7"/>
+      <c r="H109" s="8"/>
+      <c r="I109" s="8"/>
+      <c r="J109" s="8"/>
+      <c r="K109" s="8"/>
+      <c r="L109" s="8"/>
+      <c r="M109" s="9"/>
+      <c r="N109" s="7"/>
+      <c r="O109" s="8"/>
+      <c r="P109" s="8"/>
+      <c r="Q109" s="9"/>
     </row>
     <row r="110" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="20">
+      <c r="A110" s="16">
         <v>36.150000000000098</v>
       </c>
       <c r="B110" s="3" t="s">
         <v>94</v>
       </c>
       <c r="C110" s="13"/>
-      <c r="D110" s="4"/>
-      <c r="F110" s="5"/>
-      <c r="G110" s="4"/>
-      <c r="M110" s="5"/>
-      <c r="N110" s="4"/>
-      <c r="Q110" s="5"/>
+      <c r="D110" s="15"/>
+      <c r="E110" s="8"/>
+      <c r="F110" s="9"/>
+      <c r="G110" s="7"/>
+      <c r="H110" s="8"/>
+      <c r="I110" s="8"/>
+      <c r="J110" s="8"/>
+      <c r="K110" s="8"/>
+      <c r="L110" s="8"/>
+      <c r="M110" s="9"/>
+      <c r="N110" s="7"/>
+      <c r="O110" s="8"/>
+      <c r="P110" s="8"/>
+      <c r="Q110" s="9"/>
     </row>
     <row r="111" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="20">
+      <c r="A111" s="16">
         <v>36.160000000000103</v>
       </c>
       <c r="B111" s="3" t="s">
         <v>95</v>
       </c>
       <c r="C111" s="13"/>
-      <c r="D111" s="4"/>
-      <c r="F111" s="5"/>
-      <c r="G111" s="4"/>
-      <c r="M111" s="5"/>
-      <c r="N111" s="4"/>
-      <c r="Q111" s="5"/>
+      <c r="D111" s="15"/>
+      <c r="E111" s="8"/>
+      <c r="F111" s="9"/>
+      <c r="G111" s="7"/>
+      <c r="H111" s="8"/>
+      <c r="I111" s="8"/>
+      <c r="J111" s="8"/>
+      <c r="K111" s="8"/>
+      <c r="L111" s="8"/>
+      <c r="M111" s="9"/>
+      <c r="N111" s="7"/>
+      <c r="O111" s="8"/>
+      <c r="P111" s="8"/>
+      <c r="Q111" s="9"/>
     </row>
     <row r="112" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="20">
+      <c r="A112" s="16">
         <v>36.170000000000101</v>
       </c>
       <c r="B112" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C112" s="15"/>
-      <c r="D112" s="6"/>
-      <c r="E112" s="7"/>
-      <c r="F112" s="8"/>
-      <c r="G112" s="6"/>
-      <c r="H112" s="7"/>
-      <c r="I112" s="7"/>
-      <c r="J112" s="7"/>
-      <c r="K112" s="7"/>
-      <c r="L112" s="7"/>
-      <c r="M112" s="8"/>
-      <c r="N112" s="6"/>
-      <c r="O112" s="7"/>
-      <c r="P112" s="7"/>
-      <c r="Q112" s="8"/>
+      <c r="C112" s="11"/>
+      <c r="D112" s="4"/>
+      <c r="E112" s="5"/>
+      <c r="F112" s="6"/>
+      <c r="G112" s="7"/>
+      <c r="H112" s="8"/>
+      <c r="I112" s="8"/>
+      <c r="J112" s="8"/>
+      <c r="K112" s="8"/>
+      <c r="L112" s="8"/>
+      <c r="M112" s="9"/>
+      <c r="N112" s="4"/>
+      <c r="O112" s="5"/>
+      <c r="P112" s="5"/>
+      <c r="Q112" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3264,268 +4072,268 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="10.83203125" style="25"/>
-    <col min="5" max="5" width="17.1640625" style="25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="25"/>
-    <col min="7" max="7" width="22.1640625" style="25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="25"/>
-    <col min="9" max="9" width="21.6640625" style="25" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="25"/>
+    <col min="1" max="4" width="10.83203125" style="21"/>
+    <col min="5" max="5" width="17.1640625" style="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="21"/>
+    <col min="7" max="7" width="22.1640625" style="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="21"/>
+    <col min="9" max="9" width="21.6640625" style="21" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="21"/>
   </cols>
   <sheetData>
     <row r="6" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D6" s="23"/>
-      <c r="E6" s="24" t="s">
+      <c r="D6" s="19"/>
+      <c r="E6" s="20" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="7" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D7" s="23"/>
-      <c r="E7" s="24"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="20"/>
     </row>
     <row r="8" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D8" s="26">
+      <c r="D8" s="22">
         <v>33.01</v>
       </c>
-      <c r="E8" s="27" t="s">
+      <c r="E8" s="23" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="9" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D9" s="26">
+      <c r="D9" s="22">
         <v>33.020000000000003</v>
       </c>
-      <c r="E9" s="27" t="s">
+      <c r="E9" s="23" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="10" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D10" s="29">
+      <c r="D10" s="25">
         <v>1</v>
       </c>
-      <c r="E10" s="27" t="s">
+      <c r="E10" s="23" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="11" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D11" s="29">
+      <c r="D11" s="25">
         <v>2</v>
       </c>
-      <c r="E11" s="27" t="s">
+      <c r="E11" s="23" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="12" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D12" s="29">
+      <c r="D12" s="25">
         <v>3</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="E12" s="23" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="13" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D13" s="26">
+      <c r="D13" s="22">
         <v>33.03</v>
       </c>
-      <c r="E13" s="27" t="s">
+      <c r="E13" s="23" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="14" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D14" s="29">
+      <c r="D14" s="25">
         <v>4</v>
       </c>
-      <c r="E14" s="27" t="s">
+      <c r="E14" s="23" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="15" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D15" s="29">
+      <c r="D15" s="25">
         <v>5</v>
       </c>
-      <c r="E15" s="27" t="s">
+      <c r="E15" s="23" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="16" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D16" s="26">
+      <c r="D16" s="22">
         <v>33.04</v>
       </c>
-      <c r="E16" s="27" t="s">
+      <c r="E16" s="23" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D17" s="26">
+      <c r="D17" s="22">
         <v>33.049999999999997</v>
       </c>
-      <c r="E17" s="27" t="s">
+      <c r="E17" s="23" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="18" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D18" s="23"/>
-      <c r="E18" s="27"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="23"/>
     </row>
     <row r="19" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D19" s="23"/>
-      <c r="E19" s="24" t="s">
+      <c r="D19" s="19"/>
+      <c r="E19" s="20" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="20" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D20" s="23"/>
-      <c r="E20" s="24"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="20"/>
     </row>
     <row r="21" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D21" s="28">
+      <c r="D21" s="24">
         <v>35.000999999999998</v>
       </c>
-      <c r="E21" s="27" t="s">
+      <c r="E21" s="23" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="22" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D22" s="28">
+      <c r="D22" s="24">
         <v>35.002000000000002</v>
       </c>
-      <c r="E22" s="27" t="s">
+      <c r="E22" s="23" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="23" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D23" s="26">
+      <c r="D23" s="22">
         <v>35.01</v>
       </c>
-      <c r="E23" s="27" t="s">
+      <c r="E23" s="23" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="24" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D24" s="26">
+      <c r="D24" s="22">
         <v>35.020000000000003</v>
       </c>
-      <c r="E24" s="27" t="s">
+      <c r="E24" s="23" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="25" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D25" s="26">
+      <c r="D25" s="22">
         <v>35.03</v>
       </c>
-      <c r="E25" s="27" t="s">
+      <c r="E25" s="23" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="26" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D26" s="26">
+      <c r="D26" s="22">
         <v>35.04</v>
       </c>
-      <c r="E26" s="27" t="s">
+      <c r="E26" s="23" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="27" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D27" s="26">
+      <c r="D27" s="22">
         <v>35.049999999999997</v>
       </c>
-      <c r="E27" s="27" t="s">
+      <c r="E27" s="23" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="28" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D28" s="26">
+      <c r="D28" s="22">
         <v>35.06</v>
       </c>
-      <c r="E28" s="27" t="s">
+      <c r="E28" s="23" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="29" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D29" s="26">
+      <c r="D29" s="22">
         <v>35.07</v>
       </c>
-      <c r="E29" s="27" t="s">
+      <c r="E29" s="23" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="30" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D30" s="26">
+      <c r="D30" s="22">
         <v>35.08</v>
       </c>
-      <c r="E30" s="27" t="s">
+      <c r="E30" s="23" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="31" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D31" s="26">
+      <c r="D31" s="22">
         <v>35.090000000000003</v>
       </c>
-      <c r="E31" s="27" t="s">
+      <c r="E31" s="23" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="32" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D32" s="26">
+      <c r="D32" s="22">
         <v>35.1</v>
       </c>
-      <c r="E32" s="27" t="s">
+      <c r="E32" s="23" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="33" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D33" s="26">
+      <c r="D33" s="22">
         <v>35.11</v>
       </c>
-      <c r="E33" s="27" t="s">
+      <c r="E33" s="23" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="34" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D34" s="26">
+      <c r="D34" s="22">
         <v>35.120000000000097</v>
       </c>
-      <c r="E34" s="27" t="s">
+      <c r="E34" s="23" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="35" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D35" s="26">
+      <c r="D35" s="22">
         <v>35.130000000000102</v>
       </c>
-      <c r="E35" s="27" t="s">
+      <c r="E35" s="23" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="36" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D36" s="26">
+      <c r="D36" s="22">
         <v>35.1400000000001</v>
       </c>
-      <c r="E36" s="27" t="s">
+      <c r="E36" s="23" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="37" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D37" s="26">
+      <c r="D37" s="22">
         <v>35.150000000000098</v>
       </c>
-      <c r="E37" s="27" t="s">
+      <c r="E37" s="23" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="38" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D38" s="26">
+      <c r="D38" s="22">
         <v>35.160000000000103</v>
       </c>
-      <c r="E38" s="27" t="s">
+      <c r="E38" s="23" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="39" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D39" s="26">
+      <c r="D39" s="22">
         <v>35.170000000000101</v>
       </c>
-      <c r="E39" s="27" t="s">
+      <c r="E39" s="23" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding note about deque classes
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bharat/bctci/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02E69B6A-06B7-F54D-B378-CFEE98C374B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDDF08EC-4117-364B-BF94-41B0EDA1AF04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{233FF15D-0BCB-6B46-B450-599851EED7C1}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="186">
   <si>
     <t>Sets &amp; Maps</t>
   </si>
@@ -578,9 +578,6 @@
     <t>Fairly well done</t>
   </si>
   <si>
-    <t>Keep items in relevant queues, and iterate from the end till start time to get count</t>
-  </si>
-  <si>
     <t>Since timestamps are monotonic, could choose to prune old entries, either at time of entry or gets. Gets make more sense since there should be fewer of them</t>
   </si>
   <si>
@@ -594,6 +591,12 @@
   </si>
   <si>
     <t>Mostly good</t>
+  </si>
+  <si>
+    <t>Keep items in relevant arrays, and iterate from the end till start time to get count</t>
+  </si>
+  <si>
+    <t>Yes, need a basic queue class or get familiar with deque data struture</t>
   </si>
 </sst>
 </file>
@@ -1244,7 +1247,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q19" sqref="Q19"/>
+      <selection pane="bottomLeft" activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2005,7 +2008,7 @@
         <v>16</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="D19" s="15">
         <v>45865</v>
@@ -2017,25 +2020,25 @@
         <v>125</v>
       </c>
       <c r="G19" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="H19" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="H19" s="8" t="s">
+      <c r="I19" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="I19" s="8" t="s">
+      <c r="J19" s="8" t="s">
         <v>182</v>
-      </c>
-      <c r="J19" s="8" t="s">
-        <v>183</v>
       </c>
       <c r="K19" s="8" t="s">
         <v>122</v>
       </c>
       <c r="L19" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="M19" s="9" t="s">
-        <v>122</v>
+        <v>185</v>
       </c>
       <c r="N19" s="7">
         <v>4</v>

</xml_diff>

<commit_message>
Solving tought sets/maps problem
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bharat/bctci/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{572FD233-8A52-5447-8242-A36CD214BA5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E912C60-3FB4-EA46-9F33-C3DD706C1A14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{233FF15D-0BCB-6B46-B450-599851EED7C1}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="210">
   <si>
     <t>Sets &amp; Maps</t>
   </si>
@@ -645,6 +645,30 @@
   </si>
   <si>
     <t>Good problem, need to not rush</t>
+  </si>
+  <si>
+    <t>Keep two maps open, one for ticket based actions and one for agent based actions. Find anomalies based on rules</t>
+  </si>
+  <si>
+    <t>1 hour</t>
+  </si>
+  <si>
+    <t>Proper lifecycle case analysis.</t>
+  </si>
+  <si>
+    <t>Case analysis</t>
+  </si>
+  <si>
+    <t>This was a new roadblock, moved too fast for the problem, but didn't know it was going to be this intricate</t>
+  </si>
+  <si>
+    <t>Accessing named tupes</t>
+  </si>
+  <si>
+    <t>Get better at case analysis</t>
+  </si>
+  <si>
+    <t>Yes, case analysis process and examples</t>
   </si>
 </sst>
 </file>
@@ -1293,9 +1317,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4095FB6B-33CD-C94D-A3B2-EAADF58B3AE5}">
   <dimension ref="A1:Q112"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1879,21 +1903,51 @@
       <c r="B12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="8"/>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="9"/>
+      <c r="C12" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="D12" s="15">
+        <v>45868</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="L12" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="M12" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="N12" s="7">
+        <v>2</v>
+      </c>
+      <c r="O12" s="8">
+        <v>3</v>
+      </c>
+      <c r="P12" s="8">
+        <v>2</v>
+      </c>
+      <c r="Q12" s="9">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="1:17" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="16">
@@ -1972,7 +2026,7 @@
       <c r="P16" s="8"/>
       <c r="Q16" s="9"/>
     </row>
-    <row r="17" spans="1:17" ht="100" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" ht="80" x14ac:dyDescent="0.25">
       <c r="A17" s="16">
         <v>32.01</v>
       </c>

</xml_diff>

<commit_message>
Solving a stack problem
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bharat/bctci/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E912C60-3FB4-EA46-9F33-C3DD706C1A14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18153D34-BED9-0949-908A-668ED14EF082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{233FF15D-0BCB-6B46-B450-599851EED7C1}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="214">
   <si>
     <t>Sets &amp; Maps</t>
   </si>
@@ -669,6 +669,18 @@
   </si>
   <si>
     <t>Yes, case analysis process and examples</t>
+  </si>
+  <si>
+    <t>Stack to keep track of level of nesting, and an array of substrings for result</t>
+  </si>
+  <si>
+    <t>Solution was fine, just used some extra space</t>
+  </si>
+  <si>
+    <t>Storing excessive information. The answer only cared about count</t>
+  </si>
+  <si>
+    <t>It would be more impressive if I squish down on space complexity by seeing only what the answer needs</t>
   </si>
 </sst>
 </file>
@@ -1317,9 +1329,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4095FB6B-33CD-C94D-A3B2-EAADF58B3AE5}">
   <dimension ref="A1:Q112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R12" sqref="R12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2291,28 +2303,58 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" ht="100" x14ac:dyDescent="0.25">
       <c r="A22" s="16">
         <v>32.06</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="9"/>
-      <c r="N22" s="7"/>
-      <c r="O22" s="8"/>
-      <c r="P22" s="8"/>
-      <c r="Q22" s="9"/>
+      <c r="C22" s="13" t="s">
+        <v>210</v>
+      </c>
+      <c r="D22" s="15">
+        <v>45868</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="J22" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="K22" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="L22" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="M22" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="N22" s="7">
+        <v>4</v>
+      </c>
+      <c r="O22" s="8">
+        <v>4</v>
+      </c>
+      <c r="P22" s="8">
+        <v>4</v>
+      </c>
+      <c r="Q22" s="9">
+        <v>4</v>
+      </c>
     </row>
     <row r="23" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="16">

</xml_diff>

<commit_message>
Wrapping up sets and queues
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bharat/bctci/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFE3E2C9-C916-A546-8B42-40FDAD209BD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C4CEDB-2126-8540-82D0-4AF77790678A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{233FF15D-0BCB-6B46-B450-599851EED7C1}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="226">
   <si>
     <t>Sets &amp; Maps</t>
   </si>
@@ -699,6 +699,24 @@
   </si>
   <si>
     <t>Good mix of sets, dicts and stacks for this question</t>
+  </si>
+  <si>
+    <t>Keeping track of incorrect closes, and getting indices of dangling opens</t>
+  </si>
+  <si>
+    <t>Soltuion was fine</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>String concentation is expensive in python</t>
+  </si>
+  <si>
+    <t>Good solution</t>
+  </si>
+  <si>
+    <t>String concetenation</t>
   </si>
 </sst>
 </file>
@@ -1347,9 +1365,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4095FB6B-33CD-C94D-A3B2-EAADF58B3AE5}">
   <dimension ref="A1:Q112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q23" sqref="Q23"/>
+      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2427,28 +2445,58 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="16">
         <v>32.08</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="8"/>
-      <c r="M24" s="9"/>
-      <c r="N24" s="7"/>
-      <c r="O24" s="8"/>
-      <c r="P24" s="8"/>
-      <c r="Q24" s="9"/>
+      <c r="C24" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="D24" s="15">
+        <v>45869</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="I24" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="J24" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="K24" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="L24" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="M24" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="N24" s="7">
+        <v>4</v>
+      </c>
+      <c r="O24" s="8">
+        <v>3</v>
+      </c>
+      <c r="P24" s="8">
+        <v>3</v>
+      </c>
+      <c r="Q24" s="9">
+        <v>3</v>
+      </c>
     </row>
     <row r="25" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="13"/>

</xml_diff>

<commit_message>
Tough set questions (even recognised by book)
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bharat/bctci/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C4CEDB-2126-8540-82D0-4AF77790678A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2380281-A85C-C042-902A-557F08FA9DBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{233FF15D-0BCB-6B46-B450-599851EED7C1}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="234">
   <si>
     <t>Sets &amp; Maps</t>
   </si>
@@ -717,6 +717,30 @@
   </si>
   <si>
     <t>String concetenation</t>
+  </si>
+  <si>
+    <t>Find intersection of each set of values without current index, return the longest set</t>
+  </si>
+  <si>
+    <t>25 minutes</t>
+  </si>
+  <si>
+    <t>40 minutes</t>
+  </si>
+  <si>
+    <t>You can't initialise a full set, instead initialise to none, check for none in loop, and then set a value</t>
+  </si>
+  <si>
+    <t>No universal set</t>
+  </si>
+  <si>
+    <t>I missed considering values inside sets, and filtering them about based on their candidacy in other sets</t>
+  </si>
+  <si>
+    <t>Can't say. Need to read triggers chapter.</t>
+  </si>
+  <si>
+    <t>Tough question. Don't think I could have cracked this one without guidance</t>
   </si>
 </sst>
 </file>
@@ -1366,8 +1390,8 @@
   <dimension ref="A1:Q112"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2004,21 +2028,49 @@
       <c r="B13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
+      <c r="C13" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="D13" s="15">
+        <v>45868</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="L13" s="8" t="s">
+        <v>233</v>
+      </c>
       <c r="M13" s="9"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="9"/>
+      <c r="N13" s="7">
+        <v>3</v>
+      </c>
+      <c r="O13" s="8">
+        <v>2</v>
+      </c>
+      <c r="P13" s="8">
+        <v>3</v>
+      </c>
+      <c r="Q13" s="9">
+        <v>2</v>
+      </c>
     </row>
     <row r="14" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="13"/>

</xml_diff>

<commit_message>
First few recursion problems
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bharat/bctci/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2380281-A85C-C042-902A-557F08FA9DBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6998F7FA-AC4A-094E-8BA8-46A0654681A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{233FF15D-0BCB-6B46-B450-599851EED7C1}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="243">
   <si>
     <t>Sets &amp; Maps</t>
   </si>
@@ -741,6 +741,33 @@
   </si>
   <si>
     <t>Tough question. Don't think I could have cracked this one without guidance</t>
+  </si>
+  <si>
+    <t>Recursive approach, base case ""</t>
+  </si>
+  <si>
+    <t>Fine</t>
+  </si>
+  <si>
+    <t>That problem was breaking down into a subset of itself</t>
+  </si>
+  <si>
+    <t>Good practice</t>
+  </si>
+  <si>
+    <t>Used a helper function to keep track of state</t>
+  </si>
+  <si>
+    <t>Eager/lazy checking</t>
+  </si>
+  <si>
+    <t>My recursion was not very elegant</t>
+  </si>
+  <si>
+    <t>Good review</t>
+  </si>
+  <si>
+    <t>Lazy &gt; Eager for cases where there is more than one recursive call per element</t>
   </si>
 </sst>
 </file>
@@ -1390,8 +1417,8 @@
   <dimension ref="A1:Q112"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2605,51 +2632,111 @@
       <c r="P27" s="8"/>
       <c r="Q27" s="9"/>
     </row>
-    <row r="28" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" ht="40" x14ac:dyDescent="0.25">
       <c r="A28" s="16">
         <v>33.01</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="9"/>
-      <c r="N28" s="7"/>
-      <c r="O28" s="8"/>
-      <c r="P28" s="8"/>
-      <c r="Q28" s="9"/>
-    </row>
-    <row r="29" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C28" s="13" t="s">
+        <v>234</v>
+      </c>
+      <c r="D28" s="15">
+        <v>45869</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="I28" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="J28" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="K28" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="L28" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="M28" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="N28" s="7">
+        <v>4</v>
+      </c>
+      <c r="O28" s="8">
+        <v>4</v>
+      </c>
+      <c r="P28" s="8">
+        <v>4</v>
+      </c>
+      <c r="Q28" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="16">
         <v>33.020000000000003</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8"/>
-      <c r="M29" s="9"/>
-      <c r="N29" s="7"/>
-      <c r="O29" s="8"/>
-      <c r="P29" s="8"/>
-      <c r="Q29" s="9"/>
+      <c r="C29" s="13" t="s">
+        <v>238</v>
+      </c>
+      <c r="D29" s="15">
+        <v>45870</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="I29" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="J29" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="K29" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="L29" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="M29" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="N29" s="7">
+        <v>3</v>
+      </c>
+      <c r="O29" s="8">
+        <v>3</v>
+      </c>
+      <c r="P29" s="8">
+        <v>3</v>
+      </c>
+      <c r="Q29" s="9">
+        <v>3</v>
+      </c>
     </row>
     <row r="30" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="17">

</xml_diff>

<commit_message>
Power mod recursion problem
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bharat/bctci/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6998F7FA-AC4A-094E-8BA8-46A0654681A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4495B81F-01FB-6144-883A-E6FEE7682D4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{233FF15D-0BCB-6B46-B450-599851EED7C1}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="254">
   <si>
     <t>Sets &amp; Maps</t>
   </si>
@@ -768,6 +768,39 @@
   </si>
   <si>
     <t>Lazy &gt; Eager for cases where there is more than one recursive call per element</t>
+  </si>
+  <si>
+    <t>Recursive n times</t>
+  </si>
+  <si>
+    <t>The even power trick</t>
+  </si>
+  <si>
+    <t>Don't know any</t>
+  </si>
+  <si>
+    <t>Interesting trick</t>
+  </si>
+  <si>
+    <t>Yes, keep modulo-ing property, and even powers trick</t>
+  </si>
+  <si>
+    <t>Merge sort</t>
+  </si>
+  <si>
+    <t>Same as book!</t>
+  </si>
+  <si>
+    <t>30 minutes</t>
+  </si>
+  <si>
+    <t>Learning phase</t>
+  </si>
+  <si>
+    <t>There is a separate merge method</t>
+  </si>
+  <si>
+    <t>Consider how BAD applies here</t>
   </si>
 </sst>
 </file>
@@ -1414,11 +1447,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4095FB6B-33CD-C94D-A3B2-EAADF58B3AE5}">
-  <dimension ref="A1:Q112"/>
+  <dimension ref="A1:Q110"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2738,58 +2771,118 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="17">
-        <v>1</v>
+    <row r="30" spans="1:17" ht="40" x14ac:dyDescent="0.25">
+      <c r="A30" s="18">
+        <v>33.024999999999999</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="8"/>
-      <c r="M30" s="9"/>
-      <c r="N30" s="7"/>
-      <c r="O30" s="8"/>
-      <c r="P30" s="8"/>
-      <c r="Q30" s="9"/>
-    </row>
-    <row r="31" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="17">
-        <v>2</v>
+        <v>248</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="D30" s="15">
+        <v>45871</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="H30" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="I30" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="J30" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="K30" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="L30" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="M30" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="N30" s="7">
+        <v>3</v>
+      </c>
+      <c r="O30" s="8">
+        <v>3</v>
+      </c>
+      <c r="P30" s="8">
+        <v>3</v>
+      </c>
+      <c r="Q30" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" ht="40" x14ac:dyDescent="0.25">
+      <c r="A31" s="16">
+        <v>33.03</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
-      <c r="M31" s="9"/>
-      <c r="N31" s="7"/>
-      <c r="O31" s="8"/>
-      <c r="P31" s="8"/>
-      <c r="Q31" s="9"/>
+        <v>26</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>243</v>
+      </c>
+      <c r="D31" s="15">
+        <v>45871</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="H31" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="I31" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="J31" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="K31" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="L31" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="M31" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="N31" s="7">
+        <v>3</v>
+      </c>
+      <c r="O31" s="8">
+        <v>3</v>
+      </c>
+      <c r="P31" s="8">
+        <v>3</v>
+      </c>
+      <c r="Q31" s="9">
+        <v>3</v>
+      </c>
     </row>
     <row r="32" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C32" s="13"/>
       <c r="D32" s="15"/>
@@ -2808,11 +2901,11 @@
       <c r="Q32" s="9"/>
     </row>
     <row r="33" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="16">
-        <v>33.03</v>
+      <c r="A33" s="17">
+        <v>5</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C33" s="13"/>
       <c r="D33" s="15"/>
@@ -2831,11 +2924,11 @@
       <c r="Q33" s="9"/>
     </row>
     <row r="34" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="17">
-        <v>4</v>
+      <c r="A34" s="16">
+        <v>33.04</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C34" s="13"/>
       <c r="D34" s="15"/>
@@ -2854,11 +2947,11 @@
       <c r="Q34" s="9"/>
     </row>
     <row r="35" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="17">
-        <v>5</v>
+      <c r="A35" s="16">
+        <v>33.049999999999997</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C35" s="13"/>
       <c r="D35" s="15"/>
@@ -2877,12 +2970,6 @@
       <c r="Q35" s="9"/>
     </row>
     <row r="36" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="16">
-        <v>33.04</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="C36" s="13"/>
       <c r="D36" s="15"/>
       <c r="E36" s="8"/>
@@ -2900,11 +2987,8 @@
       <c r="Q36" s="9"/>
     </row>
     <row r="37" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="16">
-        <v>33.049999999999997</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>22</v>
+      <c r="B37" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="C37" s="13"/>
       <c r="D37" s="15"/>
@@ -2923,6 +3007,7 @@
       <c r="Q37" s="9"/>
     </row>
     <row r="38" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="2"/>
       <c r="C38" s="13"/>
       <c r="D38" s="15"/>
       <c r="E38" s="8"/>
@@ -2940,8 +3025,11 @@
       <c r="Q38" s="9"/>
     </row>
     <row r="39" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="2" t="s">
-        <v>32</v>
+      <c r="A39" s="18">
+        <v>35.000999999999998</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="C39" s="13"/>
       <c r="D39" s="15"/>
@@ -2960,7 +3048,12 @@
       <c r="Q39" s="9"/>
     </row>
     <row r="40" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="2"/>
+      <c r="A40" s="18">
+        <v>35.002000000000002</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="C40" s="13"/>
       <c r="D40" s="15"/>
       <c r="E40" s="8"/>
@@ -2978,11 +3071,11 @@
       <c r="Q40" s="9"/>
     </row>
     <row r="41" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="18">
-        <v>35.000999999999998</v>
+      <c r="A41" s="16">
+        <v>35.01</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C41" s="13"/>
       <c r="D41" s="15"/>
@@ -3001,11 +3094,11 @@
       <c r="Q41" s="9"/>
     </row>
     <row r="42" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="18">
-        <v>35.002000000000002</v>
+      <c r="A42" s="16">
+        <v>35.020000000000003</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C42" s="13"/>
       <c r="D42" s="15"/>
@@ -3025,10 +3118,10 @@
     </row>
     <row r="43" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="16">
-        <v>35.01</v>
+        <v>35.03</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C43" s="13"/>
       <c r="D43" s="15"/>
@@ -3048,10 +3141,10 @@
     </row>
     <row r="44" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="16">
-        <v>35.020000000000003</v>
+        <v>35.04</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C44" s="13"/>
       <c r="D44" s="15"/>
@@ -3071,10 +3164,10 @@
     </row>
     <row r="45" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="16">
-        <v>35.03</v>
+        <v>35.049999999999997</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C45" s="13"/>
       <c r="D45" s="15"/>
@@ -3094,10 +3187,10 @@
     </row>
     <row r="46" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="16">
-        <v>35.04</v>
+        <v>35.06</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C46" s="13"/>
       <c r="D46" s="15"/>
@@ -3117,10 +3210,10 @@
     </row>
     <row r="47" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="16">
-        <v>35.049999999999997</v>
+        <v>35.07</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C47" s="13"/>
       <c r="D47" s="15"/>
@@ -3140,10 +3233,10 @@
     </row>
     <row r="48" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="16">
-        <v>35.06</v>
+        <v>35.08</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C48" s="13"/>
       <c r="D48" s="15"/>
@@ -3163,10 +3256,10 @@
     </row>
     <row r="49" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="16">
-        <v>35.07</v>
+        <v>35.090000000000003</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C49" s="13"/>
       <c r="D49" s="15"/>
@@ -3186,10 +3279,10 @@
     </row>
     <row r="50" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="16">
-        <v>35.08</v>
+        <v>35.1</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C50" s="13"/>
       <c r="D50" s="15"/>
@@ -3209,10 +3302,10 @@
     </row>
     <row r="51" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="16">
-        <v>35.090000000000003</v>
+        <v>35.11</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C51" s="13"/>
       <c r="D51" s="15"/>
@@ -3232,10 +3325,10 @@
     </row>
     <row r="52" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="16">
-        <v>35.1</v>
+        <v>35.120000000000097</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C52" s="13"/>
       <c r="D52" s="15"/>
@@ -3255,10 +3348,10 @@
     </row>
     <row r="53" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="16">
-        <v>35.11</v>
+        <v>35.130000000000102</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C53" s="13"/>
       <c r="D53" s="15"/>
@@ -3278,10 +3371,10 @@
     </row>
     <row r="54" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="16">
-        <v>35.120000000000097</v>
+        <v>35.1400000000001</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C54" s="13"/>
       <c r="D54" s="15"/>
@@ -3301,10 +3394,10 @@
     </row>
     <row r="55" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="16">
-        <v>35.130000000000102</v>
+        <v>35.150000000000098</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C55" s="13"/>
       <c r="D55" s="15"/>
@@ -3324,10 +3417,10 @@
     </row>
     <row r="56" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="16">
-        <v>35.1400000000001</v>
+        <v>35.160000000000103</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C56" s="13"/>
       <c r="D56" s="15"/>
@@ -3347,10 +3440,10 @@
     </row>
     <row r="57" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="16">
-        <v>35.150000000000098</v>
+        <v>35.170000000000101</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C57" s="13"/>
       <c r="D57" s="15"/>
@@ -3369,12 +3462,6 @@
       <c r="Q57" s="9"/>
     </row>
     <row r="58" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="16">
-        <v>35.160000000000103</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>50</v>
-      </c>
       <c r="C58" s="13"/>
       <c r="D58" s="15"/>
       <c r="E58" s="8"/>
@@ -3392,11 +3479,8 @@
       <c r="Q58" s="9"/>
     </row>
     <row r="59" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="16">
-        <v>35.170000000000101</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>51</v>
+      <c r="B59" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="C59" s="13"/>
       <c r="D59" s="15"/>
@@ -3432,8 +3516,11 @@
       <c r="Q60" s="9"/>
     </row>
     <row r="61" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="2" t="s">
-        <v>53</v>
+      <c r="A61" s="17">
+        <v>1</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="C61" s="13"/>
       <c r="D61" s="15"/>
@@ -3452,6 +3539,12 @@
       <c r="Q61" s="9"/>
     </row>
     <row r="62" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="17">
+        <v>2</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="C62" s="13"/>
       <c r="D62" s="15"/>
       <c r="E62" s="8"/>
@@ -3470,10 +3563,10 @@
     </row>
     <row r="63" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C63" s="13"/>
       <c r="D63" s="15"/>
@@ -3493,10 +3586,10 @@
     </row>
     <row r="64" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="17">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C64" s="13"/>
       <c r="D64" s="15"/>
@@ -3516,10 +3609,10 @@
     </row>
     <row r="65" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="17">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C65" s="13"/>
       <c r="D65" s="15"/>
@@ -3539,10 +3632,10 @@
     </row>
     <row r="66" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="17">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C66" s="13"/>
       <c r="D66" s="15"/>
@@ -3561,12 +3654,6 @@
       <c r="Q66" s="9"/>
     </row>
     <row r="67" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="17">
-        <v>5</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>59</v>
-      </c>
       <c r="C67" s="13"/>
       <c r="D67" s="15"/>
       <c r="E67" s="8"/>
@@ -3584,11 +3671,8 @@
       <c r="Q67" s="9"/>
     </row>
     <row r="68" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="17">
-        <v>6</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>58</v>
+      <c r="B68" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="C68" s="13"/>
       <c r="D68" s="15"/>
@@ -3624,8 +3708,11 @@
       <c r="Q69" s="9"/>
     </row>
     <row r="70" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="2" t="s">
-        <v>52</v>
+      <c r="A70" s="16">
+        <v>39.01</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C70" s="13"/>
       <c r="D70" s="15"/>
@@ -3644,6 +3731,12 @@
       <c r="Q70" s="9"/>
     </row>
     <row r="71" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="16">
+        <v>39.020000000000003</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>69</v>
+      </c>
       <c r="C71" s="13"/>
       <c r="D71" s="15"/>
       <c r="E71" s="8"/>
@@ -3662,10 +3755,10 @@
     </row>
     <row r="72" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="16">
-        <v>39.01</v>
+        <v>39.03</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C72" s="13"/>
       <c r="D72" s="15"/>
@@ -3685,10 +3778,10 @@
     </row>
     <row r="73" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="16">
-        <v>39.020000000000003</v>
+        <v>39.04</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C73" s="13"/>
       <c r="D73" s="15"/>
@@ -3708,10 +3801,10 @@
     </row>
     <row r="74" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="16">
-        <v>39.03</v>
+        <v>39.049999999999997</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C74" s="13"/>
       <c r="D74" s="15"/>
@@ -3731,10 +3824,10 @@
     </row>
     <row r="75" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="16">
-        <v>39.04</v>
+        <v>39.06</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C75" s="13"/>
       <c r="D75" s="15"/>
@@ -3754,10 +3847,10 @@
     </row>
     <row r="76" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="16">
-        <v>39.049999999999997</v>
+        <v>39.07</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C76" s="13"/>
       <c r="D76" s="15"/>
@@ -3777,10 +3870,10 @@
     </row>
     <row r="77" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="16">
-        <v>39.06</v>
+        <v>39.08</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C77" s="13"/>
       <c r="D77" s="15"/>
@@ -3800,10 +3893,10 @@
     </row>
     <row r="78" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="16">
-        <v>39.07</v>
+        <v>39.090000000000003</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C78" s="13"/>
       <c r="D78" s="15"/>
@@ -3823,10 +3916,10 @@
     </row>
     <row r="79" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="16">
-        <v>39.08</v>
+        <v>39.1</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C79" s="13"/>
       <c r="D79" s="15"/>
@@ -3846,10 +3939,10 @@
     </row>
     <row r="80" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="16">
-        <v>39.090000000000003</v>
+        <v>39.11</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C80" s="13"/>
       <c r="D80" s="15"/>
@@ -3868,12 +3961,6 @@
       <c r="Q80" s="9"/>
     </row>
     <row r="81" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="16">
-        <v>39.1</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="C81" s="13"/>
       <c r="D81" s="15"/>
       <c r="E81" s="8"/>
@@ -3891,11 +3978,8 @@
       <c r="Q81" s="9"/>
     </row>
     <row r="82" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="16">
-        <v>39.11</v>
-      </c>
-      <c r="B82" s="3" t="s">
-        <v>60</v>
+      <c r="B82" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="C82" s="13"/>
       <c r="D82" s="15"/>
@@ -3914,6 +3998,7 @@
       <c r="Q82" s="9"/>
     </row>
     <row r="83" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="18"/>
       <c r="C83" s="13"/>
       <c r="D83" s="15"/>
       <c r="E83" s="8"/>
@@ -3931,8 +4016,9 @@
       <c r="Q83" s="9"/>
     </row>
     <row r="84" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B84" s="2" t="s">
-        <v>71</v>
+      <c r="A84" s="18"/>
+      <c r="B84" s="3" t="s">
+        <v>73</v>
       </c>
       <c r="C84" s="13"/>
       <c r="D84" s="15"/>
@@ -3951,7 +4037,12 @@
       <c r="Q84" s="9"/>
     </row>
     <row r="85" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="18"/>
+      <c r="A85" s="16">
+        <v>41.01</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="C85" s="13"/>
       <c r="D85" s="15"/>
       <c r="E85" s="8"/>
@@ -3969,9 +4060,11 @@
       <c r="Q85" s="9"/>
     </row>
     <row r="86" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="18"/>
+      <c r="A86" s="16">
+        <v>41.02</v>
+      </c>
       <c r="B86" s="3" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C86" s="13"/>
       <c r="D86" s="15"/>
@@ -3991,10 +4084,10 @@
     </row>
     <row r="87" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="16">
-        <v>41.01</v>
+        <v>41.03</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C87" s="13"/>
       <c r="D87" s="15"/>
@@ -4014,10 +4107,10 @@
     </row>
     <row r="88" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="16">
-        <v>41.02</v>
+        <v>41.04</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C88" s="13"/>
       <c r="D88" s="15"/>
@@ -4037,10 +4130,10 @@
     </row>
     <row r="89" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="16">
-        <v>41.03</v>
+        <v>41.05</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C89" s="13"/>
       <c r="D89" s="15"/>
@@ -4060,10 +4153,10 @@
     </row>
     <row r="90" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="16">
-        <v>41.04</v>
+        <v>41.06</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C90" s="13"/>
       <c r="D90" s="15"/>
@@ -4082,12 +4175,6 @@
       <c r="Q90" s="9"/>
     </row>
     <row r="91" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="16">
-        <v>41.05</v>
-      </c>
-      <c r="B91" s="3" t="s">
-        <v>75</v>
-      </c>
       <c r="C91" s="13"/>
       <c r="D91" s="15"/>
       <c r="E91" s="8"/>
@@ -4105,11 +4192,8 @@
       <c r="Q91" s="9"/>
     </row>
     <row r="92" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="16">
-        <v>41.06</v>
-      </c>
-      <c r="B92" s="3" t="s">
-        <v>74</v>
+      <c r="B92" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="C92" s="13"/>
       <c r="D92" s="15"/>
@@ -4145,8 +4229,11 @@
       <c r="Q93" s="9"/>
     </row>
     <row r="94" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B94" s="2" t="s">
-        <v>79</v>
+      <c r="A94" s="16">
+        <v>36.01</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>80</v>
       </c>
       <c r="C94" s="13"/>
       <c r="D94" s="15"/>
@@ -4165,6 +4252,12 @@
       <c r="Q94" s="9"/>
     </row>
     <row r="95" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="16">
+        <v>36.020000000000003</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="C95" s="13"/>
       <c r="D95" s="15"/>
       <c r="E95" s="8"/>
@@ -4183,10 +4276,10 @@
     </row>
     <row r="96" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="16">
-        <v>36.01</v>
+        <v>36.03</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C96" s="13"/>
       <c r="D96" s="15"/>
@@ -4206,10 +4299,10 @@
     </row>
     <row r="97" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="16">
-        <v>36.020000000000003</v>
+        <v>36.04</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C97" s="13"/>
       <c r="D97" s="15"/>
@@ -4229,10 +4322,10 @@
     </row>
     <row r="98" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="16">
-        <v>36.03</v>
+        <v>36.049999999999997</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C98" s="13"/>
       <c r="D98" s="15"/>
@@ -4252,10 +4345,10 @@
     </row>
     <row r="99" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="16">
-        <v>36.04</v>
+        <v>36.06</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C99" s="13"/>
       <c r="D99" s="15"/>
@@ -4275,10 +4368,10 @@
     </row>
     <row r="100" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="16">
-        <v>36.049999999999997</v>
+        <v>36.07</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C100" s="13"/>
       <c r="D100" s="15"/>
@@ -4298,10 +4391,10 @@
     </row>
     <row r="101" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="16">
-        <v>36.06</v>
+        <v>36.08</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C101" s="13"/>
       <c r="D101" s="15"/>
@@ -4321,10 +4414,10 @@
     </row>
     <row r="102" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="16">
-        <v>36.07</v>
+        <v>36.090000000000003</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C102" s="13"/>
       <c r="D102" s="15"/>
@@ -4344,10 +4437,10 @@
     </row>
     <row r="103" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="16">
-        <v>36.08</v>
+        <v>36.1</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C103" s="13"/>
       <c r="D103" s="15"/>
@@ -4367,10 +4460,10 @@
     </row>
     <row r="104" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="16">
-        <v>36.090000000000003</v>
+        <v>36.11</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C104" s="13"/>
       <c r="D104" s="15"/>
@@ -4390,10 +4483,10 @@
     </row>
     <row r="105" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="16">
-        <v>36.1</v>
+        <v>36.120000000000097</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C105" s="13"/>
       <c r="D105" s="15"/>
@@ -4413,10 +4506,10 @@
     </row>
     <row r="106" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="16">
-        <v>36.11</v>
+        <v>36.130000000000102</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C106" s="13"/>
       <c r="D106" s="15"/>
@@ -4436,10 +4529,10 @@
     </row>
     <row r="107" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="16">
-        <v>36.120000000000097</v>
+        <v>36.1400000000001</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C107" s="13"/>
       <c r="D107" s="15"/>
@@ -4459,10 +4552,10 @@
     </row>
     <row r="108" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="16">
-        <v>36.130000000000102</v>
+        <v>36.150000000000098</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C108" s="13"/>
       <c r="D108" s="15"/>
@@ -4482,10 +4575,10 @@
     </row>
     <row r="109" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="16">
-        <v>36.1400000000001</v>
+        <v>36.160000000000103</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C109" s="13"/>
       <c r="D109" s="15"/>
@@ -4505,15 +4598,15 @@
     </row>
     <row r="110" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="16">
-        <v>36.150000000000098</v>
+        <v>36.170000000000101</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C110" s="13"/>
-      <c r="D110" s="15"/>
-      <c r="E110" s="8"/>
-      <c r="F110" s="9"/>
+        <v>96</v>
+      </c>
+      <c r="C110" s="11"/>
+      <c r="D110" s="4"/>
+      <c r="E110" s="5"/>
+      <c r="F110" s="6"/>
       <c r="G110" s="7"/>
       <c r="H110" s="8"/>
       <c r="I110" s="8"/>
@@ -4521,56 +4614,10 @@
       <c r="K110" s="8"/>
       <c r="L110" s="8"/>
       <c r="M110" s="9"/>
-      <c r="N110" s="7"/>
-      <c r="O110" s="8"/>
-      <c r="P110" s="8"/>
-      <c r="Q110" s="9"/>
-    </row>
-    <row r="111" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="16">
-        <v>36.160000000000103</v>
-      </c>
-      <c r="B111" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C111" s="13"/>
-      <c r="D111" s="15"/>
-      <c r="E111" s="8"/>
-      <c r="F111" s="9"/>
-      <c r="G111" s="7"/>
-      <c r="H111" s="8"/>
-      <c r="I111" s="8"/>
-      <c r="J111" s="8"/>
-      <c r="K111" s="8"/>
-      <c r="L111" s="8"/>
-      <c r="M111" s="9"/>
-      <c r="N111" s="7"/>
-      <c r="O111" s="8"/>
-      <c r="P111" s="8"/>
-      <c r="Q111" s="9"/>
-    </row>
-    <row r="112" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="16">
-        <v>36.170000000000101</v>
-      </c>
-      <c r="B112" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C112" s="11"/>
-      <c r="D112" s="4"/>
-      <c r="E112" s="5"/>
-      <c r="F112" s="6"/>
-      <c r="G112" s="7"/>
-      <c r="H112" s="8"/>
-      <c r="I112" s="8"/>
-      <c r="J112" s="8"/>
-      <c r="K112" s="8"/>
-      <c r="L112" s="8"/>
-      <c r="M112" s="9"/>
-      <c r="N112" s="4"/>
-      <c r="O112" s="5"/>
-      <c r="P112" s="5"/>
-      <c r="Q112" s="6"/>
+      <c r="N110" s="4"/>
+      <c r="O110" s="5"/>
+      <c r="P110" s="5"/>
+      <c r="Q110" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Adding details about merge sort
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bharat/bctci/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4495B81F-01FB-6144-883A-E6FEE7682D4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95CD0202-F0DE-B643-8C9A-E7C2FA8998A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{233FF15D-0BCB-6B46-B450-599851EED7C1}"/>
   </bookViews>
@@ -1449,9 +1449,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4095FB6B-33CD-C94D-A3B2-EAADF58B3AE5}">
   <dimension ref="A1:Q110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P30" sqref="P30"/>
+      <selection pane="bottomLeft" activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Trees first warmup execise
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bharat/bctci/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{411F6C4C-F346-5849-8C06-FE586919D65A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD5D5B0-B092-5047-B9EF-31C899700698}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{233FF15D-0BCB-6B46-B450-599851EED7C1}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="273">
   <si>
     <t>Sets &amp; Maps</t>
   </si>
@@ -840,6 +840,24 @@
   </si>
   <si>
     <t>Tough problem. Plus, found a bug!</t>
+  </si>
+  <si>
+    <t>Recursive height and size went better than expected! Worked on first shot.</t>
+  </si>
+  <si>
+    <t>Some things like putting left and right child in an array to reduce code repetition</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Pretty perfect</t>
+  </si>
+  <si>
+    <t>Good progress</t>
+  </si>
+  <si>
+    <t>0 height for null, 0 level for root</t>
   </si>
 </sst>
 </file>
@@ -1503,9 +1521,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4095FB6B-33CD-C94D-A3B2-EAADF58B3AE5}">
   <dimension ref="A1:Q110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K35" sqref="K35"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3141,17 +3159,37 @@
       <c r="B39" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C39" s="13"/>
-      <c r="D39" s="15"/>
-      <c r="E39" s="8"/>
+      <c r="C39" s="13" t="s">
+        <v>267</v>
+      </c>
+      <c r="D39" s="15">
+        <v>45875</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>125</v>
+      </c>
       <c r="F39" s="9"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="8"/>
-      <c r="I39" s="8"/>
-      <c r="J39" s="8"/>
-      <c r="K39" s="8"/>
-      <c r="L39" s="8"/>
-      <c r="M39" s="9"/>
+      <c r="G39" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="H39" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="I39" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="J39" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="K39" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="L39" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="M39" s="9" t="s">
+        <v>272</v>
+      </c>
       <c r="N39" s="7"/>
       <c r="O39" s="8"/>
       <c r="P39" s="8"/>

</xml_diff>

<commit_message>
Wrapping up tree warmup problems
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bharat/bctci/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD5D5B0-B092-5047-B9EF-31C899700698}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F9F435B-103D-F544-A871-4CE178D5EBB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{233FF15D-0BCB-6B46-B450-599851EED7C1}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="278">
   <si>
     <t>Sets &amp; Maps</t>
   </si>
@@ -858,6 +858,21 @@
   </si>
   <si>
     <t>0 height for null, 0 level for root</t>
+  </si>
+  <si>
+    <t>Recursive ancestors solution, while book had iterative solution. For LCA problem, I had a similar concept, found ancestors and iterated throught them.</t>
+  </si>
+  <si>
+    <t>Missed the two pointer solution for LCA, which was similar but I guess I'm not as comfortable with node manipulation: perhaps consider more iterative options</t>
+  </si>
+  <si>
+    <t>Don’t know</t>
+  </si>
+  <si>
+    <t>Pretty good recursion actually</t>
+  </si>
+  <si>
+    <t>Two pointer solution for LCA</t>
   </si>
 </sst>
 </file>
@@ -1521,9 +1536,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4095FB6B-33CD-C94D-A3B2-EAADF58B3AE5}">
   <dimension ref="A1:Q110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M39" sqref="M39"/>
+      <selection pane="bottomLeft" activeCell="O39" sqref="O39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3152,7 +3167,7 @@
       <c r="P38" s="8"/>
       <c r="Q38" s="9"/>
     </row>
-    <row r="39" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="18">
         <v>35.000999999999998</v>
       </c>
@@ -3168,7 +3183,9 @@
       <c r="E39" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="F39" s="9"/>
+      <c r="F39" s="9" t="s">
+        <v>228</v>
+      </c>
       <c r="G39" s="7" t="s">
         <v>268</v>
       </c>
@@ -3190,33 +3207,71 @@
       <c r="M39" s="9" t="s">
         <v>272</v>
       </c>
-      <c r="N39" s="7"/>
-      <c r="O39" s="8"/>
-      <c r="P39" s="8"/>
-      <c r="Q39" s="9"/>
-    </row>
-    <row r="40" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N39" s="7">
+        <v>3</v>
+      </c>
+      <c r="O39" s="8">
+        <v>3</v>
+      </c>
+      <c r="P39" s="8">
+        <v>3</v>
+      </c>
+      <c r="Q39" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" ht="100" x14ac:dyDescent="0.25">
       <c r="A40" s="18">
         <v>35.002000000000002</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C40" s="13"/>
-      <c r="D40" s="15"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="9"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="8"/>
-      <c r="I40" s="8"/>
-      <c r="J40" s="8"/>
-      <c r="K40" s="8"/>
-      <c r="L40" s="8"/>
-      <c r="M40" s="9"/>
-      <c r="N40" s="7"/>
-      <c r="O40" s="8"/>
-      <c r="P40" s="8"/>
-      <c r="Q40" s="9"/>
+      <c r="C40" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="D40" s="15">
+        <v>45875</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="H40" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="I40" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="J40" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="K40" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="L40" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="M40" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="N40" s="7">
+        <v>3</v>
+      </c>
+      <c r="O40" s="8">
+        <v>4</v>
+      </c>
+      <c r="P40" s="8">
+        <v>3</v>
+      </c>
+      <c r="Q40" s="9">
+        <v>3</v>
+      </c>
     </row>
     <row r="41" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="16">

</xml_diff>

<commit_message>
Finishing aligned chain problem
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bharat/bctci/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F9F435B-103D-F544-A871-4CE178D5EBB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFE36276-D32A-C846-9C13-95A1CF18BA76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{233FF15D-0BCB-6B46-B450-599851EED7C1}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="285">
   <si>
     <t>Sets &amp; Maps</t>
   </si>
@@ -873,6 +873,27 @@
   </si>
   <si>
     <t>Two pointer solution for LCA</t>
+  </si>
+  <si>
+    <t>I was pretty close to the solution in terms of my pattern, but couldn't figure algorithm out</t>
+  </si>
+  <si>
+    <t>The idea that the result value of recursive function had to be what I was keeping track of, ie max aligned chain length</t>
+  </si>
+  <si>
+    <t>I chose wrong order of traversal. I was close to going to postorder, but chose to go with inorder instead</t>
+  </si>
+  <si>
+    <t>Recursion return value when using a helper</t>
+  </si>
+  <si>
+    <t>declaring nonlocal when assigning a variable inside recursive function</t>
+  </si>
+  <si>
+    <t>Decent, need to do this problem again</t>
+  </si>
+  <si>
+    <t>nonlocal</t>
   </si>
 </sst>
 </file>
@@ -1538,7 +1559,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O39" sqref="O39"/>
+      <selection pane="bottomLeft" activeCell="R41" sqref="R41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3273,28 +3294,58 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" ht="100" x14ac:dyDescent="0.25">
       <c r="A41" s="16">
         <v>35.01</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C41" s="13"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="9"/>
-      <c r="G41" s="7"/>
-      <c r="H41" s="8"/>
-      <c r="I41" s="8"/>
-      <c r="J41" s="8"/>
-      <c r="K41" s="8"/>
-      <c r="L41" s="8"/>
-      <c r="M41" s="9"/>
-      <c r="N41" s="7"/>
-      <c r="O41" s="8"/>
-      <c r="P41" s="8"/>
-      <c r="Q41" s="9"/>
+      <c r="C41" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="D41" s="15">
+        <v>45876</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="F41" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="G41" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="H41" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="I41" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="J41" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="K41" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="L41" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="M41" s="9" t="s">
+        <v>284</v>
+      </c>
+      <c r="N41" s="7">
+        <v>2</v>
+      </c>
+      <c r="O41" s="8">
+        <v>2</v>
+      </c>
+      <c r="P41" s="8">
+        <v>2</v>
+      </c>
+      <c r="Q41" s="9">
+        <v>3</v>
+      </c>
     </row>
     <row r="42" spans="1:17" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="16">

</xml_diff>

<commit_message>
Two more DFS tree problems
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bharat/bctci/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04DB905B-7392-0F49-A269-77F3897E6FC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0138F2B9-0A7C-8A4C-AE03-4ED59100DF36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15120" xr2:uid="{233FF15D-0BCB-6B46-B450-599851EED7C1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{233FF15D-0BCB-6B46-B450-599851EED7C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="309">
   <si>
     <t>Sets &amp; Maps</t>
   </si>
@@ -936,6 +936,36 @@
   </si>
   <si>
     <t>Good attempt, even if failed</t>
+  </si>
+  <si>
+    <t>Keep a dict of coords, append to and find longest value</t>
+  </si>
+  <si>
+    <t>Linear</t>
+  </si>
+  <si>
+    <t>Could have reduced space complexity since values on stack don't matter</t>
+  </si>
+  <si>
+    <t>Need to read the chapter</t>
+  </si>
+  <si>
+    <t>Storing excessive data</t>
+  </si>
+  <si>
+    <t>Need to look at triggers? Come back to this maybe?</t>
+  </si>
+  <si>
+    <t>Tried a simpler problem, looking for triangles of depth 1. Couldn't solve though</t>
+  </si>
+  <si>
+    <t>Couldn't recurse and maintain multi-node information. Also, left-left-left and corresponding right stumped me</t>
+  </si>
+  <si>
+    <t>Not so much triggers, as a clean understanding of DFS recursion paths</t>
+  </si>
+  <si>
+    <t>Good that I didn't waste too much time when I wasn't making headway -- instead choosing to spend time on understanding solution</t>
   </si>
 </sst>
 </file>
@@ -1233,6 +1263,12 @@
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1262,12 +1298,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1606,8 +1636,8 @@
   <dimension ref="A1:S110"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q43" sqref="Q43"/>
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R45" sqref="R45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1694,28 +1724,28 @@
       <c r="C2" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="29" t="s">
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="G2" s="27"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="26" t="s">
+      <c r="G2" s="29"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="26" t="s">
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="Q2" s="27"/>
-      <c r="R2" s="27"/>
-      <c r="S2" s="28"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="30"/>
     </row>
     <row r="3" spans="1:19" s="8" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14">
@@ -3108,35 +3138,35 @@
       <c r="B32" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="31" t="s">
+      <c r="C32" s="33" t="s">
         <v>254</v>
       </c>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
-      <c r="F32" s="32">
+      <c r="F32" s="34">
         <v>45871</v>
       </c>
-      <c r="G32" s="33" t="s">
+      <c r="G32" s="35" t="s">
         <v>255</v>
       </c>
-      <c r="H32" s="34" t="s">
+      <c r="H32" s="36" t="s">
         <v>255</v>
       </c>
-      <c r="I32" s="35" t="s">
+      <c r="I32" s="37" t="s">
         <v>256</v>
       </c>
-      <c r="J32" s="33"/>
-      <c r="K32" s="33"/>
-      <c r="L32" s="33"/>
-      <c r="M32" s="33"/>
-      <c r="N32" s="33"/>
-      <c r="O32" s="34"/>
-      <c r="P32" s="35">
+      <c r="J32" s="35"/>
+      <c r="K32" s="35"/>
+      <c r="L32" s="35"/>
+      <c r="M32" s="35"/>
+      <c r="N32" s="35"/>
+      <c r="O32" s="36"/>
+      <c r="P32" s="37">
         <v>2</v>
       </c>
-      <c r="Q32" s="33"/>
-      <c r="R32" s="33"/>
-      <c r="S32" s="34"/>
+      <c r="Q32" s="35"/>
+      <c r="R32" s="35"/>
+      <c r="S32" s="36"/>
     </row>
     <row r="33" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="17">
@@ -3145,23 +3175,23 @@
       <c r="B33" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="31"/>
+      <c r="C33" s="33"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
-      <c r="F33" s="32"/>
-      <c r="G33" s="33"/>
-      <c r="H33" s="34"/>
-      <c r="I33" s="35"/>
-      <c r="J33" s="33"/>
-      <c r="K33" s="33"/>
-      <c r="L33" s="33"/>
-      <c r="M33" s="33"/>
-      <c r="N33" s="33"/>
-      <c r="O33" s="34"/>
-      <c r="P33" s="35"/>
-      <c r="Q33" s="33"/>
-      <c r="R33" s="33"/>
-      <c r="S33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="35"/>
+      <c r="H33" s="36"/>
+      <c r="I33" s="37"/>
+      <c r="J33" s="35"/>
+      <c r="K33" s="35"/>
+      <c r="L33" s="35"/>
+      <c r="M33" s="35"/>
+      <c r="N33" s="35"/>
+      <c r="O33" s="36"/>
+      <c r="P33" s="37"/>
+      <c r="Q33" s="35"/>
+      <c r="R33" s="35"/>
+      <c r="S33" s="36"/>
     </row>
     <row r="34" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="16">
@@ -3597,55 +3627,123 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A44" s="16">
         <v>35.04</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C44" s="13"/>
-      <c r="D44" s="7"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="15"/>
-      <c r="G44" s="8"/>
-      <c r="H44" s="9"/>
-      <c r="I44" s="7"/>
-      <c r="J44" s="8"/>
-      <c r="K44" s="8"/>
-      <c r="L44" s="8"/>
-      <c r="M44" s="8"/>
-      <c r="N44" s="8"/>
-      <c r="O44" s="9"/>
-      <c r="P44" s="7"/>
-      <c r="Q44" s="8"/>
-      <c r="R44" s="8"/>
-      <c r="S44" s="9"/>
-    </row>
-    <row r="45" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C44" s="13" t="s">
+        <v>299</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="F44" s="15">
+        <v>45882</v>
+      </c>
+      <c r="G44" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="H44" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="I44" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="J44" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="K44" s="8" t="s">
+        <v>302</v>
+      </c>
+      <c r="L44" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="M44" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="N44" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="O44" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="P44" s="7">
+        <v>4</v>
+      </c>
+      <c r="Q44" s="8">
+        <v>4</v>
+      </c>
+      <c r="R44" s="8">
+        <v>4</v>
+      </c>
+      <c r="S44" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" ht="120" x14ac:dyDescent="0.25">
       <c r="A45" s="16">
         <v>35.049999999999997</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C45" s="13"/>
-      <c r="D45" s="7"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="15"/>
-      <c r="G45" s="8"/>
-      <c r="H45" s="9"/>
-      <c r="I45" s="7"/>
-      <c r="J45" s="8"/>
-      <c r="K45" s="8"/>
-      <c r="L45" s="8"/>
-      <c r="M45" s="8"/>
-      <c r="N45" s="8"/>
-      <c r="O45" s="9"/>
-      <c r="P45" s="7"/>
-      <c r="Q45" s="8"/>
-      <c r="R45" s="8"/>
-      <c r="S45" s="9"/>
+      <c r="C45" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="F45" s="15">
+        <v>45882</v>
+      </c>
+      <c r="G45" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="H45" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="I45" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="J45" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="K45" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="L45" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="M45" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="N45" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="O45" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="P45" s="7">
+        <v>2</v>
+      </c>
+      <c r="Q45" s="8">
+        <v>2</v>
+      </c>
+      <c r="R45" s="8">
+        <v>2</v>
+      </c>
+      <c r="S45" s="9">
+        <v>2</v>
+      </c>
     </row>
     <row r="46" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="16">
@@ -5194,8 +5292,8 @@
         <v>96</v>
       </c>
       <c r="C110" s="11"/>
-      <c r="D110" s="37"/>
-      <c r="E110" s="37"/>
+      <c r="D110" s="27"/>
+      <c r="E110" s="27"/>
       <c r="F110" s="4"/>
       <c r="G110" s="5"/>
       <c r="H110" s="6"/>

</xml_diff>

<commit_message>
Wrapping up binary trees
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bharat/bctci/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0138F2B9-0A7C-8A4C-AE03-4ED59100DF36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4691171-7D1A-3341-9A5E-424027B3BA06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{233FF15D-0BCB-6B46-B450-599851EED7C1}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="319">
   <si>
     <t>Sets &amp; Maps</t>
   </si>
@@ -966,6 +966,36 @@
   </si>
   <si>
     <t>Good that I didn't waste too much time when I wasn't making headway -- instead choosing to spend time on understanding solution</t>
+  </si>
+  <si>
+    <t>Recursive solution, swapping left and right subtrees on the way up</t>
+  </si>
+  <si>
+    <t>Linear, visit each node once</t>
+  </si>
+  <si>
+    <t>Call stack</t>
+  </si>
+  <si>
+    <t>Started with subtree, and kept reversing node till solution</t>
+  </si>
+  <si>
+    <t>Almost the same solution as book</t>
+  </si>
+  <si>
+    <t>Linear, number of nodes</t>
+  </si>
+  <si>
+    <t>Call stack height</t>
+  </si>
+  <si>
+    <t>Bottom-up, evaluate based on kind of node</t>
+  </si>
+  <si>
+    <t>All good</t>
+  </si>
+  <si>
+    <t>Either memorise math.prod or keep a helper function handy</t>
   </si>
 </sst>
 </file>
@@ -1637,7 +1667,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R45" sqref="R45"/>
+      <selection pane="bottomLeft" activeCell="T47" sqref="T47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3745,55 +3775,123 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A46" s="16">
         <v>35.06</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C46" s="13"/>
-      <c r="D46" s="7"/>
-      <c r="E46" s="7"/>
-      <c r="F46" s="15"/>
-      <c r="G46" s="8"/>
-      <c r="H46" s="9"/>
-      <c r="I46" s="7"/>
-      <c r="J46" s="8"/>
-      <c r="K46" s="8"/>
-      <c r="L46" s="8"/>
-      <c r="M46" s="8"/>
-      <c r="N46" s="8"/>
-      <c r="O46" s="9"/>
-      <c r="P46" s="7"/>
-      <c r="Q46" s="8"/>
-      <c r="R46" s="8"/>
-      <c r="S46" s="9"/>
-    </row>
-    <row r="47" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C46" s="13" t="s">
+        <v>309</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="F46" s="15">
+        <v>45883</v>
+      </c>
+      <c r="G46" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="H46" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="I46" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="J46" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="K46" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="L46" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="M46" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="N46" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="O46" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="P46" s="7">
+        <v>4</v>
+      </c>
+      <c r="Q46" s="8">
+        <v>4</v>
+      </c>
+      <c r="R46" s="8">
+        <v>4</v>
+      </c>
+      <c r="S46" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A47" s="16">
         <v>35.07</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C47" s="13"/>
-      <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="15"/>
-      <c r="G47" s="8"/>
-      <c r="H47" s="9"/>
-      <c r="I47" s="7"/>
-      <c r="J47" s="8"/>
-      <c r="K47" s="8"/>
-      <c r="L47" s="8"/>
-      <c r="M47" s="8"/>
-      <c r="N47" s="8"/>
-      <c r="O47" s="9"/>
-      <c r="P47" s="7"/>
-      <c r="Q47" s="8"/>
-      <c r="R47" s="8"/>
-      <c r="S47" s="9"/>
+      <c r="C47" s="13" t="s">
+        <v>316</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="F47" s="15">
+        <v>45883</v>
+      </c>
+      <c r="G47" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="H47" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="I47" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="J47" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="K47" s="8" t="s">
+        <v>317</v>
+      </c>
+      <c r="L47" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="M47" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="N47" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="O47" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="P47" s="7">
+        <v>4</v>
+      </c>
+      <c r="Q47" s="8">
+        <v>4</v>
+      </c>
+      <c r="R47" s="8">
+        <v>4</v>
+      </c>
+      <c r="S47" s="9">
+        <v>4</v>
+      </c>
     </row>
     <row r="48" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="16">

</xml_diff>

<commit_message>
First three BFS problems
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bharat/bctci/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4691171-7D1A-3341-9A5E-424027B3BA06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A040D849-7C64-EE43-85FA-55D1C3E39588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{233FF15D-0BCB-6B46-B450-599851EED7C1}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="327">
   <si>
     <t>Sets &amp; Maps</t>
   </si>
@@ -996,6 +996,30 @@
   </si>
   <si>
     <t>Either memorise math.prod or keep a helper function handy</t>
+  </si>
+  <si>
+    <t>BFS, keep set for seen levels, if not in set append to result array</t>
+  </si>
+  <si>
+    <t>Good BFS practice</t>
+  </si>
+  <si>
+    <t>Map that tracks members and children of every level, and then process that map</t>
+  </si>
+  <si>
+    <t>Linear (Queue is linear worst case scenario)</t>
+  </si>
+  <si>
+    <t>Almost correct, but did some repetitive work</t>
+  </si>
+  <si>
+    <t>I did keep track of current level in an array, and appended as level changed, but did some extra work</t>
+  </si>
+  <si>
+    <t>Need to review</t>
+  </si>
+  <si>
+    <t>Almost correct, perhaps not in the best mood to do the problem</t>
   </si>
 </sst>
 </file>
@@ -1226,7 +1250,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1327,6 +1351,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1666,8 +1693,8 @@
   <dimension ref="A1:S110"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T47" sqref="T47"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T50" sqref="T50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3893,80 +3920,166 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" ht="100" x14ac:dyDescent="0.25">
       <c r="A48" s="16">
         <v>35.08</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C48" s="13"/>
-      <c r="D48" s="7"/>
-      <c r="E48" s="7"/>
-      <c r="F48" s="15"/>
-      <c r="G48" s="8"/>
-      <c r="H48" s="9"/>
-      <c r="I48" s="7"/>
-      <c r="J48" s="8"/>
-      <c r="K48" s="8"/>
-      <c r="L48" s="8"/>
-      <c r="M48" s="8"/>
-      <c r="N48" s="8"/>
-      <c r="O48" s="9"/>
-      <c r="P48" s="7"/>
-      <c r="Q48" s="8"/>
-      <c r="R48" s="8"/>
-      <c r="S48" s="9"/>
-    </row>
-    <row r="49" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C48" s="13" t="s">
+        <v>319</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="F48" s="15">
+        <v>45884</v>
+      </c>
+      <c r="G48" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="H48" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="I48" s="37" t="s">
+        <v>317</v>
+      </c>
+      <c r="J48" s="38"/>
+      <c r="K48" s="38"/>
+      <c r="L48" s="38"/>
+      <c r="M48" s="38"/>
+      <c r="N48" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="O48" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="P48" s="7">
+        <v>4</v>
+      </c>
+      <c r="Q48" s="8">
+        <v>4</v>
+      </c>
+      <c r="R48" s="8">
+        <v>4</v>
+      </c>
+      <c r="S48" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A49" s="16">
         <v>35.090000000000003</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C49" s="13"/>
-      <c r="D49" s="7"/>
-      <c r="E49" s="7"/>
-      <c r="F49" s="15"/>
-      <c r="G49" s="8"/>
-      <c r="H49" s="9"/>
-      <c r="I49" s="7"/>
-      <c r="J49" s="8"/>
-      <c r="K49" s="8"/>
-      <c r="L49" s="8"/>
-      <c r="M49" s="8"/>
-      <c r="N49" s="8"/>
-      <c r="O49" s="9"/>
-      <c r="P49" s="7"/>
-      <c r="Q49" s="8"/>
-      <c r="R49" s="8"/>
-      <c r="S49" s="9"/>
-    </row>
-    <row r="50" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C49" s="13" t="s">
+        <v>321</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="F49" s="15">
+        <v>45884</v>
+      </c>
+      <c r="G49" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="H49" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="I49" s="37" t="s">
+        <v>317</v>
+      </c>
+      <c r="J49" s="38"/>
+      <c r="K49" s="38"/>
+      <c r="L49" s="38"/>
+      <c r="M49" s="38"/>
+      <c r="N49" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="O49" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="P49" s="7">
+        <v>4</v>
+      </c>
+      <c r="Q49" s="8">
+        <v>3</v>
+      </c>
+      <c r="R49" s="8">
+        <v>4</v>
+      </c>
+      <c r="S49" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A50" s="16">
         <v>35.1</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C50" s="13"/>
-      <c r="D50" s="7"/>
-      <c r="E50" s="7"/>
-      <c r="F50" s="15"/>
-      <c r="G50" s="8"/>
-      <c r="H50" s="9"/>
-      <c r="I50" s="7"/>
-      <c r="J50" s="8"/>
-      <c r="K50" s="8"/>
-      <c r="L50" s="8"/>
-      <c r="M50" s="8"/>
-      <c r="N50" s="8"/>
-      <c r="O50" s="9"/>
-      <c r="P50" s="7"/>
-      <c r="Q50" s="8"/>
-      <c r="R50" s="8"/>
-      <c r="S50" s="9"/>
+      <c r="C50" s="13" t="s">
+        <v>323</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="F50" s="15">
+        <v>45884</v>
+      </c>
+      <c r="G50" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="H50" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="I50" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="J50" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="K50" s="8" t="s">
+        <v>325</v>
+      </c>
+      <c r="L50" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="M50" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="N50" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="O50" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="P50" s="7">
+        <v>2</v>
+      </c>
+      <c r="Q50" s="8">
+        <v>2</v>
+      </c>
+      <c r="R50" s="8">
+        <v>2</v>
+      </c>
+      <c r="S50" s="9">
+        <v>2</v>
+      </c>
     </row>
     <row r="51" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="16">
@@ -5408,7 +5521,9 @@
       <c r="S110" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="11">
+    <mergeCell ref="I48:M48"/>
+    <mergeCell ref="I49:M49"/>
     <mergeCell ref="P2:S2"/>
     <mergeCell ref="F2:H2"/>
     <mergeCell ref="I2:O2"/>

</xml_diff>

<commit_message>
Wrapping up dfs and starting bst
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bharat/bctci/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A040D849-7C64-EE43-85FA-55D1C3E39588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F40797CA-A416-6349-9ED4-FD60EB4412AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{233FF15D-0BCB-6B46-B450-599851EED7C1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24380" windowHeight="16000" xr2:uid="{233FF15D-0BCB-6B46-B450-599851EED7C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="337">
   <si>
     <t>Sets &amp; Maps</t>
   </si>
@@ -1020,6 +1021,36 @@
   </si>
   <si>
     <t>Almost correct, perhaps not in the best mood to do the problem</t>
+  </si>
+  <si>
+    <t>First DFS and then DFS. Struggled with BFS because of malformed test case, but persisted with logic rather than hack and slash</t>
+  </si>
+  <si>
+    <t>Good problem, chose to stop at the right time.</t>
+  </si>
+  <si>
+    <t>Look at len(q) approach to keep tracking of levels when doing BFS</t>
+  </si>
+  <si>
+    <t>I came up with a recursive solution, but messed around comparing current with left, when I should have compared current with target</t>
+  </si>
+  <si>
+    <t>Height of tree</t>
+  </si>
+  <si>
+    <t>Height of stack, linear for skewed tree</t>
+  </si>
+  <si>
+    <t>Recursive felt more intuitive</t>
+  </si>
+  <si>
+    <t>No, but close</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Good start</t>
   </si>
 </sst>
 </file>
@@ -1029,7 +1060,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1073,6 +1104,24 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -1250,7 +1299,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1323,20 +1372,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1353,8 +1406,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1694,7 +1759,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T50" sqref="T50"/>
+      <selection pane="bottomLeft" activeCell="N52" sqref="N52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1783,26 +1848,26 @@
       </c>
       <c r="D2" s="26"/>
       <c r="E2" s="26"/>
-      <c r="F2" s="31" t="s">
+      <c r="F2" s="43" t="s">
         <v>112</v>
       </c>
-      <c r="G2" s="29"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="28" t="s">
+      <c r="G2" s="41"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="28" t="s">
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="41"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="40" t="s">
         <v>111</v>
       </c>
-      <c r="Q2" s="29"/>
-      <c r="R2" s="29"/>
-      <c r="S2" s="30"/>
+      <c r="Q2" s="41"/>
+      <c r="R2" s="41"/>
+      <c r="S2" s="42"/>
     </row>
     <row r="3" spans="1:19" s="8" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14">
@@ -3195,35 +3260,35 @@
       <c r="B32" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="33" t="s">
+      <c r="C32" s="35" t="s">
         <v>254</v>
       </c>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
-      <c r="F32" s="34">
+      <c r="F32" s="36">
         <v>45871</v>
       </c>
-      <c r="G32" s="35" t="s">
+      <c r="G32" s="37" t="s">
         <v>255</v>
       </c>
-      <c r="H32" s="36" t="s">
+      <c r="H32" s="38" t="s">
         <v>255</v>
       </c>
-      <c r="I32" s="37" t="s">
+      <c r="I32" s="39" t="s">
         <v>256</v>
       </c>
-      <c r="J32" s="35"/>
-      <c r="K32" s="35"/>
-      <c r="L32" s="35"/>
-      <c r="M32" s="35"/>
-      <c r="N32" s="35"/>
-      <c r="O32" s="36"/>
-      <c r="P32" s="37">
+      <c r="J32" s="37"/>
+      <c r="K32" s="37"/>
+      <c r="L32" s="37"/>
+      <c r="M32" s="37"/>
+      <c r="N32" s="37"/>
+      <c r="O32" s="38"/>
+      <c r="P32" s="39">
         <v>2</v>
       </c>
-      <c r="Q32" s="35"/>
-      <c r="R32" s="35"/>
-      <c r="S32" s="36"/>
+      <c r="Q32" s="37"/>
+      <c r="R32" s="37"/>
+      <c r="S32" s="38"/>
     </row>
     <row r="33" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="17">
@@ -3232,23 +3297,23 @@
       <c r="B33" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="33"/>
+      <c r="C33" s="35"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
-      <c r="F33" s="34"/>
-      <c r="G33" s="35"/>
-      <c r="H33" s="36"/>
-      <c r="I33" s="37"/>
-      <c r="J33" s="35"/>
-      <c r="K33" s="35"/>
-      <c r="L33" s="35"/>
-      <c r="M33" s="35"/>
-      <c r="N33" s="35"/>
-      <c r="O33" s="36"/>
-      <c r="P33" s="37"/>
-      <c r="Q33" s="35"/>
-      <c r="R33" s="35"/>
-      <c r="S33" s="36"/>
+      <c r="F33" s="36"/>
+      <c r="G33" s="37"/>
+      <c r="H33" s="38"/>
+      <c r="I33" s="39"/>
+      <c r="J33" s="37"/>
+      <c r="K33" s="37"/>
+      <c r="L33" s="37"/>
+      <c r="M33" s="37"/>
+      <c r="N33" s="37"/>
+      <c r="O33" s="38"/>
+      <c r="P33" s="39"/>
+      <c r="Q33" s="37"/>
+      <c r="R33" s="37"/>
+      <c r="S33" s="38"/>
     </row>
     <row r="34" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="16">
@@ -3945,13 +4010,13 @@
       <c r="H48" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="I48" s="37" t="s">
+      <c r="I48" s="39" t="s">
         <v>317</v>
       </c>
-      <c r="J48" s="38"/>
-      <c r="K48" s="38"/>
-      <c r="L48" s="38"/>
-      <c r="M48" s="38"/>
+      <c r="J48" s="37"/>
+      <c r="K48" s="37"/>
+      <c r="L48" s="37"/>
+      <c r="M48" s="37"/>
       <c r="N48" s="8" t="s">
         <v>320</v>
       </c>
@@ -3996,13 +4061,13 @@
       <c r="H49" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="I49" s="37" t="s">
+      <c r="I49" s="39" t="s">
         <v>317</v>
       </c>
-      <c r="J49" s="38"/>
-      <c r="K49" s="38"/>
-      <c r="L49" s="38"/>
-      <c r="M49" s="38"/>
+      <c r="J49" s="37"/>
+      <c r="K49" s="37"/>
+      <c r="L49" s="37"/>
+      <c r="M49" s="37"/>
       <c r="N49" s="8" t="s">
         <v>320</v>
       </c>
@@ -4081,55 +4146,115 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" ht="80" x14ac:dyDescent="0.25">
       <c r="A51" s="16">
         <v>35.11</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C51" s="13"/>
-      <c r="D51" s="7"/>
-      <c r="E51" s="7"/>
-      <c r="F51" s="15"/>
-      <c r="G51" s="8"/>
-      <c r="H51" s="9"/>
-      <c r="I51" s="7"/>
-      <c r="J51" s="8"/>
-      <c r="K51" s="8"/>
-      <c r="L51" s="8"/>
-      <c r="M51" s="8"/>
-      <c r="N51" s="8"/>
-      <c r="O51" s="9"/>
-      <c r="P51" s="7"/>
-      <c r="Q51" s="8"/>
-      <c r="R51" s="8"/>
-      <c r="S51" s="9"/>
-    </row>
-    <row r="52" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C51" s="13" t="s">
+        <v>327</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="F51" s="15">
+        <v>45885</v>
+      </c>
+      <c r="G51" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="H51" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="I51" s="39" t="s">
+        <v>317</v>
+      </c>
+      <c r="J51" s="37"/>
+      <c r="K51" s="37"/>
+      <c r="L51" s="37"/>
+      <c r="M51" s="37"/>
+      <c r="N51" s="8" t="s">
+        <v>328</v>
+      </c>
+      <c r="O51" s="9" t="s">
+        <v>329</v>
+      </c>
+      <c r="P51" s="7">
+        <v>4</v>
+      </c>
+      <c r="Q51" s="8">
+        <v>4</v>
+      </c>
+      <c r="R51" s="8">
+        <v>4</v>
+      </c>
+      <c r="S51" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" ht="80" x14ac:dyDescent="0.25">
       <c r="A52" s="16">
         <v>35.120000000000097</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C52" s="13"/>
-      <c r="D52" s="7"/>
-      <c r="E52" s="7"/>
-      <c r="F52" s="15"/>
-      <c r="G52" s="8"/>
-      <c r="H52" s="9"/>
-      <c r="I52" s="7"/>
-      <c r="J52" s="8"/>
-      <c r="K52" s="8"/>
-      <c r="L52" s="8"/>
-      <c r="M52" s="8"/>
-      <c r="N52" s="8"/>
-      <c r="O52" s="9"/>
-      <c r="P52" s="7"/>
-      <c r="Q52" s="8"/>
-      <c r="R52" s="8"/>
-      <c r="S52" s="9"/>
+      <c r="C52" s="13" t="s">
+        <v>330</v>
+      </c>
+      <c r="D52" s="7" t="s">
+        <v>331</v>
+      </c>
+      <c r="E52" s="7" t="s">
+        <v>332</v>
+      </c>
+      <c r="F52" s="15">
+        <v>45885</v>
+      </c>
+      <c r="G52" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="H52" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="I52" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="J52" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="K52" s="8" t="s">
+        <v>335</v>
+      </c>
+      <c r="L52" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="M52" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="N52" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="O52" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="P52" s="7">
+        <v>3</v>
+      </c>
+      <c r="Q52" s="8">
+        <v>3</v>
+      </c>
+      <c r="R52" s="8">
+        <v>3</v>
+      </c>
+      <c r="S52" s="9">
+        <v>3</v>
+      </c>
     </row>
     <row r="53" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="16">
@@ -5521,18 +5646,19 @@
       <c r="S110" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
+    <mergeCell ref="I51:M51"/>
     <mergeCell ref="I48:M48"/>
     <mergeCell ref="I49:M49"/>
     <mergeCell ref="P2:S2"/>
     <mergeCell ref="F2:H2"/>
     <mergeCell ref="I2:O2"/>
+    <mergeCell ref="P32:S33"/>
     <mergeCell ref="C32:C33"/>
     <mergeCell ref="F32:F33"/>
     <mergeCell ref="G32:G33"/>
     <mergeCell ref="H32:H33"/>
     <mergeCell ref="I32:O33"/>
-    <mergeCell ref="P32:S33"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
@@ -5540,6 +5666,273 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3F5BAA8-64A3-1E43-8E2B-777FEA4D7477}">
+  <dimension ref="A1:C29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.6640625" style="28" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="29"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="31"/>
+      <c r="B1" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="32"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="33">
+        <v>1</v>
+      </c>
+      <c r="B2" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="32"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="33">
+        <v>2</v>
+      </c>
+      <c r="B3" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="32"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="33">
+        <v>3</v>
+      </c>
+      <c r="B4" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="32"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="33">
+        <v>4</v>
+      </c>
+      <c r="B5" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="32"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="33">
+        <v>5</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="32"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="33">
+        <v>6</v>
+      </c>
+      <c r="B7" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="32"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="31"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="32"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="31"/>
+      <c r="B9" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="32"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="31">
+        <v>39.01</v>
+      </c>
+      <c r="B10" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="32"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="31">
+        <v>39.020000000000003</v>
+      </c>
+      <c r="B11" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="32"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="31">
+        <v>39.03</v>
+      </c>
+      <c r="B12" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="32"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="31">
+        <v>39.04</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="32"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="31">
+        <v>39.049999999999997</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" s="32"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="31">
+        <v>39.06</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="32"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="31">
+        <v>39.07</v>
+      </c>
+      <c r="B16" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="32"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="31">
+        <v>39.08</v>
+      </c>
+      <c r="B17" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="32"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="31">
+        <v>39.090000000000003</v>
+      </c>
+      <c r="B18" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="32"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="31">
+        <v>39.1</v>
+      </c>
+      <c r="B19" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="32"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="31">
+        <v>39.11</v>
+      </c>
+      <c r="B20" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="32"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="31"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="32"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="31"/>
+      <c r="B22" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="32"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="31">
+        <v>41</v>
+      </c>
+      <c r="B23" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="32"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="31">
+        <v>41.01</v>
+      </c>
+      <c r="B24" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" s="32"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="31">
+        <v>41.02</v>
+      </c>
+      <c r="B25" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" s="32"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="31">
+        <v>41.03</v>
+      </c>
+      <c r="B26" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="C26" s="32"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="31">
+        <v>41.04</v>
+      </c>
+      <c r="B27" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" s="32"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="31">
+        <v>41.05</v>
+      </c>
+      <c r="B28" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="C28" s="32"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="31">
+        <v>41.06</v>
+      </c>
+      <c r="B29" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="C29" s="32"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6E5E05C-FD85-A84F-B5CD-386963B8CD1F}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>

</xml_diff>

<commit_message>
Two more BST problems
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bharat/bctci/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F40797CA-A416-6349-9ED4-FD60EB4412AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0DCA81A-369E-854A-849D-F15348EC0A12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24380" windowHeight="16000" xr2:uid="{233FF15D-0BCB-6B46-B450-599851EED7C1}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="350">
   <si>
     <t>Sets &amp; Maps</t>
   </si>
@@ -1044,13 +1044,52 @@
     <t>Recursive felt more intuitive</t>
   </si>
   <si>
-    <t>No, but close</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
     <t>Good start</t>
+  </si>
+  <si>
+    <t>Keep track of distance of left and right with target, go to the one with lesser distance. Didn't work.</t>
+  </si>
+  <si>
+    <t>No, but close. My space complexity was not constant</t>
+  </si>
+  <si>
+    <t>Constant</t>
+  </si>
+  <si>
+    <t>Should have kept range rather than notion of how close each node is</t>
+  </si>
+  <si>
+    <t>Need to review after questions</t>
+  </si>
+  <si>
+    <t>This was a matter of identifying pattern, hard to say easily where I went wrong</t>
+  </si>
+  <si>
+    <t>Learn to identify when ranges are the way to go</t>
+  </si>
+  <si>
+    <t>Got lost at notion of parent when using inorder traversal</t>
+  </si>
+  <si>
+    <t>No solution</t>
+  </si>
+  <si>
+    <t>Did figure out intuition that with inorder traversal of BST, every subsequent value short be greater than previous one. Also couldn't figure out complex recursion for min-max approach</t>
+  </si>
+  <si>
+    <t>Learn about inorder traversal of BSTs</t>
+  </si>
+  <si>
+    <t>Inorder traversal of bst</t>
+  </si>
+  <si>
+    <t>Hard to say</t>
+  </si>
+  <si>
+    <t>Tricky, should memorise pattern</t>
   </si>
 </sst>
 </file>
@@ -1391,19 +1430,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1420,6 +1450,15 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1757,9 +1796,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4095FB6B-33CD-C94D-A3B2-EAADF58B3AE5}">
   <dimension ref="A1:S110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N52" sqref="N52"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N55" sqref="N55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1848,26 +1887,26 @@
       </c>
       <c r="D2" s="26"/>
       <c r="E2" s="26"/>
-      <c r="F2" s="43" t="s">
+      <c r="F2" s="40" t="s">
         <v>112</v>
       </c>
-      <c r="G2" s="41"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="40" t="s">
+      <c r="G2" s="38"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="37" t="s">
         <v>106</v>
       </c>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="41"/>
-      <c r="O2" s="44"/>
-      <c r="P2" s="40" t="s">
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="41"/>
+      <c r="P2" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="Q2" s="41"/>
-      <c r="R2" s="41"/>
-      <c r="S2" s="42"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="38"/>
+      <c r="S2" s="39"/>
     </row>
     <row r="3" spans="1:19" s="8" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14">
@@ -3260,35 +3299,35 @@
       <c r="B32" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="35" t="s">
+      <c r="C32" s="43" t="s">
         <v>254</v>
       </c>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
-      <c r="F32" s="36">
+      <c r="F32" s="44">
         <v>45871</v>
       </c>
-      <c r="G32" s="37" t="s">
+      <c r="G32" s="36" t="s">
         <v>255</v>
       </c>
-      <c r="H32" s="38" t="s">
+      <c r="H32" s="42" t="s">
         <v>255</v>
       </c>
-      <c r="I32" s="39" t="s">
+      <c r="I32" s="35" t="s">
         <v>256</v>
       </c>
-      <c r="J32" s="37"/>
-      <c r="K32" s="37"/>
-      <c r="L32" s="37"/>
-      <c r="M32" s="37"/>
-      <c r="N32" s="37"/>
-      <c r="O32" s="38"/>
-      <c r="P32" s="39">
+      <c r="J32" s="36"/>
+      <c r="K32" s="36"/>
+      <c r="L32" s="36"/>
+      <c r="M32" s="36"/>
+      <c r="N32" s="36"/>
+      <c r="O32" s="42"/>
+      <c r="P32" s="35">
         <v>2</v>
       </c>
-      <c r="Q32" s="37"/>
-      <c r="R32" s="37"/>
-      <c r="S32" s="38"/>
+      <c r="Q32" s="36"/>
+      <c r="R32" s="36"/>
+      <c r="S32" s="42"/>
     </row>
     <row r="33" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="17">
@@ -3297,23 +3336,23 @@
       <c r="B33" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="35"/>
+      <c r="C33" s="43"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
-      <c r="F33" s="36"/>
-      <c r="G33" s="37"/>
-      <c r="H33" s="38"/>
-      <c r="I33" s="39"/>
-      <c r="J33" s="37"/>
-      <c r="K33" s="37"/>
-      <c r="L33" s="37"/>
-      <c r="M33" s="37"/>
-      <c r="N33" s="37"/>
-      <c r="O33" s="38"/>
-      <c r="P33" s="39"/>
-      <c r="Q33" s="37"/>
-      <c r="R33" s="37"/>
-      <c r="S33" s="38"/>
+      <c r="F33" s="44"/>
+      <c r="G33" s="36"/>
+      <c r="H33" s="42"/>
+      <c r="I33" s="35"/>
+      <c r="J33" s="36"/>
+      <c r="K33" s="36"/>
+      <c r="L33" s="36"/>
+      <c r="M33" s="36"/>
+      <c r="N33" s="36"/>
+      <c r="O33" s="42"/>
+      <c r="P33" s="35"/>
+      <c r="Q33" s="36"/>
+      <c r="R33" s="36"/>
+      <c r="S33" s="42"/>
     </row>
     <row r="34" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="16">
@@ -4010,13 +4049,13 @@
       <c r="H48" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="I48" s="39" t="s">
+      <c r="I48" s="35" t="s">
         <v>317</v>
       </c>
-      <c r="J48" s="37"/>
-      <c r="K48" s="37"/>
-      <c r="L48" s="37"/>
-      <c r="M48" s="37"/>
+      <c r="J48" s="36"/>
+      <c r="K48" s="36"/>
+      <c r="L48" s="36"/>
+      <c r="M48" s="36"/>
       <c r="N48" s="8" t="s">
         <v>320</v>
       </c>
@@ -4061,13 +4100,13 @@
       <c r="H49" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="I49" s="39" t="s">
+      <c r="I49" s="35" t="s">
         <v>317</v>
       </c>
-      <c r="J49" s="37"/>
-      <c r="K49" s="37"/>
-      <c r="L49" s="37"/>
-      <c r="M49" s="37"/>
+      <c r="J49" s="36"/>
+      <c r="K49" s="36"/>
+      <c r="L49" s="36"/>
+      <c r="M49" s="36"/>
       <c r="N49" s="8" t="s">
         <v>320</v>
       </c>
@@ -4171,13 +4210,13 @@
       <c r="H51" s="9" t="s">
         <v>250</v>
       </c>
-      <c r="I51" s="39" t="s">
+      <c r="I51" s="35" t="s">
         <v>317</v>
       </c>
-      <c r="J51" s="37"/>
-      <c r="K51" s="37"/>
-      <c r="L51" s="37"/>
-      <c r="M51" s="37"/>
+      <c r="J51" s="36"/>
+      <c r="K51" s="36"/>
+      <c r="L51" s="36"/>
+      <c r="M51" s="36"/>
       <c r="N51" s="8" t="s">
         <v>328</v>
       </c>
@@ -4226,19 +4265,19 @@
         <v>333</v>
       </c>
       <c r="J52" s="8" t="s">
+        <v>337</v>
+      </c>
+      <c r="K52" s="8" t="s">
         <v>334</v>
       </c>
-      <c r="K52" s="8" t="s">
+      <c r="L52" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="M52" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="N52" s="8" t="s">
         <v>335</v>
-      </c>
-      <c r="L52" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="M52" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="N52" s="8" t="s">
-        <v>336</v>
       </c>
       <c r="O52" s="9" t="s">
         <v>122</v>
@@ -4256,51 +4295,111 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" ht="80" x14ac:dyDescent="0.25">
       <c r="A53" s="16">
         <v>35.130000000000102</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C53" s="13"/>
-      <c r="D53" s="7"/>
-      <c r="E53" s="7"/>
-      <c r="F53" s="15"/>
-      <c r="G53" s="8"/>
-      <c r="H53" s="9"/>
-      <c r="I53" s="7"/>
-      <c r="J53" s="8"/>
-      <c r="K53" s="8"/>
-      <c r="L53" s="8"/>
-      <c r="M53" s="8"/>
-      <c r="N53" s="8"/>
-      <c r="O53" s="9"/>
-      <c r="P53" s="7"/>
-      <c r="Q53" s="8"/>
-      <c r="R53" s="8"/>
-      <c r="S53" s="9"/>
-    </row>
-    <row r="54" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C53" s="13" t="s">
+        <v>336</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>331</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="F53" s="15">
+        <v>45886</v>
+      </c>
+      <c r="G53" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="H53" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="I53" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="J53" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="K53" s="8" t="s">
+        <v>340</v>
+      </c>
+      <c r="L53" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="M53" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="N53" s="8" t="s">
+        <v>342</v>
+      </c>
+      <c r="O53" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="P53" s="7">
+        <v>2</v>
+      </c>
+      <c r="Q53" s="8">
+        <v>3</v>
+      </c>
+      <c r="R53" s="8">
+        <v>2</v>
+      </c>
+      <c r="S53" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" ht="120" x14ac:dyDescent="0.25">
       <c r="A54" s="16">
         <v>35.1400000000001</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C54" s="13"/>
-      <c r="D54" s="7"/>
-      <c r="E54" s="7"/>
-      <c r="F54" s="15"/>
-      <c r="G54" s="8"/>
-      <c r="H54" s="9"/>
-      <c r="I54" s="7"/>
-      <c r="J54" s="8"/>
-      <c r="K54" s="8"/>
-      <c r="L54" s="8"/>
-      <c r="M54" s="8"/>
-      <c r="N54" s="8"/>
-      <c r="O54" s="9"/>
+      <c r="C54" s="13" t="s">
+        <v>343</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>331</v>
+      </c>
+      <c r="E54" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="F54" s="15">
+        <v>45886</v>
+      </c>
+      <c r="G54" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="H54" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="I54" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="J54" s="8" t="s">
+        <v>344</v>
+      </c>
+      <c r="K54" s="8" t="s">
+        <v>346</v>
+      </c>
+      <c r="L54" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="M54" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="N54" s="8" t="s">
+        <v>349</v>
+      </c>
+      <c r="O54" s="9" t="s">
+        <v>347</v>
+      </c>
       <c r="P54" s="7"/>
       <c r="Q54" s="8"/>
       <c r="R54" s="8"/>
@@ -5647,6 +5746,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="H32:H33"/>
+    <mergeCell ref="I32:O33"/>
     <mergeCell ref="I51:M51"/>
     <mergeCell ref="I48:M48"/>
     <mergeCell ref="I49:M49"/>
@@ -5654,11 +5758,6 @@
     <mergeCell ref="F2:H2"/>
     <mergeCell ref="I2:O2"/>
     <mergeCell ref="P32:S33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="H32:H33"/>
-    <mergeCell ref="I32:O33"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Hash set problem reflections
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bharat/bctci/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C26BC760-603F-C846-9319-5C658E5889CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7648DBA4-E6A4-9541-B79D-2451E14A07E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24380" windowHeight="16000" xr2:uid="{233FF15D-0BCB-6B46-B450-599851EED7C1}"/>
+    <workbookView xWindow="25600" yWindow="2180" windowWidth="26880" windowHeight="15120" xr2:uid="{233FF15D-0BCB-6B46-B450-599851EED7C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="376">
   <si>
     <t>Sets &amp; Maps</t>
   </si>
@@ -1123,6 +1123,51 @@
   </si>
   <si>
     <t>Yes, algorithm for merging two sorted arrays -- handling diff lens, using extend</t>
+  </si>
+  <si>
+    <t>List of arrays, to which values are index-assigned based on hashing of input integer</t>
+  </si>
+  <si>
+    <t>O(1)</t>
+  </si>
+  <si>
+    <t>Got it mostly right, but forgot to consider resizing (for better retrieval)</t>
+  </si>
+  <si>
+    <t>That it was pretty similar to the dynamic array problem</t>
+  </si>
+  <si>
+    <t>[] * len gave me copies of the same object, use list comprehension instead</t>
+  </si>
+  <si>
+    <t>Revise this implementation</t>
+  </si>
+  <si>
+    <t>List comprehension to declare array of empty arrays</t>
+  </si>
+  <si>
+    <t>Iterate through buckets to generate list, and use that as basis for union and extend</t>
+  </si>
+  <si>
+    <t>Got this one almost perfectly right</t>
+  </si>
+  <si>
+    <t>That I needed to iterate, and that involved traversing the buckets</t>
+  </si>
+  <si>
+    <t>Appending instead of extending, extending is faster</t>
+  </si>
+  <si>
+    <t>Good to know</t>
+  </si>
+  <si>
+    <t>Load factor logic</t>
+  </si>
+  <si>
+    <t>Minor changes to has set implementation</t>
+  </si>
+  <si>
+    <t>Knuth multiplicative and base128 algorithms</t>
   </si>
 </sst>
 </file>
@@ -1463,19 +1508,13 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1492,6 +1531,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1832,9 +1877,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4095FB6B-33CD-C94D-A3B2-EAADF58B3AE5}">
   <dimension ref="A1:S110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q57" sqref="Q57"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P63" sqref="P63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1923,26 +1968,26 @@
       </c>
       <c r="D2" s="26"/>
       <c r="E2" s="26"/>
-      <c r="F2" s="43" t="s">
+      <c r="F2" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="G2" s="41"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="40" t="s">
+      <c r="G2" s="39"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="41"/>
-      <c r="O2" s="44"/>
-      <c r="P2" s="40" t="s">
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="42"/>
+      <c r="P2" s="38" t="s">
         <v>111</v>
       </c>
-      <c r="Q2" s="41"/>
-      <c r="R2" s="41"/>
-      <c r="S2" s="42"/>
+      <c r="Q2" s="39"/>
+      <c r="R2" s="39"/>
+      <c r="S2" s="40"/>
     </row>
     <row r="3" spans="1:19" s="8" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14">
@@ -3335,35 +3380,35 @@
       <c r="B32" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="35" t="s">
+      <c r="C32" s="43" t="s">
         <v>254</v>
       </c>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
-      <c r="F32" s="36">
+      <c r="F32" s="44">
         <v>45871</v>
       </c>
-      <c r="G32" s="37" t="s">
+      <c r="G32" s="36" t="s">
         <v>255</v>
       </c>
-      <c r="H32" s="38" t="s">
+      <c r="H32" s="37" t="s">
         <v>255</v>
       </c>
-      <c r="I32" s="39" t="s">
+      <c r="I32" s="35" t="s">
         <v>256</v>
       </c>
-      <c r="J32" s="37"/>
-      <c r="K32" s="37"/>
-      <c r="L32" s="37"/>
-      <c r="M32" s="37"/>
-      <c r="N32" s="37"/>
-      <c r="O32" s="38"/>
-      <c r="P32" s="39">
+      <c r="J32" s="36"/>
+      <c r="K32" s="36"/>
+      <c r="L32" s="36"/>
+      <c r="M32" s="36"/>
+      <c r="N32" s="36"/>
+      <c r="O32" s="37"/>
+      <c r="P32" s="35">
         <v>2</v>
       </c>
-      <c r="Q32" s="37"/>
-      <c r="R32" s="37"/>
-      <c r="S32" s="38"/>
+      <c r="Q32" s="36"/>
+      <c r="R32" s="36"/>
+      <c r="S32" s="37"/>
     </row>
     <row r="33" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="17">
@@ -3372,23 +3417,23 @@
       <c r="B33" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="35"/>
+      <c r="C33" s="43"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
-      <c r="F33" s="36"/>
-      <c r="G33" s="37"/>
-      <c r="H33" s="38"/>
-      <c r="I33" s="39"/>
-      <c r="J33" s="37"/>
-      <c r="K33" s="37"/>
-      <c r="L33" s="37"/>
-      <c r="M33" s="37"/>
-      <c r="N33" s="37"/>
-      <c r="O33" s="38"/>
-      <c r="P33" s="39"/>
-      <c r="Q33" s="37"/>
-      <c r="R33" s="37"/>
-      <c r="S33" s="38"/>
+      <c r="F33" s="44"/>
+      <c r="G33" s="36"/>
+      <c r="H33" s="37"/>
+      <c r="I33" s="35"/>
+      <c r="J33" s="36"/>
+      <c r="K33" s="36"/>
+      <c r="L33" s="36"/>
+      <c r="M33" s="36"/>
+      <c r="N33" s="36"/>
+      <c r="O33" s="37"/>
+      <c r="P33" s="35"/>
+      <c r="Q33" s="36"/>
+      <c r="R33" s="36"/>
+      <c r="S33" s="37"/>
     </row>
     <row r="34" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="16">
@@ -4085,13 +4130,13 @@
       <c r="H48" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="I48" s="39" t="s">
+      <c r="I48" s="35" t="s">
         <v>317</v>
       </c>
-      <c r="J48" s="37"/>
-      <c r="K48" s="37"/>
-      <c r="L48" s="37"/>
-      <c r="M48" s="37"/>
+      <c r="J48" s="36"/>
+      <c r="K48" s="36"/>
+      <c r="L48" s="36"/>
+      <c r="M48" s="36"/>
       <c r="N48" s="8" t="s">
         <v>320</v>
       </c>
@@ -4136,13 +4181,13 @@
       <c r="H49" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="I49" s="39" t="s">
+      <c r="I49" s="35" t="s">
         <v>317</v>
       </c>
-      <c r="J49" s="37"/>
-      <c r="K49" s="37"/>
-      <c r="L49" s="37"/>
-      <c r="M49" s="37"/>
+      <c r="J49" s="36"/>
+      <c r="K49" s="36"/>
+      <c r="L49" s="36"/>
+      <c r="M49" s="36"/>
       <c r="N49" s="8" t="s">
         <v>320</v>
       </c>
@@ -4246,13 +4291,13 @@
       <c r="H51" s="9" t="s">
         <v>250</v>
       </c>
-      <c r="I51" s="39" t="s">
+      <c r="I51" s="35" t="s">
         <v>317</v>
       </c>
-      <c r="J51" s="37"/>
-      <c r="K51" s="37"/>
-      <c r="L51" s="37"/>
-      <c r="M51" s="37"/>
+      <c r="J51" s="36"/>
+      <c r="K51" s="36"/>
+      <c r="L51" s="36"/>
+      <c r="M51" s="36"/>
       <c r="N51" s="8" t="s">
         <v>328</v>
       </c>
@@ -4533,15 +4578,15 @@
       <c r="H56" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="I56" s="39" t="s">
+      <c r="I56" s="35" t="s">
         <v>317</v>
       </c>
-      <c r="J56" s="45"/>
-      <c r="K56" s="45"/>
-      <c r="L56" s="45"/>
-      <c r="M56" s="45"/>
-      <c r="N56" s="45"/>
-      <c r="O56" s="38"/>
+      <c r="J56" s="36"/>
+      <c r="K56" s="36"/>
+      <c r="L56" s="36"/>
+      <c r="M56" s="36"/>
+      <c r="N56" s="36"/>
+      <c r="O56" s="37"/>
       <c r="P56" s="7">
         <v>4</v>
       </c>
@@ -4674,80 +4719,172 @@
       <c r="R60" s="8"/>
       <c r="S60" s="9"/>
     </row>
-    <row r="61" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A61" s="17">
         <v>1</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C61" s="13"/>
-      <c r="D61" s="7"/>
-      <c r="E61" s="7"/>
-      <c r="F61" s="15"/>
-      <c r="G61" s="8"/>
-      <c r="H61" s="9"/>
-      <c r="I61" s="7"/>
-      <c r="J61" s="8"/>
-      <c r="K61" s="8"/>
-      <c r="L61" s="8"/>
-      <c r="M61" s="8"/>
-      <c r="N61" s="8"/>
-      <c r="O61" s="9"/>
-      <c r="P61" s="7"/>
-      <c r="Q61" s="8"/>
-      <c r="R61" s="8"/>
-      <c r="S61" s="9"/>
-    </row>
-    <row r="62" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C61" s="13" t="s">
+        <v>361</v>
+      </c>
+      <c r="D61" s="7" t="s">
+        <v>362</v>
+      </c>
+      <c r="E61" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="F61" s="15">
+        <v>45888</v>
+      </c>
+      <c r="G61" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="H61" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="I61" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="J61" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="K61" s="8" t="s">
+        <v>364</v>
+      </c>
+      <c r="L61" s="8" t="s">
+        <v>365</v>
+      </c>
+      <c r="M61" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="N61" s="8" t="s">
+        <v>366</v>
+      </c>
+      <c r="O61" s="9" t="s">
+        <v>367</v>
+      </c>
+      <c r="P61" s="7">
+        <v>3</v>
+      </c>
+      <c r="Q61" s="8">
+        <v>3</v>
+      </c>
+      <c r="R61" s="8">
+        <v>3</v>
+      </c>
+      <c r="S61" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A62" s="17">
         <v>2</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C62" s="13"/>
-      <c r="D62" s="7"/>
-      <c r="E62" s="7"/>
-      <c r="F62" s="15"/>
-      <c r="G62" s="8"/>
-      <c r="H62" s="9"/>
-      <c r="I62" s="7"/>
-      <c r="J62" s="8"/>
-      <c r="K62" s="8"/>
-      <c r="L62" s="8"/>
-      <c r="M62" s="8"/>
-      <c r="N62" s="8"/>
-      <c r="O62" s="9"/>
-      <c r="P62" s="7"/>
-      <c r="Q62" s="8"/>
-      <c r="R62" s="8"/>
-      <c r="S62" s="9"/>
-    </row>
-    <row r="63" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C62" s="13" t="s">
+        <v>368</v>
+      </c>
+      <c r="D62" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="E62" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="F62" s="15">
+        <v>45888</v>
+      </c>
+      <c r="G62" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="H62" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="I62" s="7" t="s">
+        <v>369</v>
+      </c>
+      <c r="J62" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="K62" s="8" t="s">
+        <v>370</v>
+      </c>
+      <c r="L62" s="8" t="s">
+        <v>371</v>
+      </c>
+      <c r="M62" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="N62" s="8" t="s">
+        <v>372</v>
+      </c>
+      <c r="O62" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="P62" s="7">
+        <v>4</v>
+      </c>
+      <c r="Q62" s="8">
+        <v>4</v>
+      </c>
+      <c r="R62" s="8">
+        <v>4</v>
+      </c>
+      <c r="S62" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19" ht="40" x14ac:dyDescent="0.25">
       <c r="A63" s="17">
         <v>3</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C63" s="13"/>
-      <c r="D63" s="7"/>
-      <c r="E63" s="7"/>
-      <c r="F63" s="15"/>
-      <c r="G63" s="8"/>
-      <c r="H63" s="9"/>
-      <c r="I63" s="7"/>
-      <c r="J63" s="8"/>
-      <c r="K63" s="8"/>
-      <c r="L63" s="8"/>
-      <c r="M63" s="8"/>
-      <c r="N63" s="8"/>
-      <c r="O63" s="9"/>
-      <c r="P63" s="7"/>
-      <c r="Q63" s="8"/>
-      <c r="R63" s="8"/>
-      <c r="S63" s="9"/>
+      <c r="C63" s="13" t="s">
+        <v>374</v>
+      </c>
+      <c r="D63" s="7" t="s">
+        <v>362</v>
+      </c>
+      <c r="E63" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="F63" s="15">
+        <v>45888</v>
+      </c>
+      <c r="G63" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="H63" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="I63" s="35" t="s">
+        <v>317</v>
+      </c>
+      <c r="J63" s="45"/>
+      <c r="K63" s="45"/>
+      <c r="L63" s="45"/>
+      <c r="M63" s="45"/>
+      <c r="N63" s="45"/>
+      <c r="O63" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="P63" s="7">
+        <v>4</v>
+      </c>
+      <c r="Q63" s="8">
+        <v>4</v>
+      </c>
+      <c r="R63" s="8">
+        <v>4</v>
+      </c>
+      <c r="S63" s="9">
+        <v>4</v>
+      </c>
     </row>
     <row r="64" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="17">
@@ -5879,12 +6016,8 @@
       <c r="S110" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="I56:O56"/>
-    <mergeCell ref="I51:M51"/>
-    <mergeCell ref="I48:M48"/>
-    <mergeCell ref="I49:M49"/>
-    <mergeCell ref="P2:S2"/>
+  <mergeCells count="14">
+    <mergeCell ref="I63:N63"/>
     <mergeCell ref="F2:H2"/>
     <mergeCell ref="I2:O2"/>
     <mergeCell ref="P32:S33"/>
@@ -5893,6 +6026,11 @@
     <mergeCell ref="G32:G33"/>
     <mergeCell ref="H32:H33"/>
     <mergeCell ref="I32:O33"/>
+    <mergeCell ref="I56:O56"/>
+    <mergeCell ref="I51:M51"/>
+    <mergeCell ref="I48:M48"/>
+    <mergeCell ref="I49:M49"/>
+    <mergeCell ref="P2:S2"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Wrapping up set and map implementations
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bharat/bctci/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7648DBA4-E6A4-9541-B79D-2451E14A07E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F37C4B1-E1B7-A747-8EB5-F861310AD4FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="2180" windowWidth="26880" windowHeight="15120" xr2:uid="{233FF15D-0BCB-6B46-B450-599851EED7C1}"/>
+    <workbookView xWindow="26840" yWindow="2180" windowWidth="24380" windowHeight="15120" xr2:uid="{233FF15D-0BCB-6B46-B450-599851EED7C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="387">
   <si>
     <t>Sets &amp; Maps</t>
   </si>
@@ -1164,10 +1164,43 @@
     <t>Load factor logic</t>
   </si>
   <si>
-    <t>Minor changes to has set implementation</t>
-  </si>
-  <si>
-    <t>Knuth multiplicative and base128 algorithms</t>
+    <t>Chose None as the default value for a key, but did not handle collision resistance</t>
+  </si>
+  <si>
+    <t>Forgetting collision made all methods unreliable. Should have store k and v in a tuple</t>
+  </si>
+  <si>
+    <t>That I need to handle collisions in sets AND maps. Maps don't free me from that responsibility</t>
+  </si>
+  <si>
+    <t>Iterative over buckets and get keys, iterate over buckets and get values</t>
+  </si>
+  <si>
+    <t>O(size)</t>
+  </si>
+  <si>
+    <t>Store (k, [values]) instead of (k,v) in map</t>
+  </si>
+  <si>
+    <t>store (v, count) instead of v in bucket using hashmap</t>
+  </si>
+  <si>
+    <t>Need to review this pattern</t>
+  </si>
+  <si>
+    <t>Pattern of storing count in multiset and list of values in multimap</t>
+  </si>
+  <si>
+    <t>Some off-by-one, attributable to noise around me</t>
+  </si>
+  <si>
+    <t>Good pattern</t>
+  </si>
+  <si>
+    <t>(k, [values])</t>
+  </si>
+  <si>
+    <t>Knuth multiplicative and base128 algorithms; (k, count}</t>
   </si>
 </sst>
 </file>
@@ -1514,29 +1547,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="15" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1877,9 +1910,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4095FB6B-33CD-C94D-A3B2-EAADF58B3AE5}">
   <dimension ref="A1:S110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P63" sqref="P63"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O64" sqref="O64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1968,26 +2001,26 @@
       </c>
       <c r="D2" s="26"/>
       <c r="E2" s="26"/>
-      <c r="F2" s="41" t="s">
+      <c r="F2" s="37" t="s">
         <v>112</v>
       </c>
-      <c r="G2" s="39"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="38" t="s">
+      <c r="G2" s="38"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="42"/>
-      <c r="P2" s="38" t="s">
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="40" t="s">
         <v>111</v>
       </c>
-      <c r="Q2" s="39"/>
-      <c r="R2" s="39"/>
-      <c r="S2" s="40"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="38"/>
+      <c r="S2" s="44"/>
     </row>
     <row r="3" spans="1:19" s="8" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14">
@@ -3380,18 +3413,18 @@
       <c r="B32" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="43" t="s">
+      <c r="C32" s="42" t="s">
         <v>254</v>
       </c>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
-      <c r="F32" s="44">
+      <c r="F32" s="43">
         <v>45871</v>
       </c>
       <c r="G32" s="36" t="s">
         <v>255</v>
       </c>
-      <c r="H32" s="37" t="s">
+      <c r="H32" s="41" t="s">
         <v>255</v>
       </c>
       <c r="I32" s="35" t="s">
@@ -3402,13 +3435,13 @@
       <c r="L32" s="36"/>
       <c r="M32" s="36"/>
       <c r="N32" s="36"/>
-      <c r="O32" s="37"/>
+      <c r="O32" s="41"/>
       <c r="P32" s="35">
         <v>2</v>
       </c>
       <c r="Q32" s="36"/>
       <c r="R32" s="36"/>
-      <c r="S32" s="37"/>
+      <c r="S32" s="41"/>
     </row>
     <row r="33" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="17">
@@ -3417,23 +3450,23 @@
       <c r="B33" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="43"/>
+      <c r="C33" s="42"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
-      <c r="F33" s="44"/>
+      <c r="F33" s="43"/>
       <c r="G33" s="36"/>
-      <c r="H33" s="37"/>
+      <c r="H33" s="41"/>
       <c r="I33" s="35"/>
       <c r="J33" s="36"/>
       <c r="K33" s="36"/>
       <c r="L33" s="36"/>
       <c r="M33" s="36"/>
       <c r="N33" s="36"/>
-      <c r="O33" s="37"/>
+      <c r="O33" s="41"/>
       <c r="P33" s="35"/>
       <c r="Q33" s="36"/>
       <c r="R33" s="36"/>
-      <c r="S33" s="37"/>
+      <c r="S33" s="41"/>
     </row>
     <row r="34" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="16">
@@ -4586,7 +4619,7 @@
       <c r="L56" s="36"/>
       <c r="M56" s="36"/>
       <c r="N56" s="36"/>
-      <c r="O56" s="37"/>
+      <c r="O56" s="41"/>
       <c r="P56" s="7">
         <v>4</v>
       </c>
@@ -4845,7 +4878,7 @@
         <v>56</v>
       </c>
       <c r="C63" s="13" t="s">
-        <v>374</v>
+        <v>380</v>
       </c>
       <c r="D63" s="7" t="s">
         <v>362</v>
@@ -4865,13 +4898,13 @@
       <c r="I63" s="35" t="s">
         <v>317</v>
       </c>
-      <c r="J63" s="45"/>
-      <c r="K63" s="45"/>
-      <c r="L63" s="45"/>
-      <c r="M63" s="45"/>
-      <c r="N63" s="45"/>
+      <c r="J63" s="36"/>
+      <c r="K63" s="36"/>
+      <c r="L63" s="36"/>
+      <c r="M63" s="36"/>
+      <c r="N63" s="36"/>
       <c r="O63" s="9" t="s">
-        <v>375</v>
+        <v>386</v>
       </c>
       <c r="P63" s="7">
         <v>4</v>
@@ -4886,76 +4919,158 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" ht="80" x14ac:dyDescent="0.25">
       <c r="A64" s="17">
         <v>4</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C64" s="13"/>
-      <c r="D64" s="7"/>
-      <c r="E64" s="7"/>
-      <c r="F64" s="15"/>
-      <c r="G64" s="8"/>
-      <c r="H64" s="9"/>
-      <c r="I64" s="7"/>
-      <c r="J64" s="8"/>
-      <c r="K64" s="8"/>
-      <c r="L64" s="8"/>
-      <c r="M64" s="8"/>
-      <c r="N64" s="8"/>
-      <c r="O64" s="9"/>
-      <c r="P64" s="7"/>
-      <c r="Q64" s="8"/>
-      <c r="R64" s="8"/>
-      <c r="S64" s="9"/>
-    </row>
-    <row r="65" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C64" s="13" t="s">
+        <v>374</v>
+      </c>
+      <c r="D64" s="7" t="s">
+        <v>362</v>
+      </c>
+      <c r="E64" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="F64" s="15">
+        <v>45889</v>
+      </c>
+      <c r="G64" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="H64" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="I64" s="7" t="s">
+        <v>375</v>
+      </c>
+      <c r="J64" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="K64" s="8" t="s">
+        <v>376</v>
+      </c>
+      <c r="L64" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="M64" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="N64" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="O64" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="P64" s="7">
+        <v>3</v>
+      </c>
+      <c r="Q64" s="8">
+        <v>3</v>
+      </c>
+      <c r="R64" s="8">
+        <v>2</v>
+      </c>
+      <c r="S64" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19" ht="40" x14ac:dyDescent="0.25">
       <c r="A65" s="17">
         <v>5</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C65" s="13"/>
-      <c r="D65" s="7"/>
-      <c r="E65" s="7"/>
-      <c r="F65" s="15"/>
-      <c r="G65" s="8"/>
-      <c r="H65" s="9"/>
-      <c r="I65" s="7"/>
-      <c r="J65" s="8"/>
-      <c r="K65" s="8"/>
-      <c r="L65" s="8"/>
-      <c r="M65" s="8"/>
-      <c r="N65" s="8"/>
-      <c r="O65" s="9"/>
-      <c r="P65" s="7"/>
-      <c r="Q65" s="8"/>
-      <c r="R65" s="8"/>
-      <c r="S65" s="9"/>
-    </row>
-    <row r="66" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C65" s="13" t="s">
+        <v>377</v>
+      </c>
+      <c r="D65" s="7" t="s">
+        <v>378</v>
+      </c>
+      <c r="E65" s="7" t="s">
+        <v>378</v>
+      </c>
+      <c r="F65" s="15">
+        <v>45889</v>
+      </c>
+      <c r="G65" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="H65" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="I65" s="35" t="s">
+        <v>317</v>
+      </c>
+      <c r="J65" s="45"/>
+      <c r="K65" s="45"/>
+      <c r="L65" s="45"/>
+      <c r="M65" s="45"/>
+      <c r="N65" s="45"/>
+      <c r="O65" s="41"/>
+      <c r="P65" s="7">
+        <v>4</v>
+      </c>
+      <c r="Q65" s="8">
+        <v>4</v>
+      </c>
+      <c r="R65" s="8">
+        <v>4</v>
+      </c>
+      <c r="S65" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A66" s="17">
         <v>6</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C66" s="13"/>
-      <c r="D66" s="7"/>
-      <c r="E66" s="7"/>
-      <c r="F66" s="15"/>
-      <c r="G66" s="8"/>
-      <c r="H66" s="9"/>
-      <c r="I66" s="7"/>
-      <c r="J66" s="8"/>
-      <c r="K66" s="8"/>
-      <c r="L66" s="8"/>
-      <c r="M66" s="8"/>
-      <c r="N66" s="8"/>
-      <c r="O66" s="9"/>
+      <c r="C66" s="13" t="s">
+        <v>379</v>
+      </c>
+      <c r="D66" s="7" t="s">
+        <v>378</v>
+      </c>
+      <c r="E66" s="7" t="s">
+        <v>378</v>
+      </c>
+      <c r="F66" s="15">
+        <v>45889</v>
+      </c>
+      <c r="G66" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="H66" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="I66" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="J66" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="K66" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="L66" s="8" t="s">
+        <v>383</v>
+      </c>
+      <c r="M66" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="N66" s="8" t="s">
+        <v>384</v>
+      </c>
+      <c r="O66" s="9" t="s">
+        <v>385</v>
+      </c>
       <c r="P66" s="7"/>
       <c r="Q66" s="8"/>
       <c r="R66" s="8"/>
@@ -6016,7 +6131,8 @@
       <c r="S110" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="15">
+    <mergeCell ref="I65:O65"/>
     <mergeCell ref="I63:N63"/>
     <mergeCell ref="F2:H2"/>
     <mergeCell ref="I2:O2"/>

</xml_diff>

<commit_message>
5 more backtracking problems
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bharat/bctci/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{924EF83E-0076-0046-96A8-8F63E626488F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9AAFF52-CC17-A74D-8FAC-5EFBC9F1A82F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="2180" windowWidth="26880" windowHeight="15120" xr2:uid="{233FF15D-0BCB-6B46-B450-599851EED7C1}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{233FF15D-0BCB-6B46-B450-599851EED7C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="448">
   <si>
     <t>Sets &amp; Maps</t>
   </si>
@@ -1312,6 +1312,78 @@
   </si>
   <si>
     <t>Template, partial solution data structure</t>
+  </si>
+  <si>
+    <t>Iterate through words, and make a choice to include and not include at each word</t>
+  </si>
+  <si>
+    <t>My solution and the book's solutions were identical</t>
+  </si>
+  <si>
+    <t>To make a choice, backtrack and make the not choice</t>
+  </si>
+  <si>
+    <t>To iterate through words, branching at words that have synonyms</t>
+  </si>
+  <si>
+    <t>Do as an exercise</t>
+  </si>
+  <si>
+    <t>Got to mine almost by accident. Understood that decision tree should be at root after all decisions have been taken, rather than leaves</t>
+  </si>
+  <si>
+    <t>State of decision tree at the end of traversal</t>
+  </si>
+  <si>
+    <t>Didn't solve it. Tried to iterate through index of digits via recursive function, but that did not have partial solution as argument</t>
+  </si>
+  <si>
+    <t>Even if the first step in decision tree has 10 options, subsequent ones only had two. The first step could happen outside the recursive function</t>
+  </si>
+  <si>
+    <t>I did identify that iterating over all nums less than self was suboptimal</t>
+  </si>
+  <si>
+    <t>Building up partial solution</t>
+  </si>
+  <si>
+    <t>Array of nums to string joined by "" requires ints to be mapped to str</t>
+  </si>
+  <si>
+    <t>Good problem, reinforced structure</t>
+  </si>
+  <si>
+    <t>Review backtracking template</t>
+  </si>
+  <si>
+    <t>Visit every step and decide whether to pick or not. My full solution checked for exceeding budget, when it could have happened at child stage. Also, I had methods for sums of cost and rating, when they could have been passed down.</t>
+  </si>
+  <si>
+    <t>I recognised a decision tree, and got the iteration right. However, choice of passing parameters down, and trimming decisions at child stage could have been better</t>
+  </si>
+  <si>
+    <t>That the leaf node of decision tree doesn't have to mean that all elements are present</t>
+  </si>
+  <si>
+    <t>That I could pass sums down recursive calls</t>
+  </si>
+  <si>
+    <t>Recognised that there are 26 options for the first, 25 for the second on so on. But got my recursion wrong.</t>
+  </si>
+  <si>
+    <t>Pattern for returning early in backtracking: return res else return None for edge cases or end of recursive function</t>
+  </si>
+  <si>
+    <t>Did two appends, which was a mistake. Also, missed checking on maxlen and returning pattern</t>
+  </si>
+  <si>
+    <t>I should have checked pwd at every turn, and figured out a pattern of returning early</t>
+  </si>
+  <si>
+    <t>Particularly bad if check inside for loop for alphabet characters</t>
+  </si>
+  <si>
+    <t>Good variation</t>
   </si>
 </sst>
 </file>
@@ -1542,7 +1614,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1627,21 +1699,6 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1654,8 +1711,26 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1993,9 +2068,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4095FB6B-33CD-C94D-A3B2-EAADF58B3AE5}">
   <dimension ref="A1:S120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O72" sqref="O72"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I77" sqref="I77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2084,26 +2159,26 @@
       </c>
       <c r="D2" s="26"/>
       <c r="E2" s="26"/>
-      <c r="F2" s="37" t="s">
+      <c r="F2" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="G2" s="38"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="40" t="s">
+      <c r="G2" s="33"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="38"/>
-      <c r="O2" s="39"/>
-      <c r="P2" s="40" t="s">
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="Q2" s="38"/>
-      <c r="R2" s="38"/>
-      <c r="S2" s="41"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="39"/>
     </row>
     <row r="3" spans="1:19" s="8" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14">
@@ -3496,35 +3571,35 @@
       <c r="B32" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="32" t="s">
+      <c r="C32" s="41" t="s">
         <v>251</v>
       </c>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
-      <c r="F32" s="33">
+      <c r="F32" s="42">
         <v>45871</v>
       </c>
-      <c r="G32" s="34" t="s">
+      <c r="G32" s="37" t="s">
         <v>252</v>
       </c>
-      <c r="H32" s="35" t="s">
+      <c r="H32" s="38" t="s">
         <v>252</v>
       </c>
       <c r="I32" s="36" t="s">
         <v>253</v>
       </c>
-      <c r="J32" s="34"/>
-      <c r="K32" s="34"/>
-      <c r="L32" s="34"/>
-      <c r="M32" s="34"/>
-      <c r="N32" s="34"/>
-      <c r="O32" s="35"/>
+      <c r="J32" s="37"/>
+      <c r="K32" s="37"/>
+      <c r="L32" s="37"/>
+      <c r="M32" s="37"/>
+      <c r="N32" s="37"/>
+      <c r="O32" s="38"/>
       <c r="P32" s="36">
         <v>2</v>
       </c>
-      <c r="Q32" s="34"/>
-      <c r="R32" s="34"/>
-      <c r="S32" s="35"/>
+      <c r="Q32" s="37"/>
+      <c r="R32" s="37"/>
+      <c r="S32" s="38"/>
     </row>
     <row r="33" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="17">
@@ -3533,23 +3608,23 @@
       <c r="B33" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="32"/>
+      <c r="C33" s="41"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
-      <c r="F33" s="33"/>
-      <c r="G33" s="34"/>
-      <c r="H33" s="35"/>
+      <c r="F33" s="42"/>
+      <c r="G33" s="37"/>
+      <c r="H33" s="38"/>
       <c r="I33" s="36"/>
-      <c r="J33" s="34"/>
-      <c r="K33" s="34"/>
-      <c r="L33" s="34"/>
-      <c r="M33" s="34"/>
-      <c r="N33" s="34"/>
-      <c r="O33" s="35"/>
+      <c r="J33" s="37"/>
+      <c r="K33" s="37"/>
+      <c r="L33" s="37"/>
+      <c r="M33" s="37"/>
+      <c r="N33" s="37"/>
+      <c r="O33" s="38"/>
       <c r="P33" s="36"/>
-      <c r="Q33" s="34"/>
-      <c r="R33" s="34"/>
-      <c r="S33" s="35"/>
+      <c r="Q33" s="37"/>
+      <c r="R33" s="37"/>
+      <c r="S33" s="38"/>
     </row>
     <row r="34" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="16">
@@ -4249,10 +4324,10 @@
       <c r="I48" s="36" t="s">
         <v>314</v>
       </c>
-      <c r="J48" s="34"/>
-      <c r="K48" s="34"/>
-      <c r="L48" s="34"/>
-      <c r="M48" s="34"/>
+      <c r="J48" s="37"/>
+      <c r="K48" s="37"/>
+      <c r="L48" s="37"/>
+      <c r="M48" s="37"/>
       <c r="N48" s="8" t="s">
         <v>317</v>
       </c>
@@ -4300,10 +4375,10 @@
       <c r="I49" s="36" t="s">
         <v>314</v>
       </c>
-      <c r="J49" s="34"/>
-      <c r="K49" s="34"/>
-      <c r="L49" s="34"/>
-      <c r="M49" s="34"/>
+      <c r="J49" s="37"/>
+      <c r="K49" s="37"/>
+      <c r="L49" s="37"/>
+      <c r="M49" s="37"/>
       <c r="N49" s="8" t="s">
         <v>317</v>
       </c>
@@ -4410,10 +4485,10 @@
       <c r="I51" s="36" t="s">
         <v>314</v>
       </c>
-      <c r="J51" s="34"/>
-      <c r="K51" s="34"/>
-      <c r="L51" s="34"/>
-      <c r="M51" s="34"/>
+      <c r="J51" s="37"/>
+      <c r="K51" s="37"/>
+      <c r="L51" s="37"/>
+      <c r="M51" s="37"/>
       <c r="N51" s="8" t="s">
         <v>325</v>
       </c>
@@ -4697,12 +4772,12 @@
       <c r="I56" s="36" t="s">
         <v>314</v>
       </c>
-      <c r="J56" s="34"/>
-      <c r="K56" s="34"/>
-      <c r="L56" s="34"/>
-      <c r="M56" s="34"/>
-      <c r="N56" s="34"/>
-      <c r="O56" s="35"/>
+      <c r="J56" s="37"/>
+      <c r="K56" s="37"/>
+      <c r="L56" s="37"/>
+      <c r="M56" s="37"/>
+      <c r="N56" s="37"/>
+      <c r="O56" s="38"/>
       <c r="P56" s="7">
         <v>4</v>
       </c>
@@ -4981,11 +5056,11 @@
       <c r="I63" s="36" t="s">
         <v>314</v>
       </c>
-      <c r="J63" s="34"/>
-      <c r="K63" s="34"/>
-      <c r="L63" s="34"/>
-      <c r="M63" s="34"/>
-      <c r="N63" s="34"/>
+      <c r="J63" s="37"/>
+      <c r="K63" s="37"/>
+      <c r="L63" s="37"/>
+      <c r="M63" s="37"/>
+      <c r="N63" s="37"/>
       <c r="O63" s="9" t="s">
         <v>383</v>
       </c>
@@ -5089,12 +5164,12 @@
       <c r="I65" s="36" t="s">
         <v>314</v>
       </c>
-      <c r="J65" s="34"/>
-      <c r="K65" s="34"/>
-      <c r="L65" s="34"/>
-      <c r="M65" s="34"/>
-      <c r="N65" s="34"/>
-      <c r="O65" s="35"/>
+      <c r="J65" s="37"/>
+      <c r="K65" s="37"/>
+      <c r="L65" s="37"/>
+      <c r="M65" s="37"/>
+      <c r="N65" s="37"/>
+      <c r="O65" s="38"/>
       <c r="P65" s="7">
         <v>4</v>
       </c>
@@ -5396,126 +5471,274 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A73" s="16">
         <v>39.04</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C73" s="13"/>
-      <c r="D73" s="7"/>
-      <c r="E73" s="7"/>
-      <c r="F73" s="15"/>
-      <c r="G73" s="8"/>
-      <c r="H73" s="9"/>
-      <c r="I73" s="7"/>
-      <c r="J73" s="8"/>
-      <c r="K73" s="8"/>
-      <c r="L73" s="8"/>
-      <c r="M73" s="8"/>
-      <c r="N73" s="8"/>
-      <c r="O73" s="9"/>
-      <c r="P73" s="7"/>
-      <c r="Q73" s="8"/>
-      <c r="R73" s="8"/>
-      <c r="S73" s="9"/>
-    </row>
-    <row r="74" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C73" s="13" t="s">
+        <v>424</v>
+      </c>
+      <c r="D73" s="7" t="s">
+        <v>428</v>
+      </c>
+      <c r="E73" s="7" t="s">
+        <v>428</v>
+      </c>
+      <c r="F73" s="15">
+        <v>45898</v>
+      </c>
+      <c r="G73" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="H73" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="I73" s="7" t="s">
+        <v>425</v>
+      </c>
+      <c r="J73" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="K73" s="8" t="s">
+        <v>426</v>
+      </c>
+      <c r="L73" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="M73" s="8" t="s">
+        <v>314</v>
+      </c>
+      <c r="N73" s="8" t="s">
+        <v>314</v>
+      </c>
+      <c r="O73" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="P73" s="7">
+        <v>4</v>
+      </c>
+      <c r="Q73" s="8">
+        <v>4</v>
+      </c>
+      <c r="R73" s="8">
+        <v>4</v>
+      </c>
+      <c r="S73" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:19" ht="80" x14ac:dyDescent="0.25">
       <c r="A74" s="16">
         <v>39.049999999999997</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C74" s="13"/>
-      <c r="D74" s="7"/>
-      <c r="E74" s="7"/>
-      <c r="F74" s="15"/>
-      <c r="G74" s="8"/>
-      <c r="H74" s="9"/>
-      <c r="I74" s="7"/>
-      <c r="J74" s="8"/>
-      <c r="K74" s="8"/>
-      <c r="L74" s="8"/>
-      <c r="M74" s="8"/>
-      <c r="N74" s="8"/>
-      <c r="O74" s="9"/>
-      <c r="P74" s="7"/>
-      <c r="Q74" s="8"/>
-      <c r="R74" s="8"/>
-      <c r="S74" s="9"/>
-    </row>
-    <row r="75" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C74" s="13" t="s">
+        <v>427</v>
+      </c>
+      <c r="D74" s="7" t="s">
+        <v>428</v>
+      </c>
+      <c r="E74" s="7" t="s">
+        <v>428</v>
+      </c>
+      <c r="F74" s="15">
+        <v>45898</v>
+      </c>
+      <c r="G74" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="H74" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="I74" s="7" t="s">
+        <v>429</v>
+      </c>
+      <c r="J74" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="K74" s="40" t="s">
+        <v>314</v>
+      </c>
+      <c r="L74" s="40"/>
+      <c r="M74" s="40"/>
+      <c r="N74" s="40"/>
+      <c r="O74" s="9" t="s">
+        <v>430</v>
+      </c>
+      <c r="P74" s="7">
+        <v>3</v>
+      </c>
+      <c r="Q74" s="8">
+        <v>3</v>
+      </c>
+      <c r="R74" s="8">
+        <v>3</v>
+      </c>
+      <c r="S74" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:19" ht="100" x14ac:dyDescent="0.25">
       <c r="A75" s="16">
         <v>39.06</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C75" s="13"/>
-      <c r="D75" s="7"/>
-      <c r="E75" s="7"/>
-      <c r="F75" s="15"/>
-      <c r="G75" s="8"/>
-      <c r="H75" s="9"/>
-      <c r="I75" s="7"/>
-      <c r="J75" s="8"/>
-      <c r="K75" s="8"/>
-      <c r="L75" s="8"/>
-      <c r="M75" s="8"/>
-      <c r="N75" s="8"/>
-      <c r="O75" s="9"/>
-      <c r="P75" s="7"/>
-      <c r="Q75" s="8"/>
-      <c r="R75" s="8"/>
-      <c r="S75" s="9"/>
-    </row>
-    <row r="76" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C75" s="13" t="s">
+        <v>431</v>
+      </c>
+      <c r="D75" s="7" t="s">
+        <v>428</v>
+      </c>
+      <c r="E75" s="7" t="s">
+        <v>428</v>
+      </c>
+      <c r="F75" s="15">
+        <v>45899</v>
+      </c>
+      <c r="G75" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="H75" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="I75" s="7" t="s">
+        <v>432</v>
+      </c>
+      <c r="J75" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="K75" s="8" t="s">
+        <v>433</v>
+      </c>
+      <c r="L75" s="8" t="s">
+        <v>434</v>
+      </c>
+      <c r="M75" s="8" t="s">
+        <v>435</v>
+      </c>
+      <c r="N75" s="8" t="s">
+        <v>436</v>
+      </c>
+      <c r="O75" s="9" t="s">
+        <v>437</v>
+      </c>
+      <c r="P75" s="7">
+        <v>3</v>
+      </c>
+      <c r="Q75" s="8">
+        <v>2</v>
+      </c>
+      <c r="R75" s="8">
+        <v>2</v>
+      </c>
+      <c r="S75" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:19" ht="140" x14ac:dyDescent="0.25">
       <c r="A76" s="16">
         <v>39.07</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C76" s="13"/>
+      <c r="C76" s="13" t="s">
+        <v>438</v>
+      </c>
       <c r="D76" s="7"/>
       <c r="E76" s="7"/>
-      <c r="F76" s="15"/>
-      <c r="G76" s="8"/>
-      <c r="H76" s="9"/>
-      <c r="I76" s="7"/>
-      <c r="J76" s="8"/>
-      <c r="K76" s="8"/>
-      <c r="L76" s="8"/>
-      <c r="M76" s="8"/>
-      <c r="N76" s="8"/>
-      <c r="O76" s="9"/>
-      <c r="P76" s="7"/>
-      <c r="Q76" s="8"/>
-      <c r="R76" s="8"/>
-      <c r="S76" s="9"/>
-    </row>
-    <row r="77" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F76" s="15">
+        <v>45899</v>
+      </c>
+      <c r="G76" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="H76" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="I76" s="7" t="s">
+        <v>439</v>
+      </c>
+      <c r="J76" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="K76" s="8" t="s">
+        <v>441</v>
+      </c>
+      <c r="L76" s="8" t="s">
+        <v>440</v>
+      </c>
+      <c r="M76" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="N76" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="O76" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="P76" s="7">
+        <v>2</v>
+      </c>
+      <c r="Q76" s="8">
+        <v>2</v>
+      </c>
+      <c r="R76" s="8">
+        <v>2</v>
+      </c>
+      <c r="S76" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:19" ht="80" x14ac:dyDescent="0.25">
       <c r="A77" s="16">
         <v>39.08</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C77" s="13"/>
+      <c r="C77" s="13" t="s">
+        <v>442</v>
+      </c>
       <c r="D77" s="7"/>
       <c r="E77" s="7"/>
-      <c r="F77" s="15"/>
-      <c r="G77" s="8"/>
-      <c r="H77" s="9"/>
-      <c r="I77" s="7"/>
-      <c r="J77" s="8"/>
-      <c r="K77" s="8"/>
-      <c r="L77" s="8"/>
-      <c r="M77" s="8"/>
-      <c r="N77" s="8"/>
-      <c r="O77" s="9"/>
+      <c r="F77" s="15">
+        <v>45899</v>
+      </c>
+      <c r="G77" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="H77" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="I77" s="7" t="s">
+        <v>444</v>
+      </c>
+      <c r="J77" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="K77" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="L77" s="8" t="s">
+        <v>446</v>
+      </c>
+      <c r="M77" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="N77" s="8" t="s">
+        <v>447</v>
+      </c>
+      <c r="O77" s="9" t="s">
+        <v>443</v>
+      </c>
       <c r="P77" s="7"/>
       <c r="Q77" s="8"/>
       <c r="R77" s="8"/>
@@ -6387,7 +6610,13 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
+    <mergeCell ref="K74:N74"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="H32:H33"/>
+    <mergeCell ref="I32:O33"/>
     <mergeCell ref="I65:O65"/>
     <mergeCell ref="I63:N63"/>
     <mergeCell ref="F2:H2"/>
@@ -6398,11 +6627,6 @@
     <mergeCell ref="I48:M48"/>
     <mergeCell ref="I49:M49"/>
     <mergeCell ref="P2:S2"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="H32:H33"/>
-    <mergeCell ref="I32:O33"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
One more backtracking problem (a tough one)
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bharat/bctci/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9AAFF52-CC17-A74D-8FAC-5EFBC9F1A82F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{229F9D65-9323-3247-9F30-A081D5D95167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{233FF15D-0BCB-6B46-B450-599851EED7C1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{233FF15D-0BCB-6B46-B450-599851EED7C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="453">
   <si>
     <t>Sets &amp; Maps</t>
   </si>
@@ -1384,6 +1384,21 @@
   </si>
   <si>
     <t>Good variation</t>
+  </si>
+  <si>
+    <t>Tried a simpler version with arrays, and then one version with Counter as multiset</t>
+  </si>
+  <si>
+    <t>Decide whether each element in multiset should be included or not. Another decision tree could have just cared about sum, not membership, and decision tree would have involved various keys of multisets, and how many instances of each to store</t>
+  </si>
+  <si>
+    <t>Space complexity was bad, also, couldn't figure out how to hash a Counter  -- use a sorted tuple</t>
+  </si>
+  <si>
+    <t>This was mostly fine</t>
+  </si>
+  <si>
+    <t>How to store a Counter or a List in a set (ie make hashable)</t>
   </si>
 </sst>
 </file>
@@ -1699,6 +1714,24 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1711,26 +1744,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2068,9 +2083,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4095FB6B-33CD-C94D-A3B2-EAADF58B3AE5}">
   <dimension ref="A1:S120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I77" sqref="I77"/>
+      <selection pane="bottomLeft" activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2159,26 +2174,26 @@
       </c>
       <c r="D2" s="26"/>
       <c r="E2" s="26"/>
-      <c r="F2" s="32" t="s">
+      <c r="F2" s="38" t="s">
         <v>109</v>
       </c>
-      <c r="G2" s="33"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="35" t="s">
+      <c r="G2" s="39"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="41" t="s">
         <v>103</v>
       </c>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="35" t="s">
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="40"/>
+      <c r="P2" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="39"/>
+      <c r="Q2" s="39"/>
+      <c r="R2" s="39"/>
+      <c r="S2" s="42"/>
     </row>
     <row r="3" spans="1:19" s="8" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14">
@@ -3571,35 +3586,35 @@
       <c r="B32" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="41" t="s">
+      <c r="C32" s="33" t="s">
         <v>251</v>
       </c>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
-      <c r="F32" s="42">
+      <c r="F32" s="34">
         <v>45871</v>
       </c>
-      <c r="G32" s="37" t="s">
+      <c r="G32" s="35" t="s">
         <v>252</v>
       </c>
-      <c r="H32" s="38" t="s">
+      <c r="H32" s="36" t="s">
         <v>252</v>
       </c>
-      <c r="I32" s="36" t="s">
+      <c r="I32" s="37" t="s">
         <v>253</v>
       </c>
-      <c r="J32" s="37"/>
-      <c r="K32" s="37"/>
-      <c r="L32" s="37"/>
-      <c r="M32" s="37"/>
-      <c r="N32" s="37"/>
-      <c r="O32" s="38"/>
-      <c r="P32" s="36">
+      <c r="J32" s="35"/>
+      <c r="K32" s="35"/>
+      <c r="L32" s="35"/>
+      <c r="M32" s="35"/>
+      <c r="N32" s="35"/>
+      <c r="O32" s="36"/>
+      <c r="P32" s="37">
         <v>2</v>
       </c>
-      <c r="Q32" s="37"/>
-      <c r="R32" s="37"/>
-      <c r="S32" s="38"/>
+      <c r="Q32" s="35"/>
+      <c r="R32" s="35"/>
+      <c r="S32" s="36"/>
     </row>
     <row r="33" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="17">
@@ -3608,23 +3623,23 @@
       <c r="B33" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="41"/>
+      <c r="C33" s="33"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
-      <c r="F33" s="42"/>
-      <c r="G33" s="37"/>
-      <c r="H33" s="38"/>
-      <c r="I33" s="36"/>
-      <c r="J33" s="37"/>
-      <c r="K33" s="37"/>
-      <c r="L33" s="37"/>
-      <c r="M33" s="37"/>
-      <c r="N33" s="37"/>
-      <c r="O33" s="38"/>
-      <c r="P33" s="36"/>
-      <c r="Q33" s="37"/>
-      <c r="R33" s="37"/>
-      <c r="S33" s="38"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="35"/>
+      <c r="H33" s="36"/>
+      <c r="I33" s="37"/>
+      <c r="J33" s="35"/>
+      <c r="K33" s="35"/>
+      <c r="L33" s="35"/>
+      <c r="M33" s="35"/>
+      <c r="N33" s="35"/>
+      <c r="O33" s="36"/>
+      <c r="P33" s="37"/>
+      <c r="Q33" s="35"/>
+      <c r="R33" s="35"/>
+      <c r="S33" s="36"/>
     </row>
     <row r="34" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="16">
@@ -4321,13 +4336,13 @@
       <c r="H48" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="I48" s="36" t="s">
+      <c r="I48" s="37" t="s">
         <v>314</v>
       </c>
-      <c r="J48" s="37"/>
-      <c r="K48" s="37"/>
-      <c r="L48" s="37"/>
-      <c r="M48" s="37"/>
+      <c r="J48" s="35"/>
+      <c r="K48" s="35"/>
+      <c r="L48" s="35"/>
+      <c r="M48" s="35"/>
       <c r="N48" s="8" t="s">
         <v>317</v>
       </c>
@@ -4372,13 +4387,13 @@
       <c r="H49" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="I49" s="36" t="s">
+      <c r="I49" s="37" t="s">
         <v>314</v>
       </c>
-      <c r="J49" s="37"/>
-      <c r="K49" s="37"/>
-      <c r="L49" s="37"/>
-      <c r="M49" s="37"/>
+      <c r="J49" s="35"/>
+      <c r="K49" s="35"/>
+      <c r="L49" s="35"/>
+      <c r="M49" s="35"/>
       <c r="N49" s="8" t="s">
         <v>317</v>
       </c>
@@ -4482,13 +4497,13 @@
       <c r="H51" s="9" t="s">
         <v>247</v>
       </c>
-      <c r="I51" s="36" t="s">
+      <c r="I51" s="37" t="s">
         <v>314</v>
       </c>
-      <c r="J51" s="37"/>
-      <c r="K51" s="37"/>
-      <c r="L51" s="37"/>
-      <c r="M51" s="37"/>
+      <c r="J51" s="35"/>
+      <c r="K51" s="35"/>
+      <c r="L51" s="35"/>
+      <c r="M51" s="35"/>
       <c r="N51" s="8" t="s">
         <v>325</v>
       </c>
@@ -4769,15 +4784,15 @@
       <c r="H56" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="I56" s="36" t="s">
+      <c r="I56" s="37" t="s">
         <v>314</v>
       </c>
-      <c r="J56" s="37"/>
-      <c r="K56" s="37"/>
-      <c r="L56" s="37"/>
-      <c r="M56" s="37"/>
-      <c r="N56" s="37"/>
-      <c r="O56" s="38"/>
+      <c r="J56" s="35"/>
+      <c r="K56" s="35"/>
+      <c r="L56" s="35"/>
+      <c r="M56" s="35"/>
+      <c r="N56" s="35"/>
+      <c r="O56" s="36"/>
       <c r="P56" s="7">
         <v>4</v>
       </c>
@@ -5053,14 +5068,14 @@
       <c r="H63" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="I63" s="36" t="s">
+      <c r="I63" s="37" t="s">
         <v>314</v>
       </c>
-      <c r="J63" s="37"/>
-      <c r="K63" s="37"/>
-      <c r="L63" s="37"/>
-      <c r="M63" s="37"/>
-      <c r="N63" s="37"/>
+      <c r="J63" s="35"/>
+      <c r="K63" s="35"/>
+      <c r="L63" s="35"/>
+      <c r="M63" s="35"/>
+      <c r="N63" s="35"/>
       <c r="O63" s="9" t="s">
         <v>383</v>
       </c>
@@ -5161,15 +5176,15 @@
       <c r="H65" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="I65" s="36" t="s">
+      <c r="I65" s="37" t="s">
         <v>314</v>
       </c>
-      <c r="J65" s="37"/>
-      <c r="K65" s="37"/>
-      <c r="L65" s="37"/>
-      <c r="M65" s="37"/>
-      <c r="N65" s="37"/>
-      <c r="O65" s="38"/>
+      <c r="J65" s="35"/>
+      <c r="K65" s="35"/>
+      <c r="L65" s="35"/>
+      <c r="M65" s="35"/>
+      <c r="N65" s="35"/>
+      <c r="O65" s="36"/>
       <c r="P65" s="7">
         <v>4</v>
       </c>
@@ -5561,12 +5576,12 @@
       <c r="J74" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="K74" s="40" t="s">
+      <c r="K74" s="32" t="s">
         <v>314</v>
       </c>
-      <c r="L74" s="40"/>
-      <c r="M74" s="40"/>
-      <c r="N74" s="40"/>
+      <c r="L74" s="32"/>
+      <c r="M74" s="32"/>
+      <c r="N74" s="32"/>
       <c r="O74" s="9" t="s">
         <v>430</v>
       </c>
@@ -5739,35 +5754,69 @@
       <c r="O77" s="9" t="s">
         <v>443</v>
       </c>
-      <c r="P77" s="7"/>
-      <c r="Q77" s="8"/>
-      <c r="R77" s="8"/>
-      <c r="S77" s="9"/>
-    </row>
-    <row r="78" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P77" s="7">
+        <v>2</v>
+      </c>
+      <c r="Q77" s="8">
+        <v>2</v>
+      </c>
+      <c r="R77" s="8">
+        <v>2</v>
+      </c>
+      <c r="S77" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:19" ht="160" x14ac:dyDescent="0.25">
       <c r="A78" s="16">
         <v>39.090000000000003</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C78" s="13"/>
+      <c r="C78" s="13" t="s">
+        <v>448</v>
+      </c>
       <c r="D78" s="7"/>
       <c r="E78" s="7"/>
-      <c r="F78" s="15"/>
-      <c r="G78" s="8"/>
-      <c r="H78" s="9"/>
-      <c r="I78" s="7"/>
-      <c r="J78" s="8"/>
+      <c r="F78" s="15">
+        <v>45901</v>
+      </c>
+      <c r="G78" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="H78" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="I78" s="7" t="s">
+        <v>449</v>
+      </c>
+      <c r="J78" s="8" t="s">
+        <v>450</v>
+      </c>
       <c r="K78" s="8"/>
-      <c r="L78" s="8"/>
-      <c r="M78" s="8"/>
+      <c r="L78" s="8" t="s">
+        <v>451</v>
+      </c>
+      <c r="M78" s="8" t="s">
+        <v>119</v>
+      </c>
       <c r="N78" s="8"/>
-      <c r="O78" s="9"/>
-      <c r="P78" s="7"/>
-      <c r="Q78" s="8"/>
-      <c r="R78" s="8"/>
-      <c r="S78" s="9"/>
+      <c r="O78" s="9" t="s">
+        <v>452</v>
+      </c>
+      <c r="P78" s="7">
+        <v>3</v>
+      </c>
+      <c r="Q78" s="8">
+        <v>4</v>
+      </c>
+      <c r="R78" s="8">
+        <v>3</v>
+      </c>
+      <c r="S78" s="9">
+        <v>4</v>
+      </c>
     </row>
     <row r="79" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="16">
@@ -6611,6 +6660,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="I2:O2"/>
+    <mergeCell ref="P32:S33"/>
+    <mergeCell ref="I56:O56"/>
+    <mergeCell ref="I51:M51"/>
+    <mergeCell ref="I48:M48"/>
+    <mergeCell ref="I49:M49"/>
+    <mergeCell ref="P2:S2"/>
     <mergeCell ref="K74:N74"/>
     <mergeCell ref="C32:C33"/>
     <mergeCell ref="F32:F33"/>
@@ -6619,14 +6676,6 @@
     <mergeCell ref="I32:O33"/>
     <mergeCell ref="I65:O65"/>
     <mergeCell ref="I63:N63"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="I2:O2"/>
-    <mergeCell ref="P32:S33"/>
-    <mergeCell ref="I56:O56"/>
-    <mergeCell ref="I51:M51"/>
-    <mergeCell ref="I48:M48"/>
-    <mergeCell ref="I49:M49"/>
-    <mergeCell ref="P2:S2"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
1 DP problem + 2 practice sets
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bharat/bctci/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C6C1483-04D6-6B48-B3EC-C4775023EEB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAFEFBC2-35A8-7841-B664-93DDC8D0DBB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{233FF15D-0BCB-6B46-B450-599851EED7C1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{233FF15D-0BCB-6B46-B450-599851EED7C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="470">
   <si>
     <t>Sets &amp; Maps</t>
   </si>
@@ -1432,6 +1432,24 @@
   </si>
   <si>
     <t>Counting instances of a value in a nested row</t>
+  </si>
+  <si>
+    <t>Got close in my analysis, but eventually did not recognise that the starting condition, and choices were threefold rather than twofold</t>
+  </si>
+  <si>
+    <t>6th Sep</t>
+  </si>
+  <si>
+    <t>Seemed to fit the subproblem pattern</t>
+  </si>
+  <si>
+    <t>Good intro</t>
+  </si>
+  <si>
+    <t>I needed to become familiar with the pattern for the general formula for recurrence</t>
+  </si>
+  <si>
+    <t>Recurrence formula</t>
   </si>
 </sst>
 </file>
@@ -1747,24 +1765,6 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1777,8 +1777,26 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2116,9 +2134,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4095FB6B-33CD-C94D-A3B2-EAADF58B3AE5}">
   <dimension ref="A1:S120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T80" sqref="T80"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R83" sqref="R83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2207,26 +2225,26 @@
       </c>
       <c r="D2" s="26"/>
       <c r="E2" s="26"/>
-      <c r="F2" s="38" t="s">
+      <c r="F2" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="G2" s="39"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="41" t="s">
+      <c r="G2" s="33"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="40"/>
-      <c r="P2" s="41" t="s">
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="Q2" s="39"/>
-      <c r="R2" s="39"/>
-      <c r="S2" s="42"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="39"/>
     </row>
     <row r="3" spans="1:19" s="8" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14">
@@ -3619,35 +3637,35 @@
       <c r="B32" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="33" t="s">
+      <c r="C32" s="41" t="s">
         <v>251</v>
       </c>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
-      <c r="F32" s="34">
+      <c r="F32" s="42">
         <v>45871</v>
       </c>
-      <c r="G32" s="35" t="s">
+      <c r="G32" s="37" t="s">
         <v>252</v>
       </c>
-      <c r="H32" s="36" t="s">
+      <c r="H32" s="38" t="s">
         <v>252</v>
       </c>
-      <c r="I32" s="37" t="s">
+      <c r="I32" s="36" t="s">
         <v>253</v>
       </c>
-      <c r="J32" s="35"/>
-      <c r="K32" s="35"/>
-      <c r="L32" s="35"/>
-      <c r="M32" s="35"/>
-      <c r="N32" s="35"/>
-      <c r="O32" s="36"/>
-      <c r="P32" s="37">
+      <c r="J32" s="37"/>
+      <c r="K32" s="37"/>
+      <c r="L32" s="37"/>
+      <c r="M32" s="37"/>
+      <c r="N32" s="37"/>
+      <c r="O32" s="38"/>
+      <c r="P32" s="36">
         <v>2</v>
       </c>
-      <c r="Q32" s="35"/>
-      <c r="R32" s="35"/>
-      <c r="S32" s="36"/>
+      <c r="Q32" s="37"/>
+      <c r="R32" s="37"/>
+      <c r="S32" s="38"/>
     </row>
     <row r="33" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="17">
@@ -3656,23 +3674,23 @@
       <c r="B33" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="33"/>
+      <c r="C33" s="41"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
-      <c r="F33" s="34"/>
-      <c r="G33" s="35"/>
-      <c r="H33" s="36"/>
-      <c r="I33" s="37"/>
-      <c r="J33" s="35"/>
-      <c r="K33" s="35"/>
-      <c r="L33" s="35"/>
-      <c r="M33" s="35"/>
-      <c r="N33" s="35"/>
-      <c r="O33" s="36"/>
-      <c r="P33" s="37"/>
-      <c r="Q33" s="35"/>
-      <c r="R33" s="35"/>
-      <c r="S33" s="36"/>
+      <c r="F33" s="42"/>
+      <c r="G33" s="37"/>
+      <c r="H33" s="38"/>
+      <c r="I33" s="36"/>
+      <c r="J33" s="37"/>
+      <c r="K33" s="37"/>
+      <c r="L33" s="37"/>
+      <c r="M33" s="37"/>
+      <c r="N33" s="37"/>
+      <c r="O33" s="38"/>
+      <c r="P33" s="36"/>
+      <c r="Q33" s="37"/>
+      <c r="R33" s="37"/>
+      <c r="S33" s="38"/>
     </row>
     <row r="34" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="16">
@@ -4369,13 +4387,13 @@
       <c r="H48" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="I48" s="37" t="s">
+      <c r="I48" s="36" t="s">
         <v>314</v>
       </c>
-      <c r="J48" s="35"/>
-      <c r="K48" s="35"/>
-      <c r="L48" s="35"/>
-      <c r="M48" s="35"/>
+      <c r="J48" s="37"/>
+      <c r="K48" s="37"/>
+      <c r="L48" s="37"/>
+      <c r="M48" s="37"/>
       <c r="N48" s="8" t="s">
         <v>317</v>
       </c>
@@ -4420,13 +4438,13 @@
       <c r="H49" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="I49" s="37" t="s">
+      <c r="I49" s="36" t="s">
         <v>314</v>
       </c>
-      <c r="J49" s="35"/>
-      <c r="K49" s="35"/>
-      <c r="L49" s="35"/>
-      <c r="M49" s="35"/>
+      <c r="J49" s="37"/>
+      <c r="K49" s="37"/>
+      <c r="L49" s="37"/>
+      <c r="M49" s="37"/>
       <c r="N49" s="8" t="s">
         <v>317</v>
       </c>
@@ -4530,13 +4548,13 @@
       <c r="H51" s="9" t="s">
         <v>247</v>
       </c>
-      <c r="I51" s="37" t="s">
+      <c r="I51" s="36" t="s">
         <v>314</v>
       </c>
-      <c r="J51" s="35"/>
-      <c r="K51" s="35"/>
-      <c r="L51" s="35"/>
-      <c r="M51" s="35"/>
+      <c r="J51" s="37"/>
+      <c r="K51" s="37"/>
+      <c r="L51" s="37"/>
+      <c r="M51" s="37"/>
       <c r="N51" s="8" t="s">
         <v>325</v>
       </c>
@@ -4817,15 +4835,15 @@
       <c r="H56" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="I56" s="37" t="s">
+      <c r="I56" s="36" t="s">
         <v>314</v>
       </c>
-      <c r="J56" s="35"/>
-      <c r="K56" s="35"/>
-      <c r="L56" s="35"/>
-      <c r="M56" s="35"/>
-      <c r="N56" s="35"/>
-      <c r="O56" s="36"/>
+      <c r="J56" s="37"/>
+      <c r="K56" s="37"/>
+      <c r="L56" s="37"/>
+      <c r="M56" s="37"/>
+      <c r="N56" s="37"/>
+      <c r="O56" s="38"/>
       <c r="P56" s="7">
         <v>4</v>
       </c>
@@ -5101,14 +5119,14 @@
       <c r="H63" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="I63" s="37" t="s">
+      <c r="I63" s="36" t="s">
         <v>314</v>
       </c>
-      <c r="J63" s="35"/>
-      <c r="K63" s="35"/>
-      <c r="L63" s="35"/>
-      <c r="M63" s="35"/>
-      <c r="N63" s="35"/>
+      <c r="J63" s="37"/>
+      <c r="K63" s="37"/>
+      <c r="L63" s="37"/>
+      <c r="M63" s="37"/>
+      <c r="N63" s="37"/>
       <c r="O63" s="9" t="s">
         <v>383</v>
       </c>
@@ -5209,15 +5227,15 @@
       <c r="H65" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="I65" s="37" t="s">
+      <c r="I65" s="36" t="s">
         <v>314</v>
       </c>
-      <c r="J65" s="35"/>
-      <c r="K65" s="35"/>
-      <c r="L65" s="35"/>
-      <c r="M65" s="35"/>
-      <c r="N65" s="35"/>
-      <c r="O65" s="36"/>
+      <c r="J65" s="37"/>
+      <c r="K65" s="37"/>
+      <c r="L65" s="37"/>
+      <c r="M65" s="37"/>
+      <c r="N65" s="37"/>
+      <c r="O65" s="38"/>
       <c r="P65" s="7">
         <v>4</v>
       </c>
@@ -5609,12 +5627,12 @@
       <c r="J74" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="K74" s="32" t="s">
+      <c r="K74" s="40" t="s">
         <v>314</v>
       </c>
-      <c r="L74" s="32"/>
-      <c r="M74" s="32"/>
-      <c r="N74" s="32"/>
+      <c r="L74" s="40"/>
+      <c r="M74" s="40"/>
+      <c r="N74" s="40"/>
       <c r="O74" s="9" t="s">
         <v>430</v>
       </c>
@@ -5996,30 +6014,60 @@
       <c r="R82" s="8"/>
       <c r="S82" s="9"/>
     </row>
-    <row r="83" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:19" ht="80" x14ac:dyDescent="0.25">
       <c r="A83" s="16">
         <v>40.01</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>385</v>
       </c>
-      <c r="C83" s="13"/>
+      <c r="C83" s="13" t="s">
+        <v>464</v>
+      </c>
       <c r="D83" s="7"/>
       <c r="E83" s="7"/>
-      <c r="F83" s="15"/>
-      <c r="G83" s="8"/>
-      <c r="H83" s="9"/>
-      <c r="I83" s="7"/>
-      <c r="J83" s="8"/>
-      <c r="K83" s="8"/>
-      <c r="L83" s="8"/>
-      <c r="M83" s="8"/>
-      <c r="N83" s="8"/>
-      <c r="O83" s="9"/>
-      <c r="P83" s="7"/>
-      <c r="Q83" s="8"/>
-      <c r="R83" s="8"/>
-      <c r="S83" s="9"/>
+      <c r="F83" s="15" t="s">
+        <v>465</v>
+      </c>
+      <c r="G83" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="H83" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="I83" s="7" t="s">
+        <v>468</v>
+      </c>
+      <c r="J83" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="K83" s="8" t="s">
+        <v>466</v>
+      </c>
+      <c r="L83" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="M83" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="N83" s="8" t="s">
+        <v>467</v>
+      </c>
+      <c r="O83" s="9" t="s">
+        <v>469</v>
+      </c>
+      <c r="P83" s="7">
+        <v>2</v>
+      </c>
+      <c r="Q83" s="8">
+        <v>2</v>
+      </c>
+      <c r="R83" s="8">
+        <v>2</v>
+      </c>
+      <c r="S83" s="9">
+        <v>2</v>
+      </c>
     </row>
     <row r="84" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="16">
@@ -6747,6 +6795,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="K74:N74"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="H32:H33"/>
+    <mergeCell ref="I32:O33"/>
+    <mergeCell ref="I65:O65"/>
+    <mergeCell ref="I63:N63"/>
     <mergeCell ref="F2:H2"/>
     <mergeCell ref="I2:O2"/>
     <mergeCell ref="P32:S33"/>
@@ -6755,14 +6811,6 @@
     <mergeCell ref="I48:M48"/>
     <mergeCell ref="I49:M49"/>
     <mergeCell ref="P2:S2"/>
-    <mergeCell ref="K74:N74"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="H32:H33"/>
-    <mergeCell ref="I32:O33"/>
-    <mergeCell ref="I65:O65"/>
-    <mergeCell ref="I63:N63"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Wrapping up dynamic programming problem set
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bharat/bctci/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A3AE842-6F6C-F04E-A995-124360E3EBC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E63707-BDD3-404E-B891-D159B40FEFC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{233FF15D-0BCB-6B46-B450-599851EED7C1}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="494">
   <si>
     <t>Sets &amp; Maps</t>
   </si>
@@ -1468,6 +1468,60 @@
   </si>
   <si>
     <t>(calc) + 1 as second parameter of range, making it explicit that the plus is due to syntax</t>
+  </si>
+  <si>
+    <t>I got it to work, following a similar pattern as minivan problems. However, my solution was not as elegant as the reference solution</t>
+  </si>
+  <si>
+    <t>Managed to approach the non-skipping of elements well. However, did not find the elegant, this or next one approach</t>
+  </si>
+  <si>
+    <t>That this could have subproblems. I think I could have thought of a backtracking approach for this one as well. The constraints indicated otherwise though.</t>
+  </si>
+  <si>
+    <t>No, all good here.</t>
+  </si>
+  <si>
+    <t>No, just more practice</t>
+  </si>
+  <si>
+    <t>All elements with 1 as value are lead to invalid path. For places where element is 0, go l, r, diag and check base case</t>
+  </si>
+  <si>
+    <t>Recognised that a subproblem recurs and can be cached</t>
+  </si>
+  <si>
+    <t>Cleanliness of recurrence formula</t>
+  </si>
+  <si>
+    <t>Nailed it!</t>
+  </si>
+  <si>
+    <t>Solved it, almost optimally. Recognised that there were ten options, and I could cache a few subroblems</t>
+  </si>
+  <si>
+    <t>Recognised the choices in the recurrence, and memoized correctly</t>
+  </si>
+  <si>
+    <t>Chose a complexer recurrence relation than I could have.</t>
+  </si>
+  <si>
+    <t>Got it pretty quickly</t>
+  </si>
+  <si>
+    <t>Got my recurrence formula wrong: subproblem of counting from 1 upwards, as opposed to counting towards 1, and at 1 base case is 0</t>
+  </si>
+  <si>
+    <t>Did not have a good approach for building min pairwise, important when there are optional cases</t>
+  </si>
+  <si>
+    <t>I think I made a mistake with my recurrence formula: did not consider how it is addressing the subproblem, or the general case</t>
+  </si>
+  <si>
+    <t>Maybe it was a matter of exposure to the pattern, wasn't sure how to build min</t>
+  </si>
+  <si>
+    <t>Review this exercise for the pattern</t>
   </si>
 </sst>
 </file>
@@ -2152,9 +2206,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4095FB6B-33CD-C94D-A3B2-EAADF58B3AE5}">
   <dimension ref="A1:S120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S84" sqref="S84"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A88" sqref="A88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6140,105 +6194,225 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:19" ht="140" x14ac:dyDescent="0.25">
       <c r="A85" s="16">
         <v>40.03</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>387</v>
       </c>
-      <c r="C85" s="13"/>
+      <c r="C85" s="13" t="s">
+        <v>476</v>
+      </c>
       <c r="D85" s="7"/>
       <c r="E85" s="7"/>
-      <c r="F85" s="15"/>
-      <c r="G85" s="8"/>
-      <c r="H85" s="9"/>
-      <c r="I85" s="7"/>
-      <c r="J85" s="8"/>
-      <c r="K85" s="8"/>
-      <c r="L85" s="8"/>
-      <c r="M85" s="8"/>
-      <c r="N85" s="8"/>
-      <c r="O85" s="9"/>
-      <c r="P85" s="7"/>
-      <c r="Q85" s="8"/>
-      <c r="R85" s="8"/>
-      <c r="S85" s="9"/>
-    </row>
-    <row r="86" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F85" s="15">
+        <v>45917</v>
+      </c>
+      <c r="G85" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="H85" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="I85" s="7" t="s">
+        <v>477</v>
+      </c>
+      <c r="J85" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="K85" s="8" t="s">
+        <v>478</v>
+      </c>
+      <c r="L85" s="8" t="s">
+        <v>479</v>
+      </c>
+      <c r="M85" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="N85" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="O85" s="9" t="s">
+        <v>480</v>
+      </c>
+      <c r="P85" s="7">
+        <v>3</v>
+      </c>
+      <c r="Q85" s="8">
+        <v>3</v>
+      </c>
+      <c r="R85" s="8">
+        <v>3</v>
+      </c>
+      <c r="S85" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:19" ht="80" x14ac:dyDescent="0.25">
       <c r="A86" s="16">
         <v>40.04</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>388</v>
       </c>
-      <c r="C86" s="13"/>
+      <c r="C86" s="13" t="s">
+        <v>481</v>
+      </c>
       <c r="D86" s="7"/>
       <c r="E86" s="7"/>
-      <c r="F86" s="15"/>
-      <c r="G86" s="8"/>
-      <c r="H86" s="9"/>
-      <c r="I86" s="7"/>
-      <c r="J86" s="8"/>
-      <c r="K86" s="8"/>
-      <c r="L86" s="8"/>
-      <c r="M86" s="8"/>
-      <c r="N86" s="8"/>
-      <c r="O86" s="9"/>
-      <c r="P86" s="7"/>
-      <c r="Q86" s="8"/>
-      <c r="R86" s="8"/>
-      <c r="S86" s="9"/>
-    </row>
-    <row r="87" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F86" s="15">
+        <v>45917</v>
+      </c>
+      <c r="G86" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="H86" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="I86" s="7" t="s">
+        <v>482</v>
+      </c>
+      <c r="J86" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="K86" s="8" t="s">
+        <v>331</v>
+      </c>
+      <c r="L86" s="8" t="s">
+        <v>483</v>
+      </c>
+      <c r="M86" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="N86" s="8" t="s">
+        <v>484</v>
+      </c>
+      <c r="O86" s="9" t="s">
+        <v>480</v>
+      </c>
+      <c r="P86" s="7">
+        <v>4</v>
+      </c>
+      <c r="Q86" s="8">
+        <v>4</v>
+      </c>
+      <c r="R86" s="8">
+        <v>4</v>
+      </c>
+      <c r="S86" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:19" ht="80" x14ac:dyDescent="0.25">
       <c r="A87" s="16">
         <v>40.049999999999997</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>389</v>
       </c>
-      <c r="C87" s="13"/>
+      <c r="C87" s="13" t="s">
+        <v>485</v>
+      </c>
       <c r="D87" s="7"/>
       <c r="E87" s="7"/>
-      <c r="F87" s="15"/>
-      <c r="G87" s="8"/>
-      <c r="H87" s="9"/>
-      <c r="I87" s="7"/>
-      <c r="J87" s="8"/>
-      <c r="K87" s="8"/>
-      <c r="L87" s="8"/>
-      <c r="M87" s="8"/>
-      <c r="N87" s="8"/>
-      <c r="O87" s="9"/>
-      <c r="P87" s="7"/>
-      <c r="Q87" s="8"/>
-      <c r="R87" s="8"/>
-      <c r="S87" s="9"/>
-    </row>
-    <row r="88" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F87" s="15">
+        <v>45917</v>
+      </c>
+      <c r="G87" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="H87" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="I87" s="7" t="s">
+        <v>486</v>
+      </c>
+      <c r="J87" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="K87" s="8" t="s">
+        <v>487</v>
+      </c>
+      <c r="L87" s="8" t="s">
+        <v>483</v>
+      </c>
+      <c r="M87" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="N87" s="8" t="s">
+        <v>488</v>
+      </c>
+      <c r="O87" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="P87" s="7">
+        <v>3</v>
+      </c>
+      <c r="Q87" s="8">
+        <v>3</v>
+      </c>
+      <c r="R87" s="8">
+        <v>3</v>
+      </c>
+      <c r="S87" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:19" ht="100" x14ac:dyDescent="0.25">
       <c r="A88" s="16">
         <v>40.06</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>390</v>
       </c>
-      <c r="C88" s="13"/>
+      <c r="C88" s="13" t="s">
+        <v>489</v>
+      </c>
       <c r="D88" s="7"/>
       <c r="E88" s="7"/>
-      <c r="F88" s="15"/>
-      <c r="G88" s="8"/>
-      <c r="H88" s="9"/>
-      <c r="I88" s="7"/>
-      <c r="J88" s="8"/>
-      <c r="K88" s="8"/>
-      <c r="L88" s="8"/>
-      <c r="M88" s="8"/>
-      <c r="N88" s="8"/>
-      <c r="O88" s="9"/>
-      <c r="P88" s="7"/>
-      <c r="Q88" s="8"/>
-      <c r="R88" s="8"/>
-      <c r="S88" s="9"/>
+      <c r="F88" s="15">
+        <v>45917</v>
+      </c>
+      <c r="G88" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="H88" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="I88" s="7" t="s">
+        <v>490</v>
+      </c>
+      <c r="J88" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="K88" s="8" t="s">
+        <v>491</v>
+      </c>
+      <c r="L88" s="8" t="s">
+        <v>492</v>
+      </c>
+      <c r="M88" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="N88" s="8" t="s">
+        <v>493</v>
+      </c>
+      <c r="O88" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="P88" s="7">
+        <v>2</v>
+      </c>
+      <c r="Q88" s="8">
+        <v>2</v>
+      </c>
+      <c r="R88" s="8">
+        <v>2</v>
+      </c>
+      <c r="S88" s="9">
+        <v>2</v>
+      </c>
     </row>
     <row r="89" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="16">

</xml_diff>

<commit_message>
Wrapping up Dynamic Programming
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bharat/bctci/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E63707-BDD3-404E-B891-D159B40FEFC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D6DB1E1-1123-F64C-9CA8-9DCC4F225DF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{233FF15D-0BCB-6B46-B450-599851EED7C1}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="498">
   <si>
     <t>Sets &amp; Maps</t>
   </si>
@@ -1522,6 +1522,18 @@
   </si>
   <si>
     <t>Review this exercise for the pattern</t>
+  </si>
+  <si>
+    <t>Didn't get to the solution by myself, but has some similar patterns to the DP recurrence formula. Used return value for computation, ie on the way up</t>
+  </si>
+  <si>
+    <t>Good pattern to know. Keep in mind what you're doing in the general case</t>
+  </si>
+  <si>
+    <t>Got pretty close with this one. However, couldn't figure out how to handle general case. Solution reconstruction approach is also new, should try this more often.</t>
+  </si>
+  <si>
+    <t>Good pattern to know. Keep in mind what you're doing in the general case. Esp important to practice reconstruction after recurrence implementation</t>
   </si>
 </sst>
 </file>
@@ -1752,7 +1764,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1837,24 +1849,6 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1867,8 +1861,29 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2207,8 +2222,8 @@
   <dimension ref="A1:S120"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A88" sqref="A88"/>
+      <pane ySplit="1" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A95" sqref="A95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2297,26 +2312,26 @@
       </c>
       <c r="D2" s="26"/>
       <c r="E2" s="26"/>
-      <c r="F2" s="38" t="s">
+      <c r="F2" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="G2" s="39"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="41" t="s">
+      <c r="G2" s="33"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="40"/>
-      <c r="P2" s="41" t="s">
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="Q2" s="39"/>
-      <c r="R2" s="39"/>
-      <c r="S2" s="42"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="39"/>
     </row>
     <row r="3" spans="1:19" s="8" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14">
@@ -3709,35 +3724,35 @@
       <c r="B32" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="33" t="s">
+      <c r="C32" s="41" t="s">
         <v>251</v>
       </c>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
-      <c r="F32" s="34">
+      <c r="F32" s="42">
         <v>45871</v>
       </c>
-      <c r="G32" s="35" t="s">
+      <c r="G32" s="37" t="s">
         <v>252</v>
       </c>
-      <c r="H32" s="36" t="s">
+      <c r="H32" s="38" t="s">
         <v>252</v>
       </c>
-      <c r="I32" s="37" t="s">
+      <c r="I32" s="36" t="s">
         <v>253</v>
       </c>
-      <c r="J32" s="35"/>
-      <c r="K32" s="35"/>
-      <c r="L32" s="35"/>
-      <c r="M32" s="35"/>
-      <c r="N32" s="35"/>
-      <c r="O32" s="36"/>
-      <c r="P32" s="37">
+      <c r="J32" s="37"/>
+      <c r="K32" s="37"/>
+      <c r="L32" s="37"/>
+      <c r="M32" s="37"/>
+      <c r="N32" s="37"/>
+      <c r="O32" s="38"/>
+      <c r="P32" s="36">
         <v>2</v>
       </c>
-      <c r="Q32" s="35"/>
-      <c r="R32" s="35"/>
-      <c r="S32" s="36"/>
+      <c r="Q32" s="37"/>
+      <c r="R32" s="37"/>
+      <c r="S32" s="38"/>
     </row>
     <row r="33" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="17">
@@ -3746,23 +3761,23 @@
       <c r="B33" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="33"/>
+      <c r="C33" s="41"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
-      <c r="F33" s="34"/>
-      <c r="G33" s="35"/>
-      <c r="H33" s="36"/>
-      <c r="I33" s="37"/>
-      <c r="J33" s="35"/>
-      <c r="K33" s="35"/>
-      <c r="L33" s="35"/>
-      <c r="M33" s="35"/>
-      <c r="N33" s="35"/>
-      <c r="O33" s="36"/>
-      <c r="P33" s="37"/>
-      <c r="Q33" s="35"/>
-      <c r="R33" s="35"/>
-      <c r="S33" s="36"/>
+      <c r="F33" s="42"/>
+      <c r="G33" s="37"/>
+      <c r="H33" s="38"/>
+      <c r="I33" s="36"/>
+      <c r="J33" s="37"/>
+      <c r="K33" s="37"/>
+      <c r="L33" s="37"/>
+      <c r="M33" s="37"/>
+      <c r="N33" s="37"/>
+      <c r="O33" s="38"/>
+      <c r="P33" s="36"/>
+      <c r="Q33" s="37"/>
+      <c r="R33" s="37"/>
+      <c r="S33" s="38"/>
     </row>
     <row r="34" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="16">
@@ -4459,13 +4474,13 @@
       <c r="H48" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="I48" s="37" t="s">
+      <c r="I48" s="36" t="s">
         <v>314</v>
       </c>
-      <c r="J48" s="35"/>
-      <c r="K48" s="35"/>
-      <c r="L48" s="35"/>
-      <c r="M48" s="35"/>
+      <c r="J48" s="37"/>
+      <c r="K48" s="37"/>
+      <c r="L48" s="37"/>
+      <c r="M48" s="37"/>
       <c r="N48" s="8" t="s">
         <v>317</v>
       </c>
@@ -4510,13 +4525,13 @@
       <c r="H49" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="I49" s="37" t="s">
+      <c r="I49" s="36" t="s">
         <v>314</v>
       </c>
-      <c r="J49" s="35"/>
-      <c r="K49" s="35"/>
-      <c r="L49" s="35"/>
-      <c r="M49" s="35"/>
+      <c r="J49" s="37"/>
+      <c r="K49" s="37"/>
+      <c r="L49" s="37"/>
+      <c r="M49" s="37"/>
       <c r="N49" s="8" t="s">
         <v>317</v>
       </c>
@@ -4620,13 +4635,13 @@
       <c r="H51" s="9" t="s">
         <v>247</v>
       </c>
-      <c r="I51" s="37" t="s">
+      <c r="I51" s="36" t="s">
         <v>314</v>
       </c>
-      <c r="J51" s="35"/>
-      <c r="K51" s="35"/>
-      <c r="L51" s="35"/>
-      <c r="M51" s="35"/>
+      <c r="J51" s="37"/>
+      <c r="K51" s="37"/>
+      <c r="L51" s="37"/>
+      <c r="M51" s="37"/>
       <c r="N51" s="8" t="s">
         <v>325</v>
       </c>
@@ -4907,15 +4922,15 @@
       <c r="H56" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="I56" s="37" t="s">
+      <c r="I56" s="36" t="s">
         <v>314</v>
       </c>
-      <c r="J56" s="35"/>
-      <c r="K56" s="35"/>
-      <c r="L56" s="35"/>
-      <c r="M56" s="35"/>
-      <c r="N56" s="35"/>
-      <c r="O56" s="36"/>
+      <c r="J56" s="37"/>
+      <c r="K56" s="37"/>
+      <c r="L56" s="37"/>
+      <c r="M56" s="37"/>
+      <c r="N56" s="37"/>
+      <c r="O56" s="38"/>
       <c r="P56" s="7">
         <v>4</v>
       </c>
@@ -5191,14 +5206,14 @@
       <c r="H63" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="I63" s="37" t="s">
+      <c r="I63" s="36" t="s">
         <v>314</v>
       </c>
-      <c r="J63" s="35"/>
-      <c r="K63" s="35"/>
-      <c r="L63" s="35"/>
-      <c r="M63" s="35"/>
-      <c r="N63" s="35"/>
+      <c r="J63" s="37"/>
+      <c r="K63" s="37"/>
+      <c r="L63" s="37"/>
+      <c r="M63" s="37"/>
+      <c r="N63" s="37"/>
       <c r="O63" s="9" t="s">
         <v>383</v>
       </c>
@@ -5299,15 +5314,15 @@
       <c r="H65" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="I65" s="37" t="s">
+      <c r="I65" s="36" t="s">
         <v>314</v>
       </c>
-      <c r="J65" s="35"/>
-      <c r="K65" s="35"/>
-      <c r="L65" s="35"/>
-      <c r="M65" s="35"/>
-      <c r="N65" s="35"/>
-      <c r="O65" s="36"/>
+      <c r="J65" s="37"/>
+      <c r="K65" s="37"/>
+      <c r="L65" s="37"/>
+      <c r="M65" s="37"/>
+      <c r="N65" s="37"/>
+      <c r="O65" s="38"/>
       <c r="P65" s="7">
         <v>4</v>
       </c>
@@ -5699,12 +5714,12 @@
       <c r="J74" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="K74" s="32" t="s">
+      <c r="K74" s="40" t="s">
         <v>314</v>
       </c>
-      <c r="L74" s="32"/>
-      <c r="M74" s="32"/>
-      <c r="N74" s="32"/>
+      <c r="L74" s="40"/>
+      <c r="M74" s="40"/>
+      <c r="N74" s="40"/>
       <c r="O74" s="9" t="s">
         <v>430</v>
       </c>
@@ -6414,55 +6429,91 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:19" ht="100" x14ac:dyDescent="0.25">
       <c r="A89" s="16">
         <v>40.07</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="C89" s="13"/>
+      <c r="C89" s="13" t="s">
+        <v>494</v>
+      </c>
       <c r="D89" s="7"/>
       <c r="E89" s="7"/>
-      <c r="F89" s="15"/>
-      <c r="G89" s="8"/>
-      <c r="H89" s="9"/>
-      <c r="I89" s="7"/>
-      <c r="J89" s="8"/>
-      <c r="K89" s="8"/>
-      <c r="L89" s="8"/>
-      <c r="M89" s="8"/>
-      <c r="N89" s="8"/>
-      <c r="O89" s="9"/>
-      <c r="P89" s="7"/>
-      <c r="Q89" s="8"/>
-      <c r="R89" s="8"/>
-      <c r="S89" s="9"/>
-    </row>
-    <row r="90" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F89" s="15">
+        <v>45918</v>
+      </c>
+      <c r="G89" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="H89" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="I89" s="36" t="s">
+        <v>495</v>
+      </c>
+      <c r="J89" s="43"/>
+      <c r="K89" s="43"/>
+      <c r="L89" s="43"/>
+      <c r="M89" s="43"/>
+      <c r="N89" s="43"/>
+      <c r="O89" s="38"/>
+      <c r="P89" s="7">
+        <v>2</v>
+      </c>
+      <c r="Q89" s="8">
+        <v>2</v>
+      </c>
+      <c r="R89" s="8">
+        <v>2</v>
+      </c>
+      <c r="S89" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:19" ht="100" x14ac:dyDescent="0.25">
       <c r="A90" s="16">
         <v>40.08</v>
       </c>
       <c r="B90" s="3" t="s">
         <v>392</v>
       </c>
-      <c r="C90" s="13"/>
+      <c r="C90" s="13" t="s">
+        <v>496</v>
+      </c>
       <c r="D90" s="7"/>
       <c r="E90" s="7"/>
-      <c r="F90" s="15"/>
-      <c r="G90" s="8"/>
-      <c r="H90" s="9"/>
-      <c r="I90" s="7"/>
-      <c r="J90" s="8"/>
-      <c r="K90" s="8"/>
-      <c r="L90" s="8"/>
-      <c r="M90" s="8"/>
-      <c r="N90" s="8"/>
-      <c r="O90" s="9"/>
-      <c r="P90" s="7"/>
-      <c r="Q90" s="8"/>
-      <c r="R90" s="8"/>
-      <c r="S90" s="9"/>
+      <c r="F90" s="15">
+        <v>45918</v>
+      </c>
+      <c r="G90" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="H90" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="I90" s="36" t="s">
+        <v>497</v>
+      </c>
+      <c r="J90" s="43"/>
+      <c r="K90" s="43"/>
+      <c r="L90" s="43"/>
+      <c r="M90" s="43"/>
+      <c r="N90" s="43"/>
+      <c r="O90" s="38"/>
+      <c r="P90" s="7">
+        <v>2</v>
+      </c>
+      <c r="Q90" s="8">
+        <v>3</v>
+      </c>
+      <c r="R90" s="8">
+        <v>3</v>
+      </c>
+      <c r="S90" s="9">
+        <v>2</v>
+      </c>
     </row>
     <row r="91" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C91" s="13"/>
@@ -7014,7 +7065,17 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="18">
+    <mergeCell ref="I89:O89"/>
+    <mergeCell ref="I90:O90"/>
+    <mergeCell ref="K74:N74"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="H32:H33"/>
+    <mergeCell ref="I32:O33"/>
+    <mergeCell ref="I65:O65"/>
+    <mergeCell ref="I63:N63"/>
     <mergeCell ref="F2:H2"/>
     <mergeCell ref="I2:O2"/>
     <mergeCell ref="P32:S33"/>
@@ -7023,14 +7084,6 @@
     <mergeCell ref="I48:M48"/>
     <mergeCell ref="I49:M49"/>
     <mergeCell ref="P2:S2"/>
-    <mergeCell ref="K74:N74"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="H32:H33"/>
-    <mergeCell ref="I32:O33"/>
-    <mergeCell ref="I65:O65"/>
-    <mergeCell ref="I63:N63"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Wrapping up problem notes for Greedy Algorithm problems
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bharat/bctci/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A47C19D-056C-0842-B2EE-C3AF22360C09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC4737EB-7A67-7145-BD46-3886BCD4AE7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{233FF15D-0BCB-6B46-B450-599851EED7C1}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="530">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="538">
   <si>
     <t>Sets &amp; Maps</t>
   </si>
@@ -1629,6 +1629,30 @@
   </si>
   <si>
     <t>math.dist() for points between distances</t>
+  </si>
+  <si>
+    <t>Go this right from the get go, analysing that I only needed to sort, and take the first two available for each tripet</t>
+  </si>
+  <si>
+    <t>Honestly. The biggest trigger was that the problem is in this chapter</t>
+  </si>
+  <si>
+    <t>That sorting was required, and that the triplets would start from least values</t>
+  </si>
+  <si>
+    <t>Happy to do this one well</t>
+  </si>
+  <si>
+    <t>iter format for parallel but different array iteration</t>
+  </si>
+  <si>
+    <t>My instict was that you sort meetings, and find the ones that are not overlapping. However, my answers are not passing the test case</t>
+  </si>
+  <si>
+    <t>I have an incomplete understanding, and need to revisit this problem later</t>
+  </si>
+  <si>
+    <t>Instinct was to follow a similar pattern to the time traveler problem. However, my answers are not passing the test case</t>
   </si>
 </sst>
 </file>
@@ -1638,7 +1662,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1686,6 +1710,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1815,7 +1845,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1879,6 +1909,24 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1891,25 +1939,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2248,9 +2284,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4095FB6B-33CD-C94D-A3B2-EAADF58B3AE5}">
   <dimension ref="A1:S159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U96" sqref="U96"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A98" sqref="A98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2339,26 +2375,26 @@
       </c>
       <c r="D2" s="18"/>
       <c r="E2" s="18"/>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="G2" s="24"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="26" t="s">
+      <c r="G2" s="30"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="25"/>
-      <c r="P2" s="26" t="s">
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="24"/>
-      <c r="S2" s="30"/>
+      <c r="Q2" s="30"/>
+      <c r="R2" s="30"/>
+      <c r="S2" s="33"/>
     </row>
     <row r="3" spans="1:19" s="5" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10">
@@ -3751,35 +3787,35 @@
       <c r="B32" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="32" t="s">
+      <c r="C32" s="27" t="s">
         <v>250</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
-      <c r="F32" s="33">
+      <c r="F32" s="28">
         <v>45871</v>
       </c>
-      <c r="G32" s="28" t="s">
+      <c r="G32" s="24" t="s">
         <v>251</v>
       </c>
-      <c r="H32" s="29" t="s">
+      <c r="H32" s="25" t="s">
         <v>251</v>
       </c>
-      <c r="I32" s="27" t="s">
+      <c r="I32" s="23" t="s">
         <v>252</v>
       </c>
-      <c r="J32" s="28"/>
-      <c r="K32" s="28"/>
-      <c r="L32" s="28"/>
-      <c r="M32" s="28"/>
-      <c r="N32" s="28"/>
-      <c r="O32" s="29"/>
-      <c r="P32" s="27">
+      <c r="J32" s="24"/>
+      <c r="K32" s="24"/>
+      <c r="L32" s="24"/>
+      <c r="M32" s="24"/>
+      <c r="N32" s="24"/>
+      <c r="O32" s="25"/>
+      <c r="P32" s="23">
         <v>2</v>
       </c>
-      <c r="Q32" s="28"/>
-      <c r="R32" s="28"/>
-      <c r="S32" s="29"/>
+      <c r="Q32" s="24"/>
+      <c r="R32" s="24"/>
+      <c r="S32" s="25"/>
     </row>
     <row r="33" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13">
@@ -3788,23 +3824,23 @@
       <c r="B33" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="32"/>
+      <c r="C33" s="27"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
-      <c r="F33" s="33"/>
-      <c r="G33" s="28"/>
-      <c r="H33" s="29"/>
-      <c r="I33" s="27"/>
-      <c r="J33" s="28"/>
-      <c r="K33" s="28"/>
-      <c r="L33" s="28"/>
-      <c r="M33" s="28"/>
-      <c r="N33" s="28"/>
-      <c r="O33" s="29"/>
-      <c r="P33" s="27"/>
-      <c r="Q33" s="28"/>
-      <c r="R33" s="28"/>
-      <c r="S33" s="29"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="24"/>
+      <c r="H33" s="25"/>
+      <c r="I33" s="23"/>
+      <c r="J33" s="24"/>
+      <c r="K33" s="24"/>
+      <c r="L33" s="24"/>
+      <c r="M33" s="24"/>
+      <c r="N33" s="24"/>
+      <c r="O33" s="25"/>
+      <c r="P33" s="23"/>
+      <c r="Q33" s="24"/>
+      <c r="R33" s="24"/>
+      <c r="S33" s="25"/>
     </row>
     <row r="34" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
@@ -4501,13 +4537,13 @@
       <c r="H48" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="I48" s="27" t="s">
+      <c r="I48" s="23" t="s">
         <v>313</v>
       </c>
-      <c r="J48" s="28"/>
-      <c r="K48" s="28"/>
-      <c r="L48" s="28"/>
-      <c r="M48" s="28"/>
+      <c r="J48" s="24"/>
+      <c r="K48" s="24"/>
+      <c r="L48" s="24"/>
+      <c r="M48" s="24"/>
       <c r="N48" s="5" t="s">
         <v>316</v>
       </c>
@@ -4552,13 +4588,13 @@
       <c r="H49" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="I49" s="27" t="s">
+      <c r="I49" s="23" t="s">
         <v>313</v>
       </c>
-      <c r="J49" s="28"/>
-      <c r="K49" s="28"/>
-      <c r="L49" s="28"/>
-      <c r="M49" s="28"/>
+      <c r="J49" s="24"/>
+      <c r="K49" s="24"/>
+      <c r="L49" s="24"/>
+      <c r="M49" s="24"/>
       <c r="N49" s="5" t="s">
         <v>316</v>
       </c>
@@ -4662,13 +4698,13 @@
       <c r="H51" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="I51" s="27" t="s">
+      <c r="I51" s="23" t="s">
         <v>313</v>
       </c>
-      <c r="J51" s="28"/>
-      <c r="K51" s="28"/>
-      <c r="L51" s="28"/>
-      <c r="M51" s="28"/>
+      <c r="J51" s="24"/>
+      <c r="K51" s="24"/>
+      <c r="L51" s="24"/>
+      <c r="M51" s="24"/>
       <c r="N51" s="5" t="s">
         <v>324</v>
       </c>
@@ -4949,15 +4985,15 @@
       <c r="H56" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="I56" s="27" t="s">
+      <c r="I56" s="23" t="s">
         <v>313</v>
       </c>
-      <c r="J56" s="28"/>
-      <c r="K56" s="28"/>
-      <c r="L56" s="28"/>
-      <c r="M56" s="28"/>
-      <c r="N56" s="28"/>
-      <c r="O56" s="29"/>
+      <c r="J56" s="24"/>
+      <c r="K56" s="24"/>
+      <c r="L56" s="24"/>
+      <c r="M56" s="24"/>
+      <c r="N56" s="24"/>
+      <c r="O56" s="25"/>
       <c r="P56" s="4">
         <v>4</v>
       </c>
@@ -5233,14 +5269,14 @@
       <c r="H63" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="I63" s="27" t="s">
+      <c r="I63" s="23" t="s">
         <v>313</v>
       </c>
-      <c r="J63" s="28"/>
-      <c r="K63" s="28"/>
-      <c r="L63" s="28"/>
-      <c r="M63" s="28"/>
-      <c r="N63" s="28"/>
+      <c r="J63" s="24"/>
+      <c r="K63" s="24"/>
+      <c r="L63" s="24"/>
+      <c r="M63" s="24"/>
+      <c r="N63" s="24"/>
       <c r="O63" s="6" t="s">
         <v>382</v>
       </c>
@@ -5341,15 +5377,15 @@
       <c r="H65" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="I65" s="27" t="s">
+      <c r="I65" s="23" t="s">
         <v>313</v>
       </c>
-      <c r="J65" s="28"/>
-      <c r="K65" s="28"/>
-      <c r="L65" s="28"/>
-      <c r="M65" s="28"/>
-      <c r="N65" s="28"/>
-      <c r="O65" s="29"/>
+      <c r="J65" s="24"/>
+      <c r="K65" s="24"/>
+      <c r="L65" s="24"/>
+      <c r="M65" s="24"/>
+      <c r="N65" s="24"/>
+      <c r="O65" s="25"/>
       <c r="P65" s="4">
         <v>4</v>
       </c>
@@ -5741,12 +5777,12 @@
       <c r="J74" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="K74" s="31" t="s">
+      <c r="K74" s="26" t="s">
         <v>313</v>
       </c>
-      <c r="L74" s="31"/>
-      <c r="M74" s="31"/>
-      <c r="N74" s="31"/>
+      <c r="L74" s="26"/>
+      <c r="M74" s="26"/>
+      <c r="N74" s="26"/>
       <c r="O74" s="6" t="s">
         <v>429</v>
       </c>
@@ -6477,15 +6513,15 @@
       <c r="H89" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="I89" s="27" t="s">
+      <c r="I89" s="23" t="s">
         <v>494</v>
       </c>
-      <c r="J89" s="28"/>
-      <c r="K89" s="28"/>
-      <c r="L89" s="28"/>
-      <c r="M89" s="28"/>
-      <c r="N89" s="28"/>
-      <c r="O89" s="29"/>
+      <c r="J89" s="24"/>
+      <c r="K89" s="24"/>
+      <c r="L89" s="24"/>
+      <c r="M89" s="24"/>
+      <c r="N89" s="24"/>
+      <c r="O89" s="25"/>
       <c r="P89" s="4">
         <v>2</v>
       </c>
@@ -6520,15 +6556,15 @@
       <c r="H90" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="I90" s="27" t="s">
+      <c r="I90" s="23" t="s">
         <v>496</v>
       </c>
-      <c r="J90" s="28"/>
-      <c r="K90" s="28"/>
-      <c r="L90" s="28"/>
-      <c r="M90" s="28"/>
-      <c r="N90" s="28"/>
-      <c r="O90" s="29"/>
+      <c r="J90" s="24"/>
+      <c r="K90" s="24"/>
+      <c r="L90" s="24"/>
+      <c r="M90" s="24"/>
+      <c r="N90" s="24"/>
+      <c r="O90" s="25"/>
       <c r="P90" s="4">
         <v>2</v>
       </c>
@@ -6607,7 +6643,7 @@
       <c r="A94" s="12">
         <v>41.01</v>
       </c>
-      <c r="B94" s="3" t="s">
+      <c r="B94" s="34" t="s">
         <v>69</v>
       </c>
       <c r="C94" s="9" t="s">
@@ -6725,9 +6761,15 @@
       </c>
       <c r="D96" s="4"/>
       <c r="E96" s="4"/>
-      <c r="F96" s="11"/>
-      <c r="G96" s="5"/>
-      <c r="H96" s="6"/>
+      <c r="F96" s="11">
+        <v>45919</v>
+      </c>
+      <c r="G96" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="H96" s="6" t="s">
+        <v>112</v>
+      </c>
       <c r="I96" s="4" t="s">
         <v>526</v>
       </c>
@@ -6762,79 +6804,146 @@
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:19" ht="80" x14ac:dyDescent="0.25">
       <c r="A97" s="12">
         <v>41.04</v>
       </c>
       <c r="B97" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C97" s="9"/>
+      <c r="C97" s="9" t="s">
+        <v>530</v>
+      </c>
       <c r="D97" s="4"/>
       <c r="E97" s="4"/>
-      <c r="F97" s="11"/>
-      <c r="G97" s="5"/>
-      <c r="H97" s="6"/>
-      <c r="J97" s="5"/>
-      <c r="K97" s="5"/>
-      <c r="L97" s="5"/>
-      <c r="M97" s="5"/>
-      <c r="N97" s="5"/>
-      <c r="O97" s="6"/>
-      <c r="P97" s="4"/>
-      <c r="Q97" s="5"/>
-      <c r="R97" s="5"/>
-      <c r="S97" s="6"/>
-    </row>
-    <row r="98" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F97" s="11">
+        <v>45919</v>
+      </c>
+      <c r="G97" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="H97" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="I97" s="4" t="s">
+        <v>531</v>
+      </c>
+      <c r="J97" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="K97" s="5" t="s">
+        <v>532</v>
+      </c>
+      <c r="L97" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="M97" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="N97" s="5" t="s">
+        <v>533</v>
+      </c>
+      <c r="O97" s="6" t="s">
+        <v>534</v>
+      </c>
+      <c r="P97" s="4">
+        <v>4</v>
+      </c>
+      <c r="Q97" s="5">
+        <v>4</v>
+      </c>
+      <c r="R97" s="5">
+        <v>4</v>
+      </c>
+      <c r="S97" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="98" spans="1:19" ht="100" x14ac:dyDescent="0.25">
       <c r="A98" s="12">
         <v>41.05</v>
       </c>
-      <c r="B98" s="3" t="s">
+      <c r="B98" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="C98" s="9"/>
+      <c r="C98" s="9" t="s">
+        <v>535</v>
+      </c>
       <c r="D98" s="4"/>
       <c r="E98" s="4"/>
-      <c r="F98" s="11"/>
-      <c r="G98" s="5"/>
-      <c r="H98" s="6"/>
-      <c r="I98" s="4"/>
-      <c r="J98" s="5"/>
-      <c r="K98" s="5"/>
-      <c r="L98" s="5"/>
-      <c r="M98" s="5"/>
-      <c r="N98" s="5"/>
-      <c r="O98" s="6"/>
-      <c r="P98" s="4"/>
-      <c r="Q98" s="5"/>
-      <c r="R98" s="5"/>
-      <c r="S98" s="6"/>
-    </row>
-    <row r="99" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F98" s="11">
+        <v>45919</v>
+      </c>
+      <c r="G98" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="H98" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="I98" s="23" t="s">
+        <v>536</v>
+      </c>
+      <c r="J98" s="35"/>
+      <c r="K98" s="35"/>
+      <c r="L98" s="35"/>
+      <c r="M98" s="35"/>
+      <c r="N98" s="35"/>
+      <c r="O98" s="25"/>
+      <c r="P98" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q98" s="5">
+        <v>2</v>
+      </c>
+      <c r="R98" s="5">
+        <v>1</v>
+      </c>
+      <c r="S98" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:19" ht="80" x14ac:dyDescent="0.25">
       <c r="A99" s="12">
         <v>41.06</v>
       </c>
-      <c r="B99" s="3" t="s">
+      <c r="B99" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="C99" s="9"/>
+      <c r="C99" s="9" t="s">
+        <v>537</v>
+      </c>
       <c r="D99" s="4"/>
       <c r="E99" s="4"/>
-      <c r="F99" s="11"/>
-      <c r="G99" s="5"/>
-      <c r="H99" s="6"/>
-      <c r="I99" s="4"/>
-      <c r="J99" s="5"/>
-      <c r="K99" s="5"/>
-      <c r="L99" s="5"/>
-      <c r="M99" s="5"/>
-      <c r="N99" s="5"/>
-      <c r="O99" s="6"/>
-      <c r="P99" s="4"/>
-      <c r="Q99" s="5"/>
-      <c r="R99" s="5"/>
-      <c r="S99" s="6"/>
+      <c r="F99" s="11">
+        <v>45919</v>
+      </c>
+      <c r="G99" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="H99" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="I99" s="23" t="s">
+        <v>536</v>
+      </c>
+      <c r="J99" s="35"/>
+      <c r="K99" s="35"/>
+      <c r="L99" s="35"/>
+      <c r="M99" s="35"/>
+      <c r="N99" s="35"/>
+      <c r="O99" s="25"/>
+      <c r="P99" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q99" s="5">
+        <v>2</v>
+      </c>
+      <c r="R99" s="5">
+        <v>1</v>
+      </c>
+      <c r="S99" s="6">
+        <v>2</v>
+      </c>
     </row>
     <row r="100" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C100" s="9"/>
@@ -8184,7 +8293,17 @@
       <c r="S159" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="20">
+    <mergeCell ref="I98:O98"/>
+    <mergeCell ref="I99:O99"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="I2:O2"/>
+    <mergeCell ref="P32:S33"/>
+    <mergeCell ref="I56:O56"/>
+    <mergeCell ref="I51:M51"/>
+    <mergeCell ref="I48:M48"/>
+    <mergeCell ref="I49:M49"/>
+    <mergeCell ref="P2:S2"/>
     <mergeCell ref="I89:O89"/>
     <mergeCell ref="I90:O90"/>
     <mergeCell ref="K74:N74"/>
@@ -8195,14 +8314,6 @@
     <mergeCell ref="I32:O33"/>
     <mergeCell ref="I65:O65"/>
     <mergeCell ref="I63:N63"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="I2:O2"/>
-    <mergeCell ref="P32:S33"/>
-    <mergeCell ref="I56:O56"/>
-    <mergeCell ref="I51:M51"/>
-    <mergeCell ref="I48:M48"/>
-    <mergeCell ref="I49:M49"/>
-    <mergeCell ref="P2:S2"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>